<commit_message>
updated excel, left over code files from previous commit
</commit_message>
<xml_diff>
--- a/res-econ_RA_data.xlsx
+++ b/res-econ_RA_data.xlsx
@@ -362,7 +362,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F210"/>
+  <dimension ref="A1:G210"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -410,6 +410,11 @@
           <t>Zillow URLs</t>
         </is>
       </c>
+      <c r="G1" s="0" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/renter-hub/clickRedirect?alias=4nfwvwe0ye6y&amp;r=trulia&amp;mobileFriendly=true</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="6" t="inlineStr">
@@ -431,6 +436,11 @@
           <t>2,346</t>
         </is>
       </c>
+      <c r="G2" s="0" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/6-Standish-Cir-Andover-MA-01810/56034004_zpid/</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="6" t="inlineStr">
@@ -452,6 +462,11 @@
           <t>719</t>
         </is>
       </c>
+      <c r="G3" s="0" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/150-Traincroft-NW-Medford-MA-02155/56277119_zpid/</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="6" t="inlineStr">
@@ -473,6 +488,11 @@
           <t>1,015</t>
         </is>
       </c>
+      <c r="G4" s="0" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/24-Dean-Rd-Wayland-MA-01778/57127108_zpid/</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="6" t="inlineStr">
@@ -494,6 +514,11 @@
           <t>1,754</t>
         </is>
       </c>
+      <c r="G5" s="0" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/173-Bay-Rd-Harwich-MA-02645/186993999_zpid/</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="6" t="inlineStr">
@@ -515,6 +540,11 @@
           <t>1,289</t>
         </is>
       </c>
+      <c r="G6" s="0" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/1-Ladyslipper-Ln-Hadley-MA-01035/57015531_zpid/</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="6" t="inlineStr">
@@ -536,6 +566,11 @@
           <t>1,627</t>
         </is>
       </c>
+      <c r="G7" s="0" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/170-Kilkore-Dr-Hyannis-MA-02601/55846500_zpid/</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="6" t="inlineStr">
@@ -557,6 +592,11 @@
           <t>380</t>
         </is>
       </c>
+      <c r="G8" s="0" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/39-Stevens-St-Stoneham-MA-02180/56336960_zpid/</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="6" t="inlineStr">
@@ -578,6 +618,11 @@
           <t>1,310</t>
         </is>
       </c>
+      <c r="G9" s="0" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/17-Milbery-Ln-Pembroke-MA-02359/57536844_zpid/</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="6" t="inlineStr">
@@ -599,6 +644,11 @@
           <t>1,141</t>
         </is>
       </c>
+      <c r="G10" s="0" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/12-Harris-Ln-Harvard-MA-01451/173940900_zpid/</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="6" t="inlineStr">
@@ -620,6 +670,11 @@
           <t>909</t>
         </is>
       </c>
+      <c r="G11" s="0" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/21-White-Oaks-Rd-Williamstown-MA-01267/56819688_zpid/</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="6" t="inlineStr">
@@ -641,6 +696,11 @@
           <t>2,325</t>
         </is>
       </c>
+      <c r="G12" s="0" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/12-Overlook-Dr-East-Longmeadow-MA-01028/56171419_zpid/</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="6" t="inlineStr">
@@ -667,6 +727,11 @@
           <t>https://www.zillow.com/homedetails/58-Linda-Ave-Framingham-MA-01701/165985595_zpid/</t>
         </is>
       </c>
+      <c r="G13" s="0" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/58-Linda-Ave-Framingham-MA-01701/165985595_zpid/</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="6" t="inlineStr">
@@ -693,6 +758,11 @@
           <t>https://www.zillow.com/homedetails/19-Holly-Cir-Easthampton-MA-01027/57009823_zpid/</t>
         </is>
       </c>
+      <c r="G14" s="0" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/19-Holly-Cir-Easthampton-MA-01027/57009823_zpid/</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="6" t="inlineStr">
@@ -719,6 +789,11 @@
           <t>https://www.zillow.com/homedetails/31-E-Sound-Ln-Tisbury-MA-02568/56900325_zpid/</t>
         </is>
       </c>
+      <c r="G15" s="0" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/31-E-Sound-Ln-Tisbury-MA-02568/56900325_zpid/</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="6" t="inlineStr">
@@ -745,6 +820,11 @@
           <t>https://www.zillow.com/homedetails/156-Standish-Rd-Needham-MA-02492/57478769_zpid/</t>
         </is>
       </c>
+      <c r="G16" s="0" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/156-Standish-Rd-Needham-MA-02492/57478769_zpid/</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="6" t="inlineStr">
@@ -771,6 +851,11 @@
           <t>https://www.zillow.com/homedetails/18-Bartkus-Farm-Concord-MA-01742/166021417_zpid/</t>
         </is>
       </c>
+      <c r="G17" s="0" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/18-Bartkus-Farm-Concord-MA-01742/306465917_zpid/</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="6" t="inlineStr">
@@ -797,6 +882,11 @@
           <t>https://www.zillow.com/homedetails/17-Mello-St-East-Falmouth-MA-02536/55885097_zpid/</t>
         </is>
       </c>
+      <c r="G18" s="0" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/17-Mello-St-East-Falmouth-MA-02536/55885097_zpid/</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="6" t="inlineStr">
@@ -823,6 +913,11 @@
           <t>https://www.zillow.com/homedetails/198-W-River-St-Upton-MA-01568/173952657_zpid/</t>
         </is>
       </c>
+      <c r="G19" s="0" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/198-W-River-St-Upton-MA-01568/173952657_zpid/</t>
+        </is>
+      </c>
     </row>
     <row r="20" ht="15.75" customHeight="1" s="7">
       <c r="A20" s="6" t="inlineStr">
@@ -849,6 +944,11 @@
           <t>https://www.zillow.com/homedetails/298-Heaths-Bridge-Rd-Concord-MA-01742/166021031_zpid/</t>
         </is>
       </c>
+      <c r="G20" s="0" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/298-Heaths-Bridge-Rd-Concord-MA-01742/166021031_zpid/</t>
+        </is>
+      </c>
     </row>
     <row r="21" ht="15.75" customHeight="1" s="7">
       <c r="A21" s="6" t="inlineStr">
@@ -875,6 +975,11 @@
           <t>https://www.zillow.com/homedetails/66-Milk-St-Nantucket-MA-02554/56544257_zpid/</t>
         </is>
       </c>
+      <c r="G21" s="0" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/66-Milk-St-Nantucket-MA-02554/56544257_zpid/</t>
+        </is>
+      </c>
     </row>
     <row r="22" ht="15.75" customHeight="1" s="7">
       <c r="A22" s="6" t="inlineStr">
@@ -901,6 +1006,11 @@
           <t>https://www.zillow.com/homedetails/116-Charlton-St-Oxford-MA-01540/60027614_zpid/</t>
         </is>
       </c>
+      <c r="G22" s="0" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/116-Charlton-St-Oxford-MA-01540/60027614_zpid/</t>
+        </is>
+      </c>
     </row>
     <row r="23" ht="15.75" customHeight="1" s="7">
       <c r="A23" s="6" t="inlineStr">
@@ -927,6 +1037,11 @@
           <t>https://www.zillow.com/homedetails/262-Sheep-Pond-Dr-Brewster-MA-02631/56767509_zpid/</t>
         </is>
       </c>
+      <c r="G23" s="0" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/262-Sheep-Pond-Dr-Brewster-MA-02631/56767509_zpid/</t>
+        </is>
+      </c>
     </row>
     <row r="24" ht="15.75" customHeight="1" s="7">
       <c r="A24" s="6" t="inlineStr">
@@ -953,6 +1068,11 @@
           <t>https://www.zillow.com/homedetails/67-Gorwin-Dr-Hanson-MA-02341/184281722_zpid/</t>
         </is>
       </c>
+      <c r="G24" s="0" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/67-Gorwin-Dr-Hanson-MA-02341/184281722_zpid/</t>
+        </is>
+      </c>
     </row>
     <row r="25" ht="15.75" customHeight="1" s="7">
       <c r="A25" s="6" t="inlineStr">
@@ -979,6 +1099,11 @@
           <t>https://www.zillow.com/homedetails/9-Samuel-Parlin-Dr-Acton-MA-01720/57031578_zpid/</t>
         </is>
       </c>
+      <c r="G25" s="0" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/9-Samuel-Parlin-Dr-Acton-MA-01720/57031578_zpid/</t>
+        </is>
+      </c>
     </row>
     <row r="26" ht="15.75" customHeight="1" s="7">
       <c r="A26" s="6" t="inlineStr">
@@ -1005,6 +1130,11 @@
           <t>https://www.zillow.com/homedetails/34-Hoover-Ave-Brockton-MA-02301/57161799_zpid/</t>
         </is>
       </c>
+      <c r="G26" s="0" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/34-Hoover-Ave-Brockton-MA-02301/57161799_zpid/</t>
+        </is>
+      </c>
     </row>
     <row r="27" ht="15.75" customHeight="1" s="7">
       <c r="A27" s="6" t="inlineStr">
@@ -1031,6 +1161,11 @@
           <t>https://www.zillow.com/homedetails/1-Oakwood-Rd-Acton-MA-01720/57035146_zpid/</t>
         </is>
       </c>
+      <c r="G27" s="0" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/1-Oakwood-Rd-Acton-MA-01720/57035146_zpid/</t>
+        </is>
+      </c>
     </row>
     <row r="28" ht="15.75" customHeight="1" s="7">
       <c r="A28" s="6" t="inlineStr">
@@ -1057,6 +1192,11 @@
           <t>https://www.zillow.com/homedetails/15-Foxglove-Ln-Amherst-MA-01002/56258397_zpid/</t>
         </is>
       </c>
+      <c r="G28" s="0" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/15-Foxglove-Ln-Amherst-MA-01002/56258397_zpid/</t>
+        </is>
+      </c>
     </row>
     <row r="29" ht="15.75" customHeight="1" s="7">
       <c r="A29" s="6" t="inlineStr">
@@ -1083,6 +1223,11 @@
           <t>https://www.zillow.com/homedetails/98-Heywood-Rd-Ashby-MA-01431/71129594_zpid/</t>
         </is>
       </c>
+      <c r="G29" s="0" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/98-Heywood-Rd-Ashby-MA-01431/71129594_zpid/</t>
+        </is>
+      </c>
     </row>
     <row r="30" ht="15.75" customHeight="1" s="7">
       <c r="A30" s="6" t="inlineStr">
@@ -1107,6 +1252,11 @@
           <t>None</t>
         </is>
       </c>
+      <c r="G30" s="0" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/camp-danbee-peru-ma/houses/</t>
+        </is>
+      </c>
     </row>
     <row r="31" ht="15.75" customHeight="1" s="7">
       <c r="A31" s="6" t="inlineStr">
@@ -1133,6 +1283,11 @@
           <t>https://www.zillow.com/homedetails/154-Oakham-Rd-North-Brookfield-MA-01535/57620961_zpid/</t>
         </is>
       </c>
+      <c r="G31" s="0" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/154-Oakham-Rd-North-Brookfield-MA-01535/57620961_zpid/</t>
+        </is>
+      </c>
     </row>
     <row r="32" ht="15.75" customHeight="1" s="7">
       <c r="A32" s="6" t="inlineStr">
@@ -1159,6 +1314,11 @@
           <t>https://www.zillow.com/homedetails/58-River-Rd-Gill-MA-01354/56980125_zpid/</t>
         </is>
       </c>
+      <c r="G32" s="0" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/58-River-Rd-Gill-MA-01354/56980125_zpid/</t>
+        </is>
+      </c>
     </row>
     <row r="33" ht="15.75" customHeight="1" s="7">
       <c r="A33" s="6" t="inlineStr">
@@ -1185,6 +1345,11 @@
           <t>https://www.zillow.com/homedetails/40-Glenmore-Ln-Bridgewater-MA-02324/57153009_zpid/</t>
         </is>
       </c>
+      <c r="G33" s="0" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/40-Glenmore-Ln-Bridgewater-MA-02324/57153009_zpid/</t>
+        </is>
+      </c>
     </row>
     <row r="34" ht="15.75" customHeight="1" s="7">
       <c r="A34" s="6" t="inlineStr">
@@ -1211,6 +1376,11 @@
           <t>https://www.zillow.com/homedetails/36-Green-Acres-Dr-Whitman-MA-02382/59192163_zpid/</t>
         </is>
       </c>
+      <c r="G34" s="0" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/36-Green-Acres-Dr-Whitman-MA-02382/59192163_zpid/</t>
+        </is>
+      </c>
     </row>
     <row r="35" ht="15.75" customHeight="1" s="7">
       <c r="A35" s="6" t="inlineStr">
@@ -1237,6 +1407,11 @@
           <t>https://www.zillow.com/homedetails/83-Oxford-Rd-Westwood-MA-02090/57516186_zpid/</t>
         </is>
       </c>
+      <c r="G35" s="0" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/83-Oxford-Rd-Westwood-MA-02090/57516186_zpid/</t>
+        </is>
+      </c>
     </row>
     <row r="36" ht="15.75" customHeight="1" s="7">
       <c r="A36" s="6" t="inlineStr">
@@ -1263,6 +1438,11 @@
           <t>https://www.zillow.com/homedetails/18-Proctor-Rd-Chelmsford-MA-01824/56451870_zpid/</t>
         </is>
       </c>
+      <c r="G36" s="0" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/18-Proctor-Rd-Chelmsford-MA-01824/56451870_zpid/</t>
+        </is>
+      </c>
     </row>
     <row r="37" ht="15.75" customHeight="1" s="7">
       <c r="A37" s="6" t="inlineStr">
@@ -1284,6 +1464,11 @@
           <t>3,001</t>
         </is>
       </c>
+      <c r="G37" s="0" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/409-Still-River-Rd-Bolton-MA-01740/57568730_zpid/</t>
+        </is>
+      </c>
     </row>
     <row r="38" ht="15.75" customHeight="1" s="7">
       <c r="A38" s="6" t="inlineStr">
@@ -1305,6 +1490,11 @@
           <t>1,332</t>
         </is>
       </c>
+      <c r="G38" s="0" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/4-Nicholson-Hill-Rd-Southwick-MA-01077/56996681_zpid/</t>
+        </is>
+      </c>
     </row>
     <row r="39" ht="15.75" customHeight="1" s="7">
       <c r="A39" s="6" t="inlineStr">
@@ -1326,6 +1516,11 @@
           <t>1,057</t>
         </is>
       </c>
+      <c r="G39" s="0" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/29-Harris-St-Amherst-MA-01002/56254557_zpid/</t>
+        </is>
+      </c>
     </row>
     <row r="40" ht="15.75" customHeight="1" s="7">
       <c r="A40" s="6" t="inlineStr">
@@ -1347,6 +1542,11 @@
           <t>1,120</t>
         </is>
       </c>
+      <c r="G40" s="0" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/17-Tricia-Rd-North-Falmouth-MA-02556/55881948_zpid/</t>
+        </is>
+      </c>
     </row>
     <row r="41" ht="15.75" customHeight="1" s="7">
       <c r="A41" s="6" t="inlineStr">
@@ -1368,6 +1568,11 @@
           <t>550</t>
         </is>
       </c>
+      <c r="G41" s="0" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/42-Ames-St-Medford-MA-02155/56273410_zpid/</t>
+        </is>
+      </c>
     </row>
     <row r="42" ht="15.75" customHeight="1" s="7">
       <c r="A42" s="6" t="inlineStr">
@@ -1389,6 +1594,11 @@
           <t>1,987</t>
         </is>
       </c>
+      <c r="G42" s="0" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/152-Chipman-Rd-Chester-MA-01011/80383079_zpid/</t>
+        </is>
+      </c>
     </row>
     <row r="43" ht="15.75" customHeight="1" s="7">
       <c r="A43" s="6" t="inlineStr">
@@ -1410,6 +1620,11 @@
           <t>550</t>
         </is>
       </c>
+      <c r="G43" s="0" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/18-Perkins-St-Arlington-MA-02476/56403369_zpid/</t>
+        </is>
+      </c>
     </row>
     <row r="44" ht="15.75" customHeight="1" s="7">
       <c r="A44" s="6" t="inlineStr">
@@ -1431,6 +1646,11 @@
           <t>1,754</t>
         </is>
       </c>
+      <c r="G44" s="0" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/196-South-St-Berlin-MA-01503/57564080_zpid/</t>
+        </is>
+      </c>
     </row>
     <row r="45" ht="15.75" customHeight="1" s="7">
       <c r="A45" s="6" t="inlineStr">
@@ -1452,6 +1672,11 @@
           <t>909</t>
         </is>
       </c>
+      <c r="G45" s="0" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/46-Park-Ave-Natick-MA-01760/56296372_zpid/</t>
+        </is>
+      </c>
     </row>
     <row r="46" ht="15.75" customHeight="1" s="7">
       <c r="A46" s="6" t="inlineStr">
@@ -1473,6 +1698,11 @@
           <t>1,141</t>
         </is>
       </c>
+      <c r="G46" s="0" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/19-Susan-Dr-Dudley-MA-01571/61320453_zpid/</t>
+        </is>
+      </c>
     </row>
     <row r="47" ht="15.75" customHeight="1" s="7">
       <c r="A47" s="6" t="inlineStr">
@@ -1494,6 +1724,11 @@
           <t>2,029</t>
         </is>
       </c>
+      <c r="G47" s="0" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/4-Fort-Avenue-Ter-1-Roxbury-MA-02119/2075895402_zpid/</t>
+        </is>
+      </c>
     </row>
     <row r="48" ht="15.75" customHeight="1" s="7">
       <c r="A48" s="6" t="inlineStr">
@@ -1515,6 +1750,11 @@
           <t>1,184</t>
         </is>
       </c>
+      <c r="G48" s="0" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/9-Playstead-Ln-East-Falmouth-MA-02536/55891667_zpid/</t>
+        </is>
+      </c>
     </row>
     <row r="49" ht="15.75" customHeight="1" s="7">
       <c r="A49" s="6" t="inlineStr">
@@ -1536,6 +1776,11 @@
           <t>1,162</t>
         </is>
       </c>
+      <c r="G49" s="0" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/34-Stedman-St-Chelmsford-MA-01824/56446774_zpid/</t>
+        </is>
+      </c>
     </row>
     <row r="50" ht="15.75" customHeight="1" s="7">
       <c r="A50" s="6" t="inlineStr">
@@ -1557,6 +1802,11 @@
           <t>3,424</t>
         </is>
       </c>
+      <c r="G50" s="0" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/63-Minuteman-Dr-Concord-MA-01742/166022267_zpid/</t>
+        </is>
+      </c>
     </row>
     <row r="51" ht="15.75" customHeight="1" s="7">
       <c r="A51" s="6" t="inlineStr">
@@ -1578,6 +1828,11 @@
           <t>1,141</t>
         </is>
       </c>
+      <c r="G51" s="0" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/30-Wigwam-St-Wellfleet-MA-02667/56794923_zpid/</t>
+        </is>
+      </c>
     </row>
     <row r="52" ht="15.75" customHeight="1" s="7">
       <c r="A52" s="6" t="inlineStr">
@@ -1604,6 +1859,11 @@
           <t>https://www.zillow.com/homedetails/21-Tersolo-Rd-Haverhill-MA-01832/56056744_zpid/</t>
         </is>
       </c>
+      <c r="G52" s="0" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/25-Tersolo-Rd-Haverhill-MA-01832/56056743_zpid/</t>
+        </is>
+      </c>
     </row>
     <row r="53" ht="15.75" customHeight="1" s="7">
       <c r="A53" s="6" t="inlineStr">
@@ -1630,6 +1890,11 @@
           <t>https://www.zillow.com/homedetails/110-Oaklawn-Ave-Orange-MA-01364/56140342_zpid/</t>
         </is>
       </c>
+      <c r="G53" s="0" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/110-Oaklawn-Ave-Orange-MA-01364/56140342_zpid/</t>
+        </is>
+      </c>
     </row>
     <row r="54" ht="15.75" customHeight="1" s="7">
       <c r="A54" s="6" t="inlineStr">
@@ -1656,6 +1921,11 @@
           <t>https://www.zillow.com/homedetails/226-Paddocks-Path-Dennis-MA-02638/55877916_zpid/</t>
         </is>
       </c>
+      <c r="G54" s="0" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/226-Paddocks-Path-Dennis-MA-02638/55877916_zpid/</t>
+        </is>
+      </c>
     </row>
     <row r="55" ht="15.75" customHeight="1" s="7">
       <c r="A55" s="6" t="inlineStr">
@@ -1682,6 +1952,11 @@
           <t>https://www.zillow.com/homedetails/32-Woodbury-St-Beverly-MA-01915/59226114_zpid/</t>
         </is>
       </c>
+      <c r="G55" s="0" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/32-Woodbury-St-Beverly-MA-01915/59226114_zpid/</t>
+        </is>
+      </c>
     </row>
     <row r="56" ht="15.75" customHeight="1" s="7">
       <c r="A56" s="6" t="inlineStr">
@@ -1708,6 +1983,11 @@
           <t>https://www.zillow.com/homedetails/27-Windy-Hill-Dr-Plymouth-MA-02360/57545685_zpid/</t>
         </is>
       </c>
+      <c r="G56" s="0" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/23-Windy-Hill-Dr-Plymouth-MA-02360/57545686_zpid/</t>
+        </is>
+      </c>
     </row>
     <row r="57" ht="15.75" customHeight="1" s="7">
       <c r="A57" s="6" t="inlineStr">
@@ -1734,6 +2014,11 @@
           <t>https://www.zillow.com/homedetails/20-Munroe-St-Somerville-MA-02143/271378798_zpid/</t>
         </is>
       </c>
+      <c r="G57" s="0" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/20-Munroe-St-Somerville-MA-02143/271378798_zpid/</t>
+        </is>
+      </c>
     </row>
     <row r="58" ht="15.75" customHeight="1" s="7">
       <c r="A58" s="6" t="inlineStr">
@@ -1760,6 +2045,11 @@
           <t>https://www.zillow.com/homedetails/5-Carrot-Hill-Rd-Falmouth-MA-02543/55898363_zpid/</t>
         </is>
       </c>
+      <c r="G58" s="0" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/5-Carrot-Hill-Rd-Falmouth-MA-02543/55898363_zpid/</t>
+        </is>
+      </c>
     </row>
     <row r="59" ht="15.75" customHeight="1" s="7">
       <c r="A59" s="6" t="inlineStr">
@@ -1786,6 +2076,11 @@
           <t>https://www.zillow.com/homedetails/110-Lookout-Rd-Yarmouth-Port-MA-02675/55938606_zpid/</t>
         </is>
       </c>
+      <c r="G59" s="0" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/110-Lookout-Rd-Yarmouth-Port-MA-02675/55938606_zpid/</t>
+        </is>
+      </c>
     </row>
     <row r="60" ht="15.75" customHeight="1" s="7">
       <c r="A60" s="6" t="inlineStr">
@@ -1812,6 +2107,11 @@
           <t>https://www.zillow.com/homedetails/35-Sands-Rd-Eastham-MA-02642/56781235_zpid/</t>
         </is>
       </c>
+      <c r="G60" s="0" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/35-Sands-Rd-Eastham-MA-02642/56781235_zpid/</t>
+        </is>
+      </c>
     </row>
     <row r="61" ht="15.75" customHeight="1" s="7">
       <c r="A61" s="6" t="inlineStr">
@@ -1838,6 +2138,11 @@
           <t>https://www.zillow.com/homedetails/35-Harborlight-Dr-Plymouth-MA-02360/57540785_zpid/</t>
         </is>
       </c>
+      <c r="G61" s="0" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/35-Harborlight-Dr-Plymouth-MA-02360/57540785_zpid/</t>
+        </is>
+      </c>
     </row>
     <row r="62" ht="15.75" customHeight="1" s="7">
       <c r="A62" s="6" t="inlineStr">
@@ -1864,6 +2169,11 @@
           <t>https://www.zillow.com/homedetails/101-Milton-St-Northampton-MA-01062/57022922_zpid/</t>
         </is>
       </c>
+      <c r="G62" s="0" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/101-Milton-St-Northampton-MA-01062/57022922_zpid/</t>
+        </is>
+      </c>
     </row>
     <row r="63" ht="15.75" customHeight="1" s="7">
       <c r="A63" s="6" t="inlineStr">
@@ -1890,6 +2200,11 @@
           <t>https://www.zillow.com/homedetails/321-Pochassic-Rd-Westfield-MA-01085/193631018_zpid/</t>
         </is>
       </c>
+      <c r="G63" s="0" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/321-Pochassic-Rd-Westfield-MA-01085/193631018_zpid/</t>
+        </is>
+      </c>
     </row>
     <row r="64" ht="15.75" customHeight="1" s="7">
       <c r="A64" s="6" t="inlineStr">
@@ -1916,6 +2231,11 @@
           <t>https://www.zillow.com/homedetails/401-Queen-Anne-Rd-Harwich-MA-02645/186992422_zpid/</t>
         </is>
       </c>
+      <c r="G64" s="0" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/401-Queen-Anne-Rd-Harwich-MA-02645/186992422_zpid/</t>
+        </is>
+      </c>
     </row>
     <row r="65" ht="15.75" customHeight="1" s="7">
       <c r="A65" s="6" t="inlineStr">
@@ -1942,6 +2262,11 @@
           <t>https://www.zillow.com/homedetails/301-Islington-Rd-Newton-MA-02466/56309787_zpid/</t>
         </is>
       </c>
+      <c r="G65" s="0" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/301-Islington-Rd-Newton-MA-02466/56309787_zpid/</t>
+        </is>
+      </c>
     </row>
     <row r="66" ht="15.75" customHeight="1" s="7">
       <c r="A66" s="6" t="inlineStr">
@@ -1968,6 +2293,11 @@
           <t>https://www.zillow.com/homedetails/100-Jeffrey-Rd-Springfield-MA-01119/56216024_zpid/</t>
         </is>
       </c>
+      <c r="G66" s="0" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/100-Jeffrey-Rd-Springfield-MA-01119/56216024_zpid/</t>
+        </is>
+      </c>
     </row>
     <row r="67" ht="15.75" customHeight="1" s="7">
       <c r="A67" s="6" t="inlineStr">
@@ -1994,6 +2324,11 @@
           <t>https://www.zillow.com/homedetails/6-Pheasant-Ln-Topsfield-MA-01983/56969565_zpid/</t>
         </is>
       </c>
+      <c r="G67" s="0" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/6-Pheasant-Ln-Topsfield-MA-01983/56969565_zpid/</t>
+        </is>
+      </c>
     </row>
     <row r="68" ht="15.75" customHeight="1" s="7">
       <c r="A68" s="6" t="inlineStr">
@@ -2020,6 +2355,11 @@
           <t>https://www.zillow.com/homedetails/21-Crescent-Rd-Needham-MA-02494/57477934_zpid/</t>
         </is>
       </c>
+      <c r="G68" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/21-Crescent-Rd-Needham-MA-02494/57477934_zpid/</t>
+        </is>
+      </c>
     </row>
     <row r="69" ht="15.75" customHeight="1" s="7">
       <c r="A69" s="6" t="inlineStr">
@@ -2046,6 +2386,11 @@
           <t>https://www.zillow.com/homedetails/250-Summer-St-Lee-MA-01238/56804136_zpid/</t>
         </is>
       </c>
+      <c r="G69" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/250-Summer-St-Lee-MA-01238/56804136_zpid/</t>
+        </is>
+      </c>
     </row>
     <row r="70" ht="15.75" customHeight="1" s="7">
       <c r="A70" s="6" t="inlineStr">
@@ -2072,6 +2417,11 @@
           <t>https://www.zillow.com/homedetails/1-Sea-Mist-Ln-Rockport-MA-01966/56957270_zpid/</t>
         </is>
       </c>
+      <c r="G70" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/1-Sea-Mist-Ln-Rockport-MA-01966/56957270_zpid/</t>
+        </is>
+      </c>
     </row>
     <row r="71" ht="15.75" customHeight="1" s="7">
       <c r="A71" s="6" t="inlineStr">
@@ -2098,6 +2448,11 @@
           <t>https://www.zillow.com/homedetails/184-N-Leverett-Rd-Leverett-MA-01054/80863083_zpid/</t>
         </is>
       </c>
+      <c r="G71" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/184-N-Leverett-Rd-Leverett-MA-01054/80863083_zpid/</t>
+        </is>
+      </c>
     </row>
     <row r="72" ht="15.75" customHeight="1" s="7">
       <c r="A72" s="6" t="inlineStr">
@@ -2124,6 +2479,11 @@
           <t>https://www.zillow.com/homedetails/18-Knollwood-Dr-Dartmouth-MA-02747/55966575_zpid/</t>
         </is>
       </c>
+      <c r="G72" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/18-Knollwood-Dr-Dartmouth-MA-02747/55966575_zpid/</t>
+        </is>
+      </c>
     </row>
     <row r="73" ht="15.75" customHeight="1" s="7">
       <c r="A73" s="6" t="inlineStr">
@@ -2150,6 +2510,11 @@
           <t>https://www.zillow.com/homedetails/45-Greenwood-Ave-Needham-MA-02492/57475272_zpid/</t>
         </is>
       </c>
+      <c r="G73" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/45-Greenwood-Ave-Needham-MA-02492/57475272_zpid/</t>
+        </is>
+      </c>
     </row>
     <row r="74" ht="15.75" customHeight="1" s="7">
       <c r="A74" s="6" t="inlineStr">
@@ -2176,6 +2541,11 @@
           <t>https://www.zillow.com/homedetails/3-Bowers-Ave-Tyngsboro-MA-01879/57122674_zpid/</t>
         </is>
       </c>
+      <c r="G74" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/3-Bowers-Ave-Tyngsboro-MA-01879/57122674_zpid/</t>
+        </is>
+      </c>
     </row>
     <row r="75" ht="15.75" customHeight="1" s="7">
       <c r="A75" s="6" t="inlineStr">
@@ -2202,6 +2572,11 @@
           <t>https://www.zillow.com/homedetails/24-Green-Valley-Rd-Medway-MA-02053/57461159_zpid/</t>
         </is>
       </c>
+      <c r="G75" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/24-Green-Valley-Rd-Medway-MA-02053/57461159_zpid/</t>
+        </is>
+      </c>
     </row>
     <row r="76" ht="15.75" customHeight="1" s="7">
       <c r="A76" s="6" t="inlineStr">
@@ -2228,6 +2603,11 @@
           <t>https://www.zillow.com/homedetails/105-E-Gate-Rd-Brewster-MA-02631/186846759_zpid/</t>
         </is>
       </c>
+      <c r="G76" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/105-E-Gate-Rd-Brewster-MA-02631/186846759_zpid/</t>
+        </is>
+      </c>
     </row>
     <row r="77" ht="15.75" customHeight="1" s="7">
       <c r="A77" s="6" t="inlineStr">
@@ -2254,6 +2634,11 @@
           <t>https://www.zillow.com/homedetails/26-Walnut-Rd-South-Hamilton-MA-01982/56924745_zpid/</t>
         </is>
       </c>
+      <c r="G77" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/26-Walnut-Rd-South-Hamilton-MA-01982/56924745_zpid/</t>
+        </is>
+      </c>
     </row>
     <row r="78" ht="15.75" customHeight="1" s="7">
       <c r="A78" s="6" t="inlineStr">
@@ -2280,6 +2665,11 @@
           <t>https://www.zillow.com/homedetails/42-Lake-Ave-Framingham-MA-01702/165996355_zpid/</t>
         </is>
       </c>
+      <c r="G78" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/42-Lake-Ave-Framingham-MA-01702/165996355_zpid/</t>
+        </is>
+      </c>
     </row>
     <row r="79" ht="15.75" customHeight="1" s="7">
       <c r="A79" s="6" t="inlineStr">
@@ -2306,6 +2696,11 @@
           <t>https://www.zillow.com/homedetails/17-Fernwood-Dr-Hampden-MA-01036/56173594_zpid/</t>
         </is>
       </c>
+      <c r="G79" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/17-Fernwood-Dr-Hampden-MA-01036/56173594_zpid/</t>
+        </is>
+      </c>
     </row>
     <row r="80" ht="15.75" customHeight="1" s="7">
       <c r="A80" s="6" t="inlineStr">
@@ -2332,6 +2727,11 @@
           <t>https://www.zillow.com/homedetails/342-Belknap-Rd-Framingham-MA-01701/165986610_zpid/</t>
         </is>
       </c>
+      <c r="G80" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/342-Belknap-Rd-Framingham-MA-01701/165986610_zpid/</t>
+        </is>
+      </c>
     </row>
     <row r="81" ht="15.75" customHeight="1" s="7">
       <c r="A81" s="6" t="inlineStr">
@@ -2358,6 +2758,11 @@
           <t>https://www.zillow.com/homedetails/435-Martins-Pond-Rd-Groton-MA-01450/57066211_zpid/</t>
         </is>
       </c>
+      <c r="G81" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/435-Martins-Pond-Rd-Groton-MA-01450/57066211_zpid/</t>
+        </is>
+      </c>
     </row>
     <row r="82" ht="15.75" customHeight="1" s="7">
       <c r="A82" s="6" t="inlineStr">
@@ -2384,6 +2789,11 @@
           <t>https://www.zillow.com/homedetails/103-Farm-St-Bellingham-MA-02019/123883120_zpid/</t>
         </is>
       </c>
+      <c r="G82" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/103-Farm-St-Bellingham-MA-02019/123883120_zpid/</t>
+        </is>
+      </c>
     </row>
     <row r="83" ht="15.75" customHeight="1" s="7">
       <c r="A83" s="6" t="inlineStr">
@@ -2436,6 +2846,11 @@
           <t>https://www.zillow.com/homedetails/4-Vineyard-Ave-Clinton-MA-01510/57577271_zpid/</t>
         </is>
       </c>
+      <c r="G84" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/4-Vineyard-Ave-Clinton-MA-01510/57577271_zpid/</t>
+        </is>
+      </c>
     </row>
     <row r="85" ht="15.75" customHeight="1" s="7">
       <c r="A85" s="6" t="inlineStr">
@@ -2462,6 +2877,11 @@
           <t>https://www.zillow.com/homedetails/335-Grand-Ave-Falmouth-MA-02540/55896521_zpid/</t>
         </is>
       </c>
+      <c r="G85" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/335-Grand-Ave-Falmouth-MA-02540/55896521_zpid/</t>
+        </is>
+      </c>
     </row>
     <row r="86" ht="15.75" customHeight="1" s="7">
       <c r="A86" s="6" t="inlineStr">
@@ -2488,6 +2908,11 @@
           <t>https://www.zillow.com/homedetails/55-Orchard-Hill-Dr-Plymouth-MA-02360/123191116_zpid/</t>
         </is>
       </c>
+      <c r="G86" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/55-Orchard-Hill-Dr-Plymouth-MA-02360/123191116_zpid/</t>
+        </is>
+      </c>
     </row>
     <row r="87" ht="15.75" customHeight="1" s="7">
       <c r="A87" s="6" t="inlineStr">
@@ -2514,6 +2939,11 @@
           <t>https://www.zillow.com/homedetails/9-Theresa-Ave-Burlington-MA-01803/57055850_zpid/</t>
         </is>
       </c>
+      <c r="G87" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/9-Theresa-Ave-Burlington-MA-01803/57055850_zpid/</t>
+        </is>
+      </c>
     </row>
     <row r="88" ht="15.75" customHeight="1" s="7">
       <c r="A88" s="6" t="inlineStr">
@@ -2540,6 +2970,11 @@
           <t>https://www.zillow.com/homedetails/32-Pearl-Brook-Rd-Lunenburg-MA-01462/57611448_zpid/</t>
         </is>
       </c>
+      <c r="G88" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/22-Pearl-Brook-Rd-Lunenburg-MA-01462/57611447_zpid/</t>
+        </is>
+      </c>
     </row>
     <row r="89" ht="15.75" customHeight="1" s="7">
       <c r="A89" s="6" t="inlineStr">
@@ -2566,6 +3001,11 @@
           <t>https://www.zillow.com/homedetails/23-Whittemore-St-Arlington-MA-02474/56393572_zpid/</t>
         </is>
       </c>
+      <c r="G89" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/23-Whittemore-St-Arlington-MA-02474/56393572_zpid/</t>
+        </is>
+      </c>
     </row>
     <row r="90" ht="15.75" customHeight="1" s="7">
       <c r="A90" s="6" t="inlineStr">
@@ -2587,7 +3027,12 @@
           <t>2,092</t>
         </is>
       </c>
-      <c r="F90" t="inlineStr">
+      <c r="F90" s="0" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/38-Southwick-Rd-Sutton-MA-01590/57655803_zpid/</t>
+        </is>
+      </c>
+      <c r="G90" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/38-Southwick-Rd-Sutton-MA-01590/57655803_zpid/</t>
         </is>
@@ -2613,9 +3058,14 @@
           <t>1,205</t>
         </is>
       </c>
-      <c r="F91" t="inlineStr">
+      <c r="F91" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/37-Wilson-Rd-Northborough-MA-01532/57626064_zpid/</t>
+        </is>
+      </c>
+      <c r="G91" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/33-Wilson-Rd-Northborough-MA-01532/57626065_zpid/</t>
         </is>
       </c>
     </row>
@@ -2639,9 +3089,14 @@
           <t>761</t>
         </is>
       </c>
-      <c r="F92" t="inlineStr">
+      <c r="F92" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/100-W-Chestnut-Hill-Rd-Montague-MA-01351/56984464_zpid/</t>
+        </is>
+      </c>
+      <c r="G92" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/68-W-Chestnut-Hill-Rd-Montague-MA-01351/56984468_zpid/</t>
         </is>
       </c>
     </row>
@@ -2665,7 +3120,12 @@
           <t>972</t>
         </is>
       </c>
-      <c r="F93" t="inlineStr">
+      <c r="F93" s="0" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/5-Chestnut-Hill-Rd-Warwick-MA-01378/56987857_zpid/</t>
+        </is>
+      </c>
+      <c r="G93" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/5-Chestnut-Hill-Rd-Warwick-MA-01378/56987857_zpid/</t>
         </is>
@@ -2691,7 +3151,12 @@
           <t>613</t>
         </is>
       </c>
-      <c r="F94" t="inlineStr">
+      <c r="F94" s="0" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/100-Montclair-Ave-Waltham-MA-02451/56358859_zpid/</t>
+        </is>
+      </c>
+      <c r="G94" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/100-Montclair-Ave-Waltham-MA-02451/56358859_zpid/</t>
         </is>
@@ -2717,9 +3182,14 @@
           <t>5,707</t>
         </is>
       </c>
-      <c r="F95" t="inlineStr">
+      <c r="F95" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/63-Pokeberry-Rdg-Amherst-MA-01002/56255297_zpid/</t>
+        </is>
+      </c>
+      <c r="G95" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/amherst-ma-01004/sold/9_p/</t>
         </is>
       </c>
     </row>
@@ -2743,7 +3213,12 @@
           <t>1,226</t>
         </is>
       </c>
-      <c r="F96" t="inlineStr">
+      <c r="F96" s="0" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/114-Pine-St-Northampton-MA-01062/57021156_zpid/</t>
+        </is>
+      </c>
+      <c r="G96" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/114-Pine-St-Northampton-MA-01062/57021156_zpid/</t>
         </is>
@@ -2769,7 +3244,12 @@
           <t>740</t>
         </is>
       </c>
-      <c r="F97" t="inlineStr">
+      <c r="F97" s="0" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/27-Hammond-Rd-Hopedale-MA-01747/57602678_zpid/</t>
+        </is>
+      </c>
+      <c r="G97" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/27-Hammond-Rd-Hopedale-MA-01747/57602678_zpid/</t>
         </is>
@@ -2795,7 +3275,12 @@
           <t>951</t>
         </is>
       </c>
-      <c r="F98" t="inlineStr">
+      <c r="F98" s="0" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/38-Blackberry-Ln-Brewster-MA-02631/56769623_zpid/</t>
+        </is>
+      </c>
+      <c r="G98" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/38-Blackberry-Ln-Brewster-MA-02631/56769623_zpid/</t>
         </is>
@@ -2821,7 +3306,12 @@
           <t>2,219</t>
         </is>
       </c>
-      <c r="F99" t="inlineStr">
+      <c r="F99" s="0" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/50-Deerpath-Rd-Dedham-MA-02026/61317928_zpid/</t>
+        </is>
+      </c>
+      <c r="G99" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/50-Deerpath-Rd-Dedham-MA-02026/61317928_zpid/</t>
         </is>
@@ -2847,7 +3337,12 @@
           <t>1,649</t>
         </is>
       </c>
-      <c r="F100" t="inlineStr">
+      <c r="F100" s="0" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/239-Otis-Stage-Rd-Blandford-MA-01008/56989402_zpid/</t>
+        </is>
+      </c>
+      <c r="G100" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/239-Otis-Stage-Rd-Blandford-MA-01008/56989402_zpid/</t>
         </is>
@@ -2873,7 +3368,12 @@
           <t>1,120</t>
         </is>
       </c>
-      <c r="F101" t="inlineStr">
+      <c r="F101" s="0" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/11-Woodland-Dr-Westminster-MA-01473/57681661_zpid/</t>
+        </is>
+      </c>
+      <c r="G101" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/11-Woodland-Dr-Westminster-MA-01473/57681661_zpid/</t>
         </is>
@@ -2899,9 +3399,14 @@
           <t>1,501</t>
         </is>
       </c>
-      <c r="F102" t="inlineStr">
+      <c r="F102" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/4-Barilone-Cir-Maynard-MA-01754/57089849_zpid/</t>
+        </is>
+      </c>
+      <c r="G102" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/7-Barilone-Cir-Maynard-MA-01754/57089852_zpid/</t>
         </is>
       </c>
     </row>
@@ -2925,7 +3430,12 @@
           <t>1,141</t>
         </is>
       </c>
-      <c r="F103" t="inlineStr">
+      <c r="F103" s="0" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/1-Jackson-Ct-Natick-MA-01760/56296174_zpid/</t>
+        </is>
+      </c>
+      <c r="G103" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/1-Jackson-Ct-Natick-MA-01760/56296174_zpid/</t>
         </is>
@@ -2951,7 +3461,12 @@
           <t>1,395</t>
         </is>
       </c>
-      <c r="F104" t="inlineStr">
+      <c r="F104" s="0" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/128-Bridge-St-Manchester-MA-01944/56934086_zpid/</t>
+        </is>
+      </c>
+      <c r="G104" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/128-Bridge-St-Manchester-MA-01944/56934086_zpid/</t>
         </is>
@@ -2977,7 +3492,12 @@
           <t>1,310</t>
         </is>
       </c>
-      <c r="F105" t="inlineStr">
+      <c r="F105" s="0" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/458-East-St-Easthampton-MA-01027/57009565_zpid/</t>
+        </is>
+      </c>
+      <c r="G105" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/458-East-St-Easthampton-MA-01027/57009565_zpid/</t>
         </is>
@@ -3003,7 +3523,12 @@
           <t>1,627</t>
         </is>
       </c>
-      <c r="F106" t="inlineStr">
+      <c r="F106" s="0" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/23-Orchard-St-Northampton-MA-01060/87798678_zpid/</t>
+        </is>
+      </c>
+      <c r="G106" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/23-Orchard-St-Northampton-MA-01060/87798678_zpid/</t>
         </is>
@@ -3029,7 +3554,12 @@
           <t>888</t>
         </is>
       </c>
-      <c r="F107" t="inlineStr">
+      <c r="F107" s="0" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/770-Waltham-St-Lexington-MA-02421/56488902_zpid/</t>
+        </is>
+      </c>
+      <c r="G107" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/770-Waltham-St-Lexington-MA-02421/56488902_zpid/</t>
         </is>
@@ -3055,7 +3585,12 @@
           <t>1,226</t>
         </is>
       </c>
-      <c r="F108" t="inlineStr">
+      <c r="F108" s="0" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/100-Moser-St-Northampton-MA-01060/121252390_zpid/</t>
+        </is>
+      </c>
+      <c r="G108" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/100-Moser-St-Northampton-MA-01060/121252390_zpid/</t>
         </is>
@@ -3081,7 +3616,12 @@
           <t>1,374</t>
         </is>
       </c>
-      <c r="F109" t="inlineStr">
+      <c r="F109" s="0" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/82-Rocky-Neck-Ave-A-Gloucester-MA-01930/2111229081_zpid/</t>
+        </is>
+      </c>
+      <c r="G109" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/82-Rocky-Neck-Ave-A-Gloucester-MA-01930/2111229081_zpid/</t>
         </is>
@@ -3107,7 +3647,12 @@
           <t>1,057</t>
         </is>
       </c>
-      <c r="F110" t="inlineStr">
+      <c r="F110" s="0" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/48-Gannett-Pasture-Ln-Scituate-MA-02066/57222367_zpid/</t>
+        </is>
+      </c>
+      <c r="G110" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/48-Gannett-Pasture-Ln-Scituate-MA-02066/57222367_zpid/</t>
         </is>
@@ -3133,7 +3678,12 @@
           <t>803</t>
         </is>
       </c>
-      <c r="F111" t="inlineStr">
+      <c r="F111" s="0" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/183-Lincoln-Rd-Medford-MA-02155/56275377_zpid/</t>
+        </is>
+      </c>
+      <c r="G111" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/183-Lincoln-Rd-Medford-MA-02155/56275377_zpid/</t>
         </is>
@@ -3159,7 +3709,12 @@
           <t>888</t>
         </is>
       </c>
-      <c r="F112" t="inlineStr">
+      <c r="F112" s="0" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/15-Milne-Rd-Osterville-MA-02655/55853966_zpid/</t>
+        </is>
+      </c>
+      <c r="G112" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/15-Milne-Rd-Osterville-MA-02655/55853966_zpid/</t>
         </is>
@@ -3185,7 +3740,12 @@
           <t>1,289</t>
         </is>
       </c>
-      <c r="F113" t="inlineStr">
+      <c r="F113" s="0" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/4-Pershing-Rd-Needham-MA-02494/57479045_zpid/</t>
+        </is>
+      </c>
+      <c r="G113" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/4-Pershing-Rd-Needham-MA-02494/57479045_zpid/</t>
         </is>
@@ -3211,7 +3771,12 @@
           <t>1,860</t>
         </is>
       </c>
-      <c r="F114" t="inlineStr">
+      <c r="F114" s="0" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/55-Sheffield-Ln-Northampton-MA-01062/57020171_zpid/</t>
+        </is>
+      </c>
+      <c r="G114" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/55-Sheffield-Ln-Northampton-MA-01062/57020171_zpid/</t>
         </is>
@@ -3237,7 +3802,12 @@
           <t>1,522</t>
         </is>
       </c>
-      <c r="F115" t="inlineStr">
+      <c r="F115" s="0" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/51-53-Oakland-St-Melrose-MA-02176/165805876_zpid/</t>
+        </is>
+      </c>
+      <c r="G115" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/51-53-Oakland-St-Melrose-MA-02176/165805876_zpid/</t>
         </is>
@@ -3263,7 +3833,12 @@
           <t>2,177</t>
         </is>
       </c>
-      <c r="F116" t="inlineStr">
+      <c r="F116" s="0" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/42-Wianno-Rd-Bourne-MA-02532/186977019_zpid/</t>
+        </is>
+      </c>
+      <c r="G116" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/42-Wianno-Rd-Bourne-MA-02532/186977019_zpid/</t>
         </is>
@@ -3289,7 +3864,12 @@
           <t>1,162</t>
         </is>
       </c>
-      <c r="F117" t="inlineStr">
+      <c r="F117" s="0" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/16-Common-St-Brookfield-MA-01506/57571006_zpid/</t>
+        </is>
+      </c>
+      <c r="G117" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/16-Common-St-Brookfield-MA-01506/57571006_zpid/</t>
         </is>
@@ -3315,7 +3895,12 @@
           <t>2,283</t>
         </is>
       </c>
-      <c r="F118" t="inlineStr">
+      <c r="F118" s="0" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/235-Bay-Rd-Harwich-MA-02645/186996433_zpid/</t>
+        </is>
+      </c>
+      <c r="G118" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/235-Bay-Rd-Harwich-MA-02645/186996433_zpid/</t>
         </is>
@@ -3341,7 +3926,12 @@
           <t>550</t>
         </is>
       </c>
-      <c r="F119" t="inlineStr">
+      <c r="F119" s="0" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/183-Buckwood-Dr-Hyannis-MA-02601/55846204_zpid/</t>
+        </is>
+      </c>
+      <c r="G119" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/183-Buckwood-Dr-Hyannis-MA-02601/55846204_zpid/</t>
         </is>
@@ -3367,7 +3957,12 @@
           <t>1,860</t>
         </is>
       </c>
-      <c r="F120" t="inlineStr">
+      <c r="F120" s="0" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/35-Woodbury-St-Beverly-MA-01915/59225949_zpid/</t>
+        </is>
+      </c>
+      <c r="G120" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/35-Woodbury-St-Beverly-MA-01915/59225949_zpid/</t>
         </is>
@@ -3393,7 +3988,12 @@
           <t>697</t>
         </is>
       </c>
-      <c r="F121" t="inlineStr">
+      <c r="F121" s="0" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/36-Hill-St-Haverhill-MA-01832/56054458_zpid/</t>
+        </is>
+      </c>
+      <c r="G121" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/36-Hill-St-Haverhill-MA-01832/56054458_zpid/</t>
         </is>
@@ -3419,7 +4019,12 @@
           <t>(Data Not Found)</t>
         </is>
       </c>
-      <c r="F122" t="inlineStr">
+      <c r="F122" s="0" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/27-Hawthorne-Ave-Arlington-MA-02476/56403359_zpid/</t>
+        </is>
+      </c>
+      <c r="G122" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/27-Hawthorne-Ave-Arlington-MA-02476/56403359_zpid/</t>
         </is>
@@ -3445,7 +4050,12 @@
           <t>1,184</t>
         </is>
       </c>
-      <c r="F123" t="inlineStr">
+      <c r="F123" s="0" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/98-Prescott-Rd-Concord-MA-01742/166022245_zpid/</t>
+        </is>
+      </c>
+      <c r="G123" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/98-Prescott-Rd-Concord-MA-01742/166022245_zpid/</t>
         </is>
@@ -3471,7 +4081,12 @@
           <t>1,416</t>
         </is>
       </c>
-      <c r="F124" t="inlineStr">
+      <c r="F124" s="0" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/2-Candida-Ln-Acton-MA-01720/57035751_zpid/</t>
+        </is>
+      </c>
+      <c r="G124" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/2-Candida-Ln-Acton-MA-01720/57035751_zpid/</t>
         </is>
@@ -3497,7 +4112,12 @@
           <t>1,120</t>
         </is>
       </c>
-      <c r="F125" t="inlineStr">
+      <c r="F125" s="0" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/11-Mary-Chilton-Rd-Needham-MA-02492/57480236_zpid/</t>
+        </is>
+      </c>
+      <c r="G125" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/11-Mary-Chilton-Rd-Needham-MA-02492/57480236_zpid/</t>
         </is>
@@ -3523,7 +4143,12 @@
           <t>1,543</t>
         </is>
       </c>
-      <c r="F126" t="inlineStr">
+      <c r="F126" s="0" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/42-Birchtree-Dr-Westwood-MA-02090/57516342_zpid/</t>
+        </is>
+      </c>
+      <c r="G126" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/42-Birchtree-Dr-Westwood-MA-02090/57516342_zpid/</t>
         </is>
@@ -3549,7 +4174,12 @@
           <t>1,522</t>
         </is>
       </c>
-      <c r="F127" t="inlineStr">
+      <c r="F127" s="0" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/279-Davis-St-Northborough-MA-01532/57625738_zpid/</t>
+        </is>
+      </c>
+      <c r="G127" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/279-Davis-St-Northborough-MA-01532/57625738_zpid/</t>
         </is>
@@ -3575,7 +4205,12 @@
           <t>1,247</t>
         </is>
       </c>
-      <c r="F128" t="inlineStr">
+      <c r="F128" s="0" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/32-Oak-Knoll-Dr-Hampden-MA-01036/56173214_zpid/</t>
+        </is>
+      </c>
+      <c r="G128" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/32-Oak-Knoll-Dr-Hampden-MA-01036/56173214_zpid/</t>
         </is>
@@ -3601,7 +4236,12 @@
           <t>1,733</t>
         </is>
       </c>
-      <c r="F129" t="inlineStr">
+      <c r="F129" s="0" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/49-Ford-Xing-Northampton-MA-01060/246300174_zpid/</t>
+        </is>
+      </c>
+      <c r="G129" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/49-Ford-Xing-Northampton-MA-01060/246300174_zpid/</t>
         </is>
@@ -3627,7 +4267,12 @@
           <t>1,078</t>
         </is>
       </c>
-      <c r="F130" t="inlineStr">
+      <c r="F130" s="0" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/15-Grandview-Rd-Haverhill-MA-01832/56054467_zpid/</t>
+        </is>
+      </c>
+      <c r="G130" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/15-Grandview-Rd-Haverhill-MA-01832/56054467_zpid/</t>
         </is>
@@ -3653,7 +4298,12 @@
           <t>2,177</t>
         </is>
       </c>
-      <c r="F131" t="inlineStr">
+      <c r="F131" s="0" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/143-Holden-Wood-Rd-Concord-MA-01742/166020986_zpid/</t>
+        </is>
+      </c>
+      <c r="G131" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/143-Holden-Wood-Rd-Concord-MA-01742/166020986_zpid/</t>
         </is>
@@ -3679,7 +4329,12 @@
           <t>1,670</t>
         </is>
       </c>
-      <c r="F132" t="inlineStr">
+      <c r="F132" s="0" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/117-Park-Rd-Chelmsford-MA-01824/56452429_zpid/</t>
+        </is>
+      </c>
+      <c r="G132" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/117-Park-Rd-Chelmsford-MA-01824/56452429_zpid/</t>
         </is>
@@ -3705,7 +4360,12 @@
           <t>1,522</t>
         </is>
       </c>
-      <c r="F133" t="inlineStr">
+      <c r="F133" s="0" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/177-Monsen-Rd-Concord-MA-01742/166021937_zpid/</t>
+        </is>
+      </c>
+      <c r="G133" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/177-Monsen-Rd-Concord-MA-01742/166021937_zpid/</t>
         </is>
@@ -3731,7 +4391,12 @@
           <t>4,650</t>
         </is>
       </c>
-      <c r="F134" t="inlineStr">
+      <c r="F134" s="0" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/6-Sutton-Pl-Acton-MA-01720/57031615_zpid/</t>
+        </is>
+      </c>
+      <c r="G134" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/6-Sutton-Pl-Acton-MA-01720/57031615_zpid/</t>
         </is>
@@ -3757,7 +4422,12 @@
           <t>486</t>
         </is>
       </c>
-      <c r="F135" t="inlineStr">
+      <c r="F135" s="0" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/286-College-Farm-Rd-Waltham-MA-02451/56358789_zpid/</t>
+        </is>
+      </c>
+      <c r="G135" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/286-College-Farm-Rd-Waltham-MA-02451/56358789_zpid/</t>
         </is>
@@ -3783,7 +4453,12 @@
           <t>719</t>
         </is>
       </c>
-      <c r="F136" t="inlineStr">
+      <c r="F136" s="0" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/1-Wade-Rd-Plainville-MA-02762/57492677_zpid/</t>
+        </is>
+      </c>
+      <c r="G136" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/1-Wade-Rd-Plainville-MA-02762/57492677_zpid/</t>
         </is>
@@ -3809,7 +4484,12 @@
           <t>930</t>
         </is>
       </c>
-      <c r="F137" t="inlineStr">
+      <c r="F137" s="0" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/34-Shannon-Way-Dartmouth-MA-02747/59880382_zpid/</t>
+        </is>
+      </c>
+      <c r="G137" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/34-Shannon-Way-Dartmouth-MA-02747/59880382_zpid/</t>
         </is>
@@ -3835,7 +4515,12 @@
           <t>2,177</t>
         </is>
       </c>
-      <c r="F138" t="inlineStr">
+      <c r="F138" s="0" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/13-Secluded-Rdg-Southwick-MA-01077/56996781_zpid/</t>
+        </is>
+      </c>
+      <c r="G138" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/13-Secluded-Rdg-Southwick-MA-01077/56996781_zpid/</t>
         </is>
@@ -3861,7 +4546,12 @@
           <t>613</t>
         </is>
       </c>
-      <c r="F139" t="inlineStr">
+      <c r="F139" s="0" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/23-Powell-St-Northampton-MA-01062/57020013_zpid/</t>
+        </is>
+      </c>
+      <c r="G139" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/23-Powell-St-Northampton-MA-01062/57020013_zpid/</t>
         </is>
@@ -3887,7 +4577,12 @@
           <t>296</t>
         </is>
       </c>
-      <c r="F140" t="inlineStr">
+      <c r="F140" s="0" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/4-Sheeps-Crossing-Ln-Falmouth-MA-02543/55898730_zpid/</t>
+        </is>
+      </c>
+      <c r="G140" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/4-Sheeps-Crossing-Ln-Falmouth-MA-02543/55898730_zpid/</t>
         </is>
@@ -3913,7 +4608,12 @@
           <t>2,092</t>
         </is>
       </c>
-      <c r="F141" t="inlineStr">
+      <c r="F141" s="0" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/7-Pheasant-Ln-Topsfield-MA-01983/56969630_zpid/</t>
+        </is>
+      </c>
+      <c r="G141" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/7-Pheasant-Ln-Topsfield-MA-01983/56969630_zpid/</t>
         </is>
@@ -3939,7 +4639,12 @@
           <t>2,431</t>
         </is>
       </c>
-      <c r="F142" t="inlineStr">
+      <c r="F142" s="0" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/336-Station-Rd-Amherst-MA-01002/56258370_zpid/</t>
+        </is>
+      </c>
+      <c r="G142" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/336-Station-Rd-Amherst-MA-01002/56258370_zpid/</t>
         </is>
@@ -3965,7 +4670,12 @@
           <t>592</t>
         </is>
       </c>
-      <c r="F143" t="inlineStr">
+      <c r="F143" s="0" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/14-Mount-Walley-Rd-Waltham-MA-02451/56359215_zpid/</t>
+        </is>
+      </c>
+      <c r="G143" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/14-Mount-Walley-Rd-Waltham-MA-02451/56359215_zpid/</t>
         </is>
@@ -3991,7 +4701,12 @@
           <t>1,437</t>
         </is>
       </c>
-      <c r="F144" t="inlineStr">
+      <c r="F144" s="0" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/10-Aloha-Dr-Hadley-MA-01035/57015527_zpid/</t>
+        </is>
+      </c>
+      <c r="G144" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/10-Aloha-Dr-Hadley-MA-01035/57015527_zpid/</t>
         </is>
@@ -4017,7 +4732,12 @@
           <t>571</t>
         </is>
       </c>
-      <c r="F145" t="inlineStr">
+      <c r="F145" s="0" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/18-Mount-Ida-Ter-Waltham-MA-02451/56359233_zpid/</t>
+        </is>
+      </c>
+      <c r="G145" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/18-Mount-Ida-Ter-Waltham-MA-02451/56359233_zpid/</t>
         </is>
@@ -4043,7 +4763,12 @@
           <t>909</t>
         </is>
       </c>
-      <c r="F146" t="inlineStr">
+      <c r="F146" s="0" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/7-Oak-Ridge-Rd-East-Falmouth-MA-02536/55891673_zpid/</t>
+        </is>
+      </c>
+      <c r="G146" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/7-Oak-Ridge-Rd-East-Falmouth-MA-02536/55891673_zpid/</t>
         </is>
@@ -4069,7 +4794,12 @@
           <t>528</t>
         </is>
       </c>
-      <c r="F147" t="inlineStr">
+      <c r="F147" s="0" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/175-Shepardson-Rd-Warwick-MA-01378/56987841_zpid/</t>
+        </is>
+      </c>
+      <c r="G147" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/175-Shepardson-Rd-Warwick-MA-01378/56987841_zpid/</t>
         </is>
@@ -4095,7 +4825,12 @@
           <t>824</t>
         </is>
       </c>
-      <c r="F148" t="inlineStr">
+      <c r="F148" s="0" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/33-Hill-St-Haverhill-MA-01832/56054482_zpid/</t>
+        </is>
+      </c>
+      <c r="G148" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/33-Hill-St-Haverhill-MA-01832/56054482_zpid/</t>
         </is>
@@ -4121,7 +4856,12 @@
           <t>845</t>
         </is>
       </c>
-      <c r="F149" t="inlineStr">
+      <c r="F149" s="0" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/6-Pine-Ave-Tyngsboro-MA-01879/57122748_zpid/</t>
+        </is>
+      </c>
+      <c r="G149" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/6-Pine-Ave-Tyngsboro-MA-01879/57122748_zpid/</t>
         </is>
@@ -4147,7 +4887,12 @@
           <t>845</t>
         </is>
       </c>
-      <c r="F150" t="inlineStr">
+      <c r="F150" s="0" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/12-Barbara-Cir-Burlington-MA-01803/57056333_zpid/</t>
+        </is>
+      </c>
+      <c r="G150" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/12-Barbara-Cir-Burlington-MA-01803/57056333_zpid/</t>
         </is>
@@ -4173,6 +4918,11 @@
           <t>634</t>
         </is>
       </c>
+      <c r="G151" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/52-Stickney-Rd-Medford-MA-02155/56275415_zpid/</t>
+        </is>
+      </c>
     </row>
     <row r="152" ht="15.75" customHeight="1" s="7">
       <c r="A152" s="6" t="inlineStr">
@@ -4194,6 +4944,11 @@
           <t>1,226</t>
         </is>
       </c>
+      <c r="G152" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/16-Stedman-St-Chelmsford-MA-01824/56446782_zpid/</t>
+        </is>
+      </c>
     </row>
     <row r="153" ht="15.75" customHeight="1" s="7">
       <c r="A153" s="6" t="inlineStr">
@@ -4215,6 +4970,11 @@
           <t>465</t>
         </is>
       </c>
+      <c r="G153" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/37-Andrews-St-Medford-MA-02155/56273730_zpid/</t>
+        </is>
+      </c>
     </row>
     <row r="154" ht="15.75" customHeight="1" s="7">
       <c r="A154" s="6" t="inlineStr">
@@ -4236,6 +4996,11 @@
           <t>528</t>
         </is>
       </c>
+      <c r="G154" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/49-Braemore-Rd-Waltham-MA-02451/56358904_zpid/</t>
+        </is>
+      </c>
     </row>
     <row r="155" ht="15.75" customHeight="1" s="7">
       <c r="A155" s="6" t="inlineStr">
@@ -4257,6 +5022,11 @@
           <t>1,015</t>
         </is>
       </c>
+      <c r="G155" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/1-Stockdale-Rd-Needham-MA-02492/57478584_zpid/</t>
+        </is>
+      </c>
     </row>
     <row r="156" ht="15.75" customHeight="1" s="7">
       <c r="A156" s="6" t="inlineStr">
@@ -4278,6 +5048,11 @@
           <t>1,141</t>
         </is>
       </c>
+      <c r="G156" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/67-Greenwood-Ave-Needham-MA-02492/57475276_zpid/</t>
+        </is>
+      </c>
     </row>
     <row r="157" ht="15.75" customHeight="1" s="7">
       <c r="A157" s="6" t="inlineStr">
@@ -4299,6 +5074,11 @@
           <t>1,754</t>
         </is>
       </c>
+      <c r="G157" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/34-Seltsam-Way-Pembroke-MA-02359/121878579_zpid/</t>
+        </is>
+      </c>
     </row>
     <row r="158" ht="15.75" customHeight="1" s="7">
       <c r="A158" s="6" t="inlineStr">
@@ -4320,6 +5100,11 @@
           <t>1,966</t>
         </is>
       </c>
+      <c r="G158" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/260-Vaughn-Hill-Rd-Bolton-MA-01740/57568665_zpid/</t>
+        </is>
+      </c>
     </row>
     <row r="159" ht="15.75" customHeight="1" s="7">
       <c r="A159" s="6" t="inlineStr">
@@ -4341,6 +5126,11 @@
           <t>2,642</t>
         </is>
       </c>
+      <c r="G159" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/5-Merrinott-Rd-Bolton-MA-01740/57568570_zpid/</t>
+        </is>
+      </c>
     </row>
     <row r="160" ht="15.75" customHeight="1" s="7">
       <c r="A160" s="6" t="inlineStr">
@@ -4362,6 +5152,11 @@
           <t>867</t>
         </is>
       </c>
+      <c r="G160" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/76-Woodlot-Rd-Amherst-MA-01002/56258359_zpid/</t>
+        </is>
+      </c>
     </row>
     <row r="161" ht="15.75" customHeight="1" s="7">
       <c r="A161" s="6" t="inlineStr">
@@ -4383,6 +5178,11 @@
           <t>2,240</t>
         </is>
       </c>
+      <c r="G161" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/26-Foxglove-Ln-Amherst-MA-01002/56258411_zpid/</t>
+        </is>
+      </c>
     </row>
     <row r="162" ht="15.75" customHeight="1" s="7">
       <c r="A162" s="6" t="inlineStr">
@@ -4404,6 +5204,11 @@
           <t>2,705</t>
         </is>
       </c>
+      <c r="G162" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/12-Bayberry-Ln-Hadley-MA-01035/67714823_zpid/</t>
+        </is>
+      </c>
     </row>
     <row r="163" ht="15.75" customHeight="1" s="7">
       <c r="A163" s="6" t="inlineStr">
@@ -4425,6 +5230,11 @@
           <t>1,141</t>
         </is>
       </c>
+      <c r="G163" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/124-Moser-St-Northampton-MA-01060/121251942_zpid/</t>
+        </is>
+      </c>
     </row>
     <row r="164" ht="15.75" customHeight="1" s="7">
       <c r="A164" s="6" t="inlineStr">
@@ -4446,6 +5256,11 @@
           <t>1,754</t>
         </is>
       </c>
+      <c r="G164" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/442-East-St-Easthampton-MA-01027/59881486_zpid/</t>
+        </is>
+      </c>
     </row>
     <row r="165" ht="15.75" customHeight="1" s="7">
       <c r="A165" s="6" t="inlineStr">
@@ -4467,6 +5282,11 @@
           <t>1,416</t>
         </is>
       </c>
+      <c r="G165" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/5-Bean-Porridge-Hill-Rd-Westminster-MA-01473/57681454_zpid/</t>
+        </is>
+      </c>
     </row>
     <row r="166" ht="15.75" customHeight="1" s="7">
       <c r="A166" s="6" t="inlineStr">
@@ -4488,6 +5308,11 @@
           <t>803</t>
         </is>
       </c>
+      <c r="G166" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/68-McGee-Dr-Hyannis-MA-02601/55846054_zpid/</t>
+        </is>
+      </c>
     </row>
     <row r="167" ht="15.75" customHeight="1" s="7">
       <c r="A167" s="6" t="inlineStr">
@@ -4509,6 +5334,11 @@
           <t>1,141</t>
         </is>
       </c>
+      <c r="G167" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/118-Wild-Harbor-Rd-North-Falmouth-MA-02556/55881954_zpid/</t>
+        </is>
+      </c>
     </row>
     <row r="168" ht="15.75" customHeight="1" s="7">
       <c r="A168" s="6" t="inlineStr">
@@ -4530,6 +5360,11 @@
           <t>1,289</t>
         </is>
       </c>
+      <c r="G168" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/46-Scotland-Heights-Rd-Haverhill-MA-01832/56056737_zpid/</t>
+        </is>
+      </c>
     </row>
     <row r="169" ht="15.75" customHeight="1" s="7">
       <c r="A169" s="6" t="inlineStr">
@@ -4551,6 +5386,11 @@
           <t>1,416</t>
         </is>
       </c>
+      <c r="G169" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/13-Kenwood-St-Chelmsford-MA-01824/56451880_zpid/</t>
+        </is>
+      </c>
     </row>
     <row r="170" ht="15.75" customHeight="1" s="7">
       <c r="A170" s="6" t="inlineStr">
@@ -4572,6 +5412,11 @@
           <t>1,437</t>
         </is>
       </c>
+      <c r="G170" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/22-Orchard-Ln-Groton-MA-01450/61315789_zpid/</t>
+        </is>
+      </c>
     </row>
     <row r="171" ht="15.75" customHeight="1" s="7">
       <c r="A171" s="6" t="inlineStr">
@@ -4593,6 +5438,11 @@
           <t>613</t>
         </is>
       </c>
+      <c r="G171" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/84-Ramshead-Rd-Medford-MA-02155/56275351_zpid/</t>
+        </is>
+      </c>
     </row>
     <row r="172" ht="15.75" customHeight="1" s="7">
       <c r="A172" s="6" t="inlineStr">
@@ -4614,6 +5464,11 @@
           <t>444</t>
         </is>
       </c>
+      <c r="G172" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/25-Stockdale-Rd-Needham-MA-02492/57478581_zpid/</t>
+        </is>
+      </c>
     </row>
     <row r="173" ht="15.75" customHeight="1" s="7">
       <c r="A173" s="6" t="inlineStr">
@@ -4635,6 +5490,11 @@
           <t>486</t>
         </is>
       </c>
+      <c r="G173" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/34-Rawson-Rd-Bellingham-MA-02019/57424042_zpid/</t>
+        </is>
+      </c>
     </row>
     <row r="174" ht="15.75" customHeight="1" s="7">
       <c r="A174" s="6" t="inlineStr">
@@ -4656,6 +5516,11 @@
           <t>2,071</t>
         </is>
       </c>
+      <c r="G174" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/155-Raymond-Dr-Hampden-MA-01036/56173315_zpid/</t>
+        </is>
+      </c>
     </row>
     <row r="175" ht="15.75" customHeight="1" s="7">
       <c r="A175" s="6" t="inlineStr">
@@ -4677,6 +5542,11 @@
           <t>2,240</t>
         </is>
       </c>
+      <c r="G175" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/37-Harris-St-Amherst-MA-01002/56254550_zpid/</t>
+        </is>
+      </c>
     </row>
     <row r="176" ht="15.75" customHeight="1" s="7">
       <c r="A176" s="6" t="inlineStr">
@@ -4698,6 +5568,11 @@
           <t>1,818</t>
         </is>
       </c>
+      <c r="G176" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/19-Foxglove-Ln-Amherst-MA-01002/56258404_zpid/</t>
+        </is>
+      </c>
     </row>
     <row r="177" ht="15.75" customHeight="1" s="7">
       <c r="A177" s="6" t="inlineStr">
@@ -4719,6 +5594,11 @@
           <t>550</t>
         </is>
       </c>
+      <c r="G177" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/10-Frost-Ln-Hadley-MA-01035/57015383_zpid/</t>
+        </is>
+      </c>
     </row>
     <row r="178" ht="15.75" customHeight="1" s="7">
       <c r="A178" s="6" t="inlineStr">
@@ -4740,6 +5620,11 @@
           <t>1,099</t>
         </is>
       </c>
+      <c r="G178" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/104-Wildflower-Dr-Amherst-MA-01002/56258337_zpid/</t>
+        </is>
+      </c>
     </row>
     <row r="179" ht="15.75" customHeight="1" s="7">
       <c r="A179" s="6" t="inlineStr">
@@ -4761,6 +5646,11 @@
           <t>2,050</t>
         </is>
       </c>
+      <c r="G179" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/152-Birchtree-Dr-Westwood-MA-02090/57515978_zpid/</t>
+        </is>
+      </c>
     </row>
     <row r="180" ht="15.75" customHeight="1" s="7">
       <c r="A180" s="6" t="inlineStr">
@@ -4782,6 +5672,11 @@
           <t>317</t>
         </is>
       </c>
+      <c r="G180" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/21-Blaisdell-Rd-Medford-MA-02155/56275330_zpid/</t>
+        </is>
+      </c>
     </row>
     <row r="181" ht="15.75" customHeight="1" s="7">
       <c r="A181" s="6" t="inlineStr">
@@ -4803,6 +5698,11 @@
           <t>655</t>
         </is>
       </c>
+      <c r="G181" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/28-Longview-Rd-North-Falmouth-MA-02556/55883394_zpid/</t>
+        </is>
+      </c>
     </row>
     <row r="182" ht="15.75" customHeight="1" s="7">
       <c r="A182" s="6" t="inlineStr">
@@ -4824,6 +5724,11 @@
           <t>1,310</t>
         </is>
       </c>
+      <c r="G182" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/25-Kaileys-Way-Groton-MA-01450/57066228_zpid/</t>
+        </is>
+      </c>
     </row>
     <row r="183" ht="15.75" customHeight="1" s="7">
       <c r="A183" s="6" t="inlineStr">
@@ -4845,6 +5750,11 @@
           <t>1,099</t>
         </is>
       </c>
+      <c r="G183" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/55-Cedar-Hill-Rd-Bellingham-MA-02019/57423546_zpid/</t>
+        </is>
+      </c>
     </row>
     <row r="184" ht="15.75" customHeight="1" s="7">
       <c r="A184" s="6" t="inlineStr">
@@ -4866,6 +5776,11 @@
           <t>1,015</t>
         </is>
       </c>
+      <c r="G184" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/10-Hillview-Ln-Plymouth-MA-02360/71374281_zpid/</t>
+        </is>
+      </c>
     </row>
     <row r="185" ht="15.75" customHeight="1" s="7">
       <c r="A185" s="6" t="inlineStr">
@@ -4887,6 +5802,11 @@
           <t>1,310</t>
         </is>
       </c>
+      <c r="G185" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/15-Hope-St-Hopedale-MA-01747/57603536_zpid/</t>
+        </is>
+      </c>
     </row>
     <row r="186" ht="15.75" customHeight="1" s="7">
       <c r="A186" s="6" t="inlineStr">
@@ -4908,6 +5828,11 @@
           <t>1,923</t>
         </is>
       </c>
+      <c r="G186" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/7-Kennedy-Dr-Hadley-MA-01035/57015490_zpid/</t>
+        </is>
+      </c>
     </row>
     <row r="187" ht="15.75" customHeight="1" s="7">
       <c r="A187" s="6" t="inlineStr">
@@ -4929,6 +5854,11 @@
           <t>1,966</t>
         </is>
       </c>
+      <c r="G187" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/4-Bayberry-Ln-Hadley-MA-01035/61806216_zpid/</t>
+        </is>
+      </c>
     </row>
     <row r="188" ht="15.75" customHeight="1" s="7">
       <c r="A188" s="6" t="inlineStr">
@@ -4950,6 +5880,11 @@
           <t>1,226</t>
         </is>
       </c>
+      <c r="G188" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/130-Hillcrest-Dr-Northampton-MA-01062/57020096_zpid/</t>
+        </is>
+      </c>
     </row>
     <row r="189" ht="15.75" customHeight="1" s="7">
       <c r="A189" s="6" t="inlineStr">
@@ -4971,6 +5906,11 @@
           <t>2,536</t>
         </is>
       </c>
+      <c r="G189" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/91-Moser-St-Northampton-MA-01060/121252645_zpid/</t>
+        </is>
+      </c>
     </row>
     <row r="190" ht="15.75" customHeight="1" s="7">
       <c r="A190" s="6" t="inlineStr">
@@ -4992,6 +5932,11 @@
           <t>1,902</t>
         </is>
       </c>
+      <c r="G190" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/5-Elm-Top-Ln-Beverly-MA-01915/59225870_zpid/</t>
+        </is>
+      </c>
     </row>
     <row r="191" ht="15.75" customHeight="1" s="7">
       <c r="A191" s="6" t="inlineStr">
@@ -5013,6 +5958,11 @@
           <t>888</t>
         </is>
       </c>
+      <c r="G191" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/89-Park-Rd-Chelmsford-MA-01824/56451860_zpid/</t>
+        </is>
+      </c>
     </row>
     <row r="192" ht="15.75" customHeight="1" s="7">
       <c r="A192" s="6" t="inlineStr">
@@ -5034,6 +5984,11 @@
           <t>1,522</t>
         </is>
       </c>
+      <c r="G192" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/4-Grasshopper-Ln-Oxford-MA-01540/60027617_zpid/</t>
+        </is>
+      </c>
     </row>
     <row r="193" ht="15.75" customHeight="1" s="7">
       <c r="A193" s="6" t="inlineStr">
@@ -5055,6 +6010,11 @@
           <t>1,184</t>
         </is>
       </c>
+      <c r="G193" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/17-Bakers-Dr-Harwich-MA-02645/55904878_zpid/</t>
+        </is>
+      </c>
     </row>
     <row r="194" ht="15.75" customHeight="1" s="7">
       <c r="A194" s="6" t="inlineStr">
@@ -5076,6 +6036,11 @@
           <t>254</t>
         </is>
       </c>
+      <c r="G194" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/49-Bakers-Dr-Harwich-MA-02645/186993268_zpid/</t>
+        </is>
+      </c>
     </row>
     <row r="195" ht="15.75" customHeight="1" s="7">
       <c r="A195" s="6" t="inlineStr">
@@ -5097,6 +6062,11 @@
           <t>909</t>
         </is>
       </c>
+      <c r="G195" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/28-Stedman-St-Chelmsford-MA-01824/56446777_zpid/</t>
+        </is>
+      </c>
     </row>
     <row r="196" ht="15.75" customHeight="1" s="7">
       <c r="A196" s="6" t="inlineStr">
@@ -5118,6 +6088,11 @@
           <t>1,818</t>
         </is>
       </c>
+      <c r="G196" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/1123-Monument-St-Concord-MA-01742/166021646_zpid/</t>
+        </is>
+      </c>
     </row>
     <row r="197" ht="15.75" customHeight="1" s="7">
       <c r="A197" s="6" t="inlineStr">
@@ -5139,6 +6114,11 @@
           <t>1,437</t>
         </is>
       </c>
+      <c r="G197" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/58-Farmers-Cliff-Rd-Concord-MA-01742/166021917_zpid/</t>
+        </is>
+      </c>
     </row>
     <row r="198" ht="15.75" customHeight="1" s="7">
       <c r="A198" s="6" t="inlineStr">
@@ -5160,6 +6140,11 @@
           <t>972</t>
         </is>
       </c>
+      <c r="G198" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/7-Barilone-Cir-Maynard-MA-01754/57089852_zpid/</t>
+        </is>
+      </c>
     </row>
     <row r="199" ht="15.75" customHeight="1" s="7">
       <c r="A199" s="6" t="inlineStr">
@@ -5181,6 +6166,11 @@
           <t>1,543</t>
         </is>
       </c>
+      <c r="G199" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/16-Ash-Ln-Dudley-MA-01571/59207910_zpid/</t>
+        </is>
+      </c>
     </row>
     <row r="200" ht="15.75" customHeight="1" s="7">
       <c r="A200" s="6" t="inlineStr">
@@ -5202,6 +6192,11 @@
           <t>2,367</t>
         </is>
       </c>
+      <c r="G200" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/225-Nonotuck-St-B-Northampton-MA-01062/92203160_zpid/</t>
+        </is>
+      </c>
     </row>
     <row r="201" ht="15.75" customHeight="1" s="7">
       <c r="A201" s="6" t="inlineStr">
@@ -5223,6 +6218,11 @@
           <t>1,247</t>
         </is>
       </c>
+      <c r="G201" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/1-Honey-Hill-Rd-Cummington-MA-01026/57006376_zpid/</t>
+        </is>
+      </c>
     </row>
     <row r="202" ht="15.75" customHeight="1" s="7">
       <c r="A202" s="6" t="inlineStr">
@@ -5244,6 +6244,11 @@
           <t>1,691</t>
         </is>
       </c>
+      <c r="G202" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/208-Trouble-St-Cummington-MA-01026/57006372_zpid/</t>
+        </is>
+      </c>
     </row>
     <row r="203" ht="15.75" customHeight="1" s="7">
       <c r="A203" s="6" t="inlineStr">
@@ -5265,6 +6270,11 @@
           <t>845</t>
         </is>
       </c>
+      <c r="G203" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/80-Wigwam-St-Wellfleet-MA-02667/56794929_zpid/</t>
+        </is>
+      </c>
     </row>
     <row r="204" ht="15.75" customHeight="1" s="7">
       <c r="A204" s="6" t="inlineStr">
@@ -5286,6 +6296,11 @@
           <t>2,536</t>
         </is>
       </c>
+      <c r="G204" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/100-Waterfield-Rd-Osterville-MA-02655/55854086_zpid/</t>
+        </is>
+      </c>
     </row>
     <row r="205" ht="15.75" customHeight="1" s="7">
       <c r="A205" s="6" t="inlineStr">
@@ -5307,6 +6322,11 @@
           <t>211</t>
         </is>
       </c>
+      <c r="G205" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/27-Columbus-Ave-Somerville-MA-02143/56333517_zpid/</t>
+        </is>
+      </c>
     </row>
     <row r="206" ht="15.75" customHeight="1" s="7">
       <c r="A206" s="6" t="inlineStr">
@@ -5328,6 +6348,11 @@
           <t>1,797</t>
         </is>
       </c>
+      <c r="G206" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/9-Snake-Brook-Rd-Wayland-MA-01778/57127136_zpid/</t>
+        </is>
+      </c>
     </row>
     <row r="207" ht="15.75" customHeight="1" s="7">
       <c r="A207" s="6" t="inlineStr">
@@ -5349,6 +6374,11 @@
           <t>676</t>
         </is>
       </c>
+      <c r="G207" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/23-Oak-St-Wayland-MA-01778/57127303_zpid/</t>
+        </is>
+      </c>
     </row>
     <row r="208" ht="15.75" customHeight="1" s="7">
       <c r="A208" s="6" t="inlineStr">
@@ -5370,6 +6400,11 @@
           <t>359</t>
         </is>
       </c>
+      <c r="G208" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/231-Melrose-St-Newton-MA-02466/56309625_zpid/</t>
+        </is>
+      </c>
     </row>
     <row r="209" ht="15.75" customHeight="1" s="7">
       <c r="A209" s="6" t="inlineStr">
@@ -5391,6 +6426,11 @@
           <t>719</t>
         </is>
       </c>
+      <c r="G209" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/47-Kingswood-Rd-Newton-MA-02466/56309758_zpid/</t>
+        </is>
+      </c>
     </row>
     <row r="210" ht="15.75" customHeight="1" s="7">
       <c r="A210" s="6" t="inlineStr">
@@ -5410,6 +6450,11 @@
       <c r="E210" s="6" t="inlineStr">
         <is>
           <t>761</t>
+        </is>
+      </c>
+      <c r="G210" t="inlineStr">
+        <is>
+          <t>https://www.zillow.com/homedetails/45-July-St-Lowell-MA-01850/56511098_zpid/</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
updates excel with zillow data, and modifed logic for bright data collection
</commit_message>
<xml_diff>
--- a/res-econ_RA_data.xlsx
+++ b/res-econ_RA_data.xlsx
@@ -356,7 +356,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F999"/>
+  <dimension ref="A1:O999"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -419,9 +419,44 @@
           <t>2,346</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="F2" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/6-Standish-Cir-Andover-MA-01810/56034004_zpid/</t>
+        </is>
+      </c>
+      <c r="G2" s="0" t="n">
+        <v>894400</v>
+      </c>
+      <c r="H2" s="0" t="n">
+        <v>752900</v>
+      </c>
+      <c r="I2" s="0" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="J2" s="0" t="n">
+        <v>2148</v>
+      </c>
+      <c r="K2" s="0" t="n">
+        <v>1964</v>
+      </c>
+      <c r="L2" s="0" t="n">
+        <v>0.4699954086317722</v>
+      </c>
+      <c r="M2" s="0" t="inlineStr">
+        <is>
+          <t>Acres</t>
+        </is>
+      </c>
+      <c r="N2" s="0" t="inlineStr">
+        <is>
+          <t>Forced air,Gas</t>
+        </is>
+      </c>
+      <c r="O2" s="0" t="inlineStr">
+        <is>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -445,9 +480,44 @@
           <t>719</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr">
+      <c r="F3" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/150-Traincroft-NW-Medford-MA-02155/56277119_zpid/</t>
+        </is>
+      </c>
+      <c r="G3" s="0" t="n">
+        <v>1191400</v>
+      </c>
+      <c r="H3" s="0" t="n">
+        <v>931700</v>
+      </c>
+      <c r="I3" s="0" t="inlineStr">
+        <is>
+          <t>2012-07-24</t>
+        </is>
+      </c>
+      <c r="J3" s="0" t="n">
+        <v>2258</v>
+      </c>
+      <c r="K3" s="0" t="n">
+        <v>1929</v>
+      </c>
+      <c r="L3" s="0" t="n">
+        <v>7405</v>
+      </c>
+      <c r="M3" s="0" t="inlineStr">
+        <is>
+          <t>Square Feet</t>
+        </is>
+      </c>
+      <c r="N3" s="0" t="inlineStr">
+        <is>
+          <t>Forced air,Gas</t>
+        </is>
+      </c>
+      <c r="O3" s="0" t="inlineStr">
+        <is>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -471,9 +541,44 @@
           <t>1,015</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr">
+      <c r="F4" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/24-Dean-Rd-Wayland-MA-01778/57127108_zpid/</t>
+        </is>
+      </c>
+      <c r="G4" s="0" t="n">
+        <v>1030900</v>
+      </c>
+      <c r="H4" s="0" t="n">
+        <v>831600</v>
+      </c>
+      <c r="I4" s="0" t="inlineStr">
+        <is>
+          <t>2008-06-27</t>
+        </is>
+      </c>
+      <c r="J4" s="0" t="n">
+        <v>1668</v>
+      </c>
+      <c r="K4" s="0" t="n">
+        <v>1952</v>
+      </c>
+      <c r="L4" s="0" t="n">
+        <v>0.5799816345270891</v>
+      </c>
+      <c r="M4" s="0" t="inlineStr">
+        <is>
+          <t>Acres</t>
+        </is>
+      </c>
+      <c r="N4" s="0" t="inlineStr">
+        <is>
+          <t>Forced air,Gas</t>
+        </is>
+      </c>
+      <c r="O4" s="0" t="inlineStr">
+        <is>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -497,7 +602,7 @@
           <t>1,754</t>
         </is>
       </c>
-      <c r="F5" t="inlineStr">
+      <c r="F5" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/173-Bay-Rd-Harwich-MA-02645/186993999_zpid/</t>
         </is>
@@ -523,9 +628,44 @@
           <t>1,289</t>
         </is>
       </c>
-      <c r="F6" t="inlineStr">
+      <c r="F6" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/1-Ladyslipper-Ln-Hadley-MA-01035/57015531_zpid/</t>
+        </is>
+      </c>
+      <c r="G6" t="n">
+        <v>631400</v>
+      </c>
+      <c r="H6" t="n">
+        <v>505800</v>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>1987-09-01</t>
+        </is>
+      </c>
+      <c r="J6" t="n">
+        <v>2366</v>
+      </c>
+      <c r="K6" t="n">
+        <v>1987</v>
+      </c>
+      <c r="L6" t="n">
+        <v>0.55</v>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>Acres</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>Other,Oil</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -549,9 +689,44 @@
           <t>1,627</t>
         </is>
       </c>
-      <c r="F7" t="inlineStr">
+      <c r="F7" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/170-Kilkore-Dr-Hyannis-MA-02601/55846500_zpid/</t>
+        </is>
+      </c>
+      <c r="G7" t="n">
+        <v>757800</v>
+      </c>
+      <c r="H7" t="n">
+        <v>622300</v>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>2008-10-16</t>
+        </is>
+      </c>
+      <c r="J7" t="n">
+        <v>1612</v>
+      </c>
+      <c r="K7" t="n">
+        <v>2000</v>
+      </c>
+      <c r="L7" t="n">
+        <v>9583</v>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>Square Feet</t>
+        </is>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>Forced air,Gas</t>
+        </is>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>Central</t>
         </is>
       </c>
     </row>
@@ -575,9 +750,44 @@
           <t>380</t>
         </is>
       </c>
-      <c r="F8" t="inlineStr">
+      <c r="F8" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/39-Stevens-St-Stoneham-MA-02180/56336960_zpid/</t>
+        </is>
+      </c>
+      <c r="G8" t="n">
+        <v>793400</v>
+      </c>
+      <c r="H8" t="n">
+        <v>655300</v>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>1996-05-24</t>
+        </is>
+      </c>
+      <c r="J8" t="n">
+        <v>1333</v>
+      </c>
+      <c r="K8" t="n">
+        <v>1930</v>
+      </c>
+      <c r="L8" t="n">
+        <v>0.3994490358126722</v>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>Acres</t>
+        </is>
+      </c>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>Heat pump,Electric,Solar</t>
+        </is>
+      </c>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>Central,Solar</t>
         </is>
       </c>
     </row>
@@ -601,9 +811,44 @@
           <t>1,310</t>
         </is>
       </c>
-      <c r="F9" t="inlineStr">
+      <c r="F9" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/17-Milbery-Ln-Pembroke-MA-02359/57536844_zpid/</t>
+        </is>
+      </c>
+      <c r="G9" t="n">
+        <v>896300</v>
+      </c>
+      <c r="H9" t="n">
+        <v>736800</v>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="J9" t="n">
+        <v>2520</v>
+      </c>
+      <c r="K9" t="n">
+        <v>1989</v>
+      </c>
+      <c r="L9" t="n">
+        <v>1.069995408631772</v>
+      </c>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>Acres</t>
+        </is>
+      </c>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>Other,Oil</t>
+        </is>
+      </c>
+      <c r="O9" t="inlineStr">
+        <is>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -627,9 +872,44 @@
           <t>1,141</t>
         </is>
       </c>
-      <c r="F10" t="inlineStr">
+      <c r="F10" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/16-Harris-Ln-Harvard-MA-01451/173940899_zpid/</t>
+        </is>
+      </c>
+      <c r="G10" t="n">
+        <v>1207700</v>
+      </c>
+      <c r="H10" t="n">
+        <v>985500</v>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>2015-08-14</t>
+        </is>
+      </c>
+      <c r="J10" t="n">
+        <v>3564</v>
+      </c>
+      <c r="K10" t="n">
+        <v>2000</v>
+      </c>
+      <c r="L10" t="n">
+        <v>4.479981634527089</v>
+      </c>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>Acres</t>
+        </is>
+      </c>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>Forced air,Heat pump,Stove,Oil,Solar,Wood / Pellet</t>
+        </is>
+      </c>
+      <c r="O10" t="inlineStr">
+        <is>
+          <t>Central,Solar</t>
         </is>
       </c>
     </row>
@@ -653,7 +933,7 @@
           <t>909</t>
         </is>
       </c>
-      <c r="F11" t="inlineStr">
+      <c r="F11" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/21-White-Oaks-Rd-Williamstown-MA-01267/56819688_zpid/</t>
         </is>
@@ -679,7 +959,7 @@
           <t>2,325</t>
         </is>
       </c>
-      <c r="F12" t="inlineStr">
+      <c r="F12" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/20-Overlook-Dr-East-Longmeadow-MA-01028/56171418_zpid/</t>
         </is>
@@ -705,7 +985,7 @@
           <t>1,036</t>
         </is>
       </c>
-      <c r="F13" t="inlineStr">
+      <c r="F13" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/58-Linda-Ave-Framingham-MA-01701/165985595_zpid/</t>
         </is>
@@ -731,7 +1011,7 @@
           <t>2,198</t>
         </is>
       </c>
-      <c r="F14" t="inlineStr">
+      <c r="F14" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/19-Holly-Cir-Easthampton-MA-01027/57009823_zpid/</t>
         </is>
@@ -757,7 +1037,7 @@
           <t>1,966</t>
         </is>
       </c>
-      <c r="F15" t="inlineStr">
+      <c r="F15" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/31-E-Sound-Ln-Tisbury-MA-02568/56900325_zpid/</t>
         </is>
@@ -783,7 +1063,7 @@
           <t>909</t>
         </is>
       </c>
-      <c r="F16" t="inlineStr">
+      <c r="F16" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/156-Standish-Rd-Needham-MA-02492/57478769_zpid/</t>
         </is>
@@ -809,7 +1089,7 @@
           <t>2,283</t>
         </is>
       </c>
-      <c r="F17" t="inlineStr">
+      <c r="F17" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/18-Bartkus-Farm-Concord-MA-01742/306465917_zpid/</t>
         </is>
@@ -835,7 +1115,7 @@
           <t>930</t>
         </is>
       </c>
-      <c r="F18" t="inlineStr">
+      <c r="F18" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/17-Mello-St-East-Falmouth-MA-02536/55885097_zpid/</t>
         </is>
@@ -861,7 +1141,7 @@
           <t>1,691</t>
         </is>
       </c>
-      <c r="F19" t="inlineStr">
+      <c r="F19" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/198-W-River-St-Upton-MA-01568/173952657_zpid/</t>
         </is>
@@ -887,7 +1167,7 @@
           <t>1,564</t>
         </is>
       </c>
-      <c r="F20" t="inlineStr">
+      <c r="F20" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/298-Heaths-Bridge-Rd-Concord-MA-01742/166021031_zpid/</t>
         </is>
@@ -913,7 +1193,7 @@
           <t>1,226</t>
         </is>
       </c>
-      <c r="F21" t="inlineStr">
+      <c r="F21" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/66-Milk-St-Nantucket-MA-02554/56544257_zpid/</t>
         </is>
@@ -939,7 +1219,7 @@
           <t>1,987</t>
         </is>
       </c>
-      <c r="F22" t="inlineStr">
+      <c r="F22" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/116-Charlton-St-Oxford-MA-01540/60027614_zpid/</t>
         </is>
@@ -965,7 +1245,7 @@
           <t>2,367</t>
         </is>
       </c>
-      <c r="F23" t="inlineStr">
+      <c r="F23" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/262-Sheep-Pond-Dr-Brewster-MA-02631/56767509_zpid/</t>
         </is>
@@ -991,7 +1271,7 @@
           <t>740</t>
         </is>
       </c>
-      <c r="F24" t="inlineStr">
+      <c r="F24" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/67-Gorwin-Dr-Hanson-MA-02341/184281722_zpid/</t>
         </is>
@@ -1017,7 +1297,7 @@
           <t>1,712</t>
         </is>
       </c>
-      <c r="F25" t="inlineStr">
+      <c r="F25" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/9-Samuel-Parlin-Dr-Acton-MA-01720/57031578_zpid/</t>
         </is>
@@ -1043,7 +1323,7 @@
           <t>1,606</t>
         </is>
       </c>
-      <c r="F26" t="inlineStr">
+      <c r="F26" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/34-Hoover-Ave-Brockton-MA-02301/57161799_zpid/</t>
         </is>
@@ -1069,7 +1349,7 @@
           <t>1,670</t>
         </is>
       </c>
-      <c r="F27" t="inlineStr">
+      <c r="F27" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/1-Oakwood-Rd-Acton-MA-01720/57035146_zpid/</t>
         </is>
@@ -1095,7 +1375,7 @@
           <t>2,431</t>
         </is>
       </c>
-      <c r="F28" t="inlineStr">
+      <c r="F28" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/15-Foxglove-Ln-Amherst-MA-01002/56258397_zpid/</t>
         </is>
@@ -1121,7 +1401,7 @@
           <t>1,374</t>
         </is>
       </c>
-      <c r="F29" t="inlineStr">
+      <c r="F29" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/98-Heywood-Rd-Ashby-MA-01431/71129594_zpid/</t>
         </is>
@@ -1145,7 +1425,7 @@
       <c r="E30" s="4" t="n">
         <v>909</v>
       </c>
-      <c r="F30" t="inlineStr">
+      <c r="F30" s="0" t="inlineStr">
         <is>
           <t>None</t>
         </is>
@@ -1171,7 +1451,7 @@
           <t>1,501</t>
         </is>
       </c>
-      <c r="F31" t="inlineStr">
+      <c r="F31" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/154-Oakham-Rd-North-Brookfield-MA-01535/57620961_zpid/</t>
         </is>
@@ -1197,7 +1477,7 @@
           <t>1,733</t>
         </is>
       </c>
-      <c r="F32" t="inlineStr">
+      <c r="F32" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/58-River-Rd-Gill-MA-01354/56980125_zpid/</t>
         </is>
@@ -1223,7 +1503,7 @@
           <t>845</t>
         </is>
       </c>
-      <c r="F33" t="inlineStr">
+      <c r="F33" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/40-Glenmore-Ln-Bridgewater-MA-02324/57153009_zpid/</t>
         </is>
@@ -1249,7 +1529,7 @@
           <t>1,162</t>
         </is>
       </c>
-      <c r="F34" t="inlineStr">
+      <c r="F34" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/36-Green-Acres-Dr-Whitman-MA-02382/59192163_zpid/</t>
         </is>
@@ -1275,7 +1555,7 @@
           <t>1,289</t>
         </is>
       </c>
-      <c r="F35" t="inlineStr">
+      <c r="F35" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/83-Oxford-Rd-Westwood-MA-02090/57516186_zpid/</t>
         </is>
@@ -1301,7 +1581,7 @@
           <t>1,226</t>
         </is>
       </c>
-      <c r="F36" t="inlineStr">
+      <c r="F36" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/18-Proctor-Rd-Chelmsford-MA-01824/56451870_zpid/</t>
         </is>
@@ -1327,7 +1607,7 @@
           <t>3,001</t>
         </is>
       </c>
-      <c r="F37" t="inlineStr">
+      <c r="F37" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/409-Still-River-Rd-Bolton-MA-01740/57568730_zpid/</t>
         </is>
@@ -1353,7 +1633,7 @@
           <t>1,332</t>
         </is>
       </c>
-      <c r="F38" t="inlineStr">
+      <c r="F38" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/4-Nicholson-Hill-Rd-Southwick-MA-01077/56996681_zpid/</t>
         </is>
@@ -1379,7 +1659,7 @@
           <t>1,057</t>
         </is>
       </c>
-      <c r="F39" t="inlineStr">
+      <c r="F39" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/29-Harris-St-Amherst-MA-01002/56254557_zpid/</t>
         </is>
@@ -1405,7 +1685,7 @@
           <t>1,120</t>
         </is>
       </c>
-      <c r="F40" t="inlineStr">
+      <c r="F40" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/17-Tricia-Rd-North-Falmouth-MA-02556/55881948_zpid/</t>
         </is>
@@ -1431,7 +1711,7 @@
           <t>550</t>
         </is>
       </c>
-      <c r="F41" t="inlineStr">
+      <c r="F41" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/42-Ames-St-Medford-MA-02155/56273410_zpid/</t>
         </is>
@@ -1457,7 +1737,7 @@
           <t>1,987</t>
         </is>
       </c>
-      <c r="F42" t="inlineStr">
+      <c r="F42" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/152-Chipman-Rd-Chester-MA-01011/80383079_zpid/</t>
         </is>
@@ -1483,7 +1763,7 @@
           <t>550</t>
         </is>
       </c>
-      <c r="F43" t="inlineStr">
+      <c r="F43" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/18-Perkins-St-Arlington-MA-02476/56403369_zpid/</t>
         </is>
@@ -1509,7 +1789,7 @@
           <t>1,754</t>
         </is>
       </c>
-      <c r="F44" t="inlineStr">
+      <c r="F44" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/196-South-St-Berlin-MA-01503/57564080_zpid/</t>
         </is>
@@ -1535,7 +1815,7 @@
           <t>909</t>
         </is>
       </c>
-      <c r="F45" t="inlineStr">
+      <c r="F45" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/46-Park-Ave-Natick-MA-01760/56296372_zpid/</t>
         </is>
@@ -1561,7 +1841,7 @@
           <t>1,141</t>
         </is>
       </c>
-      <c r="F46" t="inlineStr">
+      <c r="F46" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/19-Susan-Dr-Dudley-MA-01571/61320453_zpid/</t>
         </is>
@@ -1587,7 +1867,7 @@
           <t>2,029</t>
         </is>
       </c>
-      <c r="F47" t="inlineStr">
+      <c r="F47" s="0" t="inlineStr">
         <is>
           <t>None</t>
         </is>
@@ -1613,7 +1893,7 @@
           <t>1,184</t>
         </is>
       </c>
-      <c r="F48" t="inlineStr">
+      <c r="F48" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/9-Playstead-Ln-East-Falmouth-MA-02536/55891667_zpid/</t>
         </is>
@@ -1639,7 +1919,7 @@
           <t>1,162</t>
         </is>
       </c>
-      <c r="F49" t="inlineStr">
+      <c r="F49" s="0" t="inlineStr">
         <is>
           <t>None</t>
         </is>
@@ -1665,7 +1945,7 @@
           <t>3,424</t>
         </is>
       </c>
-      <c r="F50" t="inlineStr">
+      <c r="F50" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/63-Minuteman-Dr-Concord-MA-01742/166022267_zpid/</t>
         </is>
@@ -1691,7 +1971,7 @@
           <t>1,141</t>
         </is>
       </c>
-      <c r="F51" t="inlineStr">
+      <c r="F51" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/30-Wigwam-St-Wellfleet-MA-02667/56794923_zpid/</t>
         </is>
@@ -1717,7 +1997,7 @@
           <t>1,226</t>
         </is>
       </c>
-      <c r="F52" t="inlineStr">
+      <c r="F52" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/21-Tersolo-Rd-Haverhill-MA-01832/56056744_zpid/</t>
         </is>
@@ -1743,7 +2023,7 @@
           <t>1,015</t>
         </is>
       </c>
-      <c r="F53" t="inlineStr">
+      <c r="F53" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/110-Oaklawn-Ave-Orange-MA-01364/56140342_zpid/</t>
         </is>
@@ -1769,7 +2049,7 @@
           <t>1,839</t>
         </is>
       </c>
-      <c r="F54" t="inlineStr">
+      <c r="F54" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/226-Paddocks-Path-Dennis-MA-02638/55877916_zpid/</t>
         </is>
@@ -1795,7 +2075,7 @@
           <t>423</t>
         </is>
       </c>
-      <c r="F55" t="inlineStr">
+      <c r="F55" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/32-Woodbury-St-Beverly-MA-01915/59226114_zpid/</t>
         </is>
@@ -1821,7 +2101,7 @@
           <t>1,733</t>
         </is>
       </c>
-      <c r="F56" t="inlineStr">
+      <c r="F56" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/27-Windy-Hill-Dr-Plymouth-MA-02360/57545685_zpid/</t>
         </is>
@@ -1847,7 +2127,7 @@
           <t>507</t>
         </is>
       </c>
-      <c r="F57" t="inlineStr">
+      <c r="F57" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/20-Munroe-St-Somerville-MA-02143/271378798_zpid/</t>
         </is>
@@ -1873,7 +2153,7 @@
           <t>1,627</t>
         </is>
       </c>
-      <c r="F58" t="inlineStr">
+      <c r="F58" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/5-Carrot-Hill-Rd-Falmouth-MA-02543/55898363_zpid/</t>
         </is>
@@ -1899,7 +2179,7 @@
           <t>2,600</t>
         </is>
       </c>
-      <c r="F59" t="inlineStr">
+      <c r="F59" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/110-Lookout-Rd-Yarmouth-Port-MA-02675/55938606_zpid/</t>
         </is>
@@ -1925,7 +2205,7 @@
           <t>3,234</t>
         </is>
       </c>
-      <c r="F60" t="inlineStr">
+      <c r="F60" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/35-Sands-Rd-Eastham-MA-02642/56781235_zpid/</t>
         </is>
@@ -1951,7 +2231,7 @@
           <t>1,754</t>
         </is>
       </c>
-      <c r="F61" t="inlineStr">
+      <c r="F61" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/35-Harborlight-Dr-Plymouth-MA-02360/57540785_zpid/</t>
         </is>
@@ -1977,7 +2257,7 @@
           <t>888</t>
         </is>
       </c>
-      <c r="F62" t="inlineStr">
+      <c r="F62" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/101-Milton-St-Northampton-MA-01062/57022922_zpid/</t>
         </is>
@@ -2003,7 +2283,7 @@
           <t>1,036</t>
         </is>
       </c>
-      <c r="F63" t="inlineStr">
+      <c r="F63" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/321-Pochassic-Rd-Westfield-MA-01085/193631018_zpid/</t>
         </is>
@@ -2029,7 +2309,7 @@
           <t>761</t>
         </is>
       </c>
-      <c r="F64" t="inlineStr">
+      <c r="F64" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/401-Queen-Anne-Rd-Harwich-MA-02645/186992422_zpid/</t>
         </is>
@@ -2055,7 +2335,7 @@
           <t>930</t>
         </is>
       </c>
-      <c r="F65" t="inlineStr">
+      <c r="F65" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/301-Islington-Rd-Newton-MA-02466/56309787_zpid/</t>
         </is>
@@ -2081,7 +2361,7 @@
           <t>1,649</t>
         </is>
       </c>
-      <c r="F66" t="inlineStr">
+      <c r="F66" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/100-Jeffrey-Rd-Springfield-MA-01119/56216024_zpid/</t>
         </is>
@@ -2107,7 +2387,7 @@
           <t>1,458</t>
         </is>
       </c>
-      <c r="F67" t="inlineStr">
+      <c r="F67" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/6-Pheasant-Ln-Topsfield-MA-01983/56969565_zpid/</t>
         </is>
@@ -2133,7 +2413,7 @@
           <t>993</t>
         </is>
       </c>
-      <c r="F68" t="inlineStr">
+      <c r="F68" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/21-Crescent-Rd-Needham-MA-02494/57477934_zpid/</t>
         </is>
@@ -2159,7 +2439,7 @@
           <t>845</t>
         </is>
       </c>
-      <c r="F69" t="inlineStr">
+      <c r="F69" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/250-Summer-St-Lee-MA-01238/56804136_zpid/</t>
         </is>
@@ -2185,7 +2465,7 @@
           <t>803</t>
         </is>
       </c>
-      <c r="F70" t="inlineStr">
+      <c r="F70" s="0" t="inlineStr">
         <is>
           <t>None</t>
         </is>
@@ -2211,7 +2491,7 @@
           <t>2,050</t>
         </is>
       </c>
-      <c r="F71" t="inlineStr">
+      <c r="F71" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/184-N-Leverett-Rd-Leverett-MA-01054/80863083_zpid/</t>
         </is>
@@ -2237,7 +2517,7 @@
           <t>1,268</t>
         </is>
       </c>
-      <c r="F72" t="inlineStr">
+      <c r="F72" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/18-Knollwood-Dr-Dartmouth-MA-02747/55966575_zpid/</t>
         </is>
@@ -2263,7 +2543,7 @@
           <t>1,606</t>
         </is>
       </c>
-      <c r="F73" t="inlineStr">
+      <c r="F73" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/45-Greenwood-Ave-Needham-MA-02492/57475272_zpid/</t>
         </is>
@@ -2289,7 +2569,7 @@
           <t>1,057</t>
         </is>
       </c>
-      <c r="F74" t="inlineStr">
+      <c r="F74" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/3-Bowers-Ave-Tyngsboro-MA-01879/57122674_zpid/</t>
         </is>
@@ -2315,7 +2595,7 @@
           <t>1,395</t>
         </is>
       </c>
-      <c r="F75" t="inlineStr">
+      <c r="F75" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/24-Green-Valley-Rd-Medway-MA-02053/57461159_zpid/</t>
         </is>
@@ -2341,7 +2621,7 @@
           <t>423</t>
         </is>
       </c>
-      <c r="F76" t="inlineStr">
+      <c r="F76" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/105-E-Gate-Rd-Brewster-MA-02631/186846759_zpid/</t>
         </is>
@@ -2367,7 +2647,7 @@
           <t>1,205</t>
         </is>
       </c>
-      <c r="F77" t="inlineStr">
+      <c r="F77" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/26-Walnut-Rd-South-Hamilton-MA-01982/56924745_zpid/</t>
         </is>
@@ -2393,7 +2673,7 @@
           <t>85</t>
         </is>
       </c>
-      <c r="F78" t="inlineStr">
+      <c r="F78" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/42-Lake-Ave-Framingham-MA-01702/165996355_zpid/</t>
         </is>
@@ -2419,7 +2699,7 @@
           <t>1,860</t>
         </is>
       </c>
-      <c r="F79" t="inlineStr">
+      <c r="F79" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/17-Fernwood-Dr-Hampden-MA-01036/56173594_zpid/</t>
         </is>
@@ -2445,7 +2725,7 @@
           <t>1,247</t>
         </is>
       </c>
-      <c r="F80" t="inlineStr">
+      <c r="F80" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/342-Belknap-Rd-Framingham-MA-01701/165986610_zpid/</t>
         </is>
@@ -2471,7 +2751,7 @@
           <t>10,969</t>
         </is>
       </c>
-      <c r="F81" t="inlineStr">
+      <c r="F81" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/435-Martins-Pond-Rd-Groton-MA-01450/57066211_zpid/</t>
         </is>
@@ -2497,7 +2777,7 @@
           <t>1,522</t>
         </is>
       </c>
-      <c r="F82" t="inlineStr">
+      <c r="F82" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/103-Farm-St-Bellingham-MA-02019/123883120_zpid/</t>
         </is>
@@ -2523,7 +2803,7 @@
           <t>1,839</t>
         </is>
       </c>
-      <c r="F83" t="inlineStr">
+      <c r="F83" s="0" t="inlineStr">
         <is>
           <t>None</t>
         </is>
@@ -2549,7 +2829,7 @@
           <t>867</t>
         </is>
       </c>
-      <c r="F84" t="inlineStr">
+      <c r="F84" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/4-Vineyard-Ave-Clinton-MA-01510/57577271_zpid/</t>
         </is>
@@ -2575,7 +2855,7 @@
           <t>1,310</t>
         </is>
       </c>
-      <c r="F85" t="inlineStr">
+      <c r="F85" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/335-Grand-Ave-Falmouth-MA-02540/55896521_zpid/</t>
         </is>
@@ -2601,7 +2881,7 @@
           <t>1,691</t>
         </is>
       </c>
-      <c r="F86" t="inlineStr">
+      <c r="F86" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/55-Orchard-Hill-Dr-Plymouth-MA-02360/123191116_zpid/</t>
         </is>
@@ -2627,7 +2907,7 @@
           <t>613</t>
         </is>
       </c>
-      <c r="F87" t="inlineStr">
+      <c r="F87" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/9-Theresa-Ave-Burlington-MA-01803/57055850_zpid/</t>
         </is>
@@ -2653,7 +2933,7 @@
           <t>1,268</t>
         </is>
       </c>
-      <c r="F88" t="inlineStr">
+      <c r="F88" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/32-Pearl-Brook-Rd-Lunenburg-MA-01462/57611448_zpid/</t>
         </is>
@@ -2679,7 +2959,7 @@
           <t>571</t>
         </is>
       </c>
-      <c r="F89" t="inlineStr">
+      <c r="F89" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/23-Whittemore-St-Arlington-MA-02474/56393572_zpid/</t>
         </is>
@@ -2705,7 +2985,7 @@
           <t>2,092</t>
         </is>
       </c>
-      <c r="F90" t="inlineStr">
+      <c r="F90" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/38-Southwick-Rd-Sutton-MA-01590/57655803_zpid/</t>
         </is>
@@ -2731,7 +3011,7 @@
           <t>1,205</t>
         </is>
       </c>
-      <c r="F91" t="inlineStr">
+      <c r="F91" s="0" t="inlineStr">
         <is>
           <t>None</t>
         </is>
@@ -2757,7 +3037,7 @@
           <t>761</t>
         </is>
       </c>
-      <c r="F92" t="inlineStr">
+      <c r="F92" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/100-W-Chestnut-Hill-Rd-Montague-MA-01351/56984464_zpid/</t>
         </is>
@@ -2783,7 +3063,7 @@
           <t>972</t>
         </is>
       </c>
-      <c r="F93" t="inlineStr">
+      <c r="F93" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/5-Chestnut-Hill-Rd-Warwick-MA-01378/56987857_zpid/</t>
         </is>
@@ -2809,7 +3089,7 @@
           <t>613</t>
         </is>
       </c>
-      <c r="F94" t="inlineStr">
+      <c r="F94" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/100-Montclair-Ave-Waltham-MA-02451/56358859_zpid/</t>
         </is>
@@ -2835,7 +3115,7 @@
           <t>5,707</t>
         </is>
       </c>
-      <c r="F95" t="inlineStr">
+      <c r="F95" s="0" t="inlineStr">
         <is>
           <t>None</t>
         </is>
@@ -2861,7 +3141,7 @@
           <t>1,226</t>
         </is>
       </c>
-      <c r="F96" t="inlineStr">
+      <c r="F96" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/114-Pine-St-Northampton-MA-01062/57021156_zpid/</t>
         </is>
@@ -2887,7 +3167,7 @@
           <t>740</t>
         </is>
       </c>
-      <c r="F97" t="inlineStr">
+      <c r="F97" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/27-Hammond-Rd-Hopedale-MA-01747/57602678_zpid/</t>
         </is>
@@ -2913,7 +3193,7 @@
           <t>951</t>
         </is>
       </c>
-      <c r="F98" t="inlineStr">
+      <c r="F98" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/38-Blackberry-Ln-Brewster-MA-02631/56769623_zpid/</t>
         </is>
@@ -2939,7 +3219,7 @@
           <t>2,219</t>
         </is>
       </c>
-      <c r="F99" t="inlineStr">
+      <c r="F99" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/50-Deerpath-Rd-Dedham-MA-02026/61317928_zpid/</t>
         </is>
@@ -2965,7 +3245,7 @@
           <t>1,649</t>
         </is>
       </c>
-      <c r="F100" t="inlineStr">
+      <c r="F100" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/239-Otis-Stage-Rd-Blandford-MA-01008/56989402_zpid/</t>
         </is>
@@ -2991,7 +3271,7 @@
           <t>1,120</t>
         </is>
       </c>
-      <c r="F101" t="inlineStr">
+      <c r="F101" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/11-Woodland-Dr-Westminster-MA-01473/57681661_zpid/</t>
         </is>
@@ -3017,7 +3297,7 @@
           <t>1,501</t>
         </is>
       </c>
-      <c r="F102" t="inlineStr">
+      <c r="F102" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/4-Barilone-Cir-Maynard-MA-01754/57089849_zpid/</t>
         </is>
@@ -3043,7 +3323,7 @@
           <t>1,141</t>
         </is>
       </c>
-      <c r="F103" t="inlineStr">
+      <c r="F103" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/1-Jackson-Ct-Natick-MA-01760/56296174_zpid/</t>
         </is>
@@ -3069,7 +3349,7 @@
           <t>1,395</t>
         </is>
       </c>
-      <c r="F104" t="inlineStr">
+      <c r="F104" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/128-Bridge-St-Manchester-MA-01944/56934086_zpid/</t>
         </is>
@@ -3095,7 +3375,7 @@
           <t>1,310</t>
         </is>
       </c>
-      <c r="F105" t="inlineStr">
+      <c r="F105" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/458-East-St-Easthampton-MA-01027/57009565_zpid/</t>
         </is>
@@ -3121,7 +3401,7 @@
           <t>1,627</t>
         </is>
       </c>
-      <c r="F106" t="inlineStr">
+      <c r="F106" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/23-Orchard-St-Northampton-MA-01060/87798678_zpid/</t>
         </is>
@@ -3147,7 +3427,7 @@
           <t>888</t>
         </is>
       </c>
-      <c r="F107" t="inlineStr">
+      <c r="F107" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/770-Waltham-St-Lexington-MA-02421/56488902_zpid/</t>
         </is>
@@ -3173,7 +3453,7 @@
           <t>1,226</t>
         </is>
       </c>
-      <c r="F108" t="inlineStr">
+      <c r="F108" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/100-Moser-St-Northampton-MA-01060/121252390_zpid/</t>
         </is>
@@ -3199,7 +3479,7 @@
           <t>1,374</t>
         </is>
       </c>
-      <c r="F109" t="inlineStr">
+      <c r="F109" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/82-Rocky-Neck-Ave-A-Gloucester-MA-01930/2111229081_zpid/</t>
         </is>
@@ -3225,7 +3505,7 @@
           <t>1,057</t>
         </is>
       </c>
-      <c r="F110" t="inlineStr">
+      <c r="F110" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/48-Gannett-Pasture-Ln-Scituate-MA-02066/57222367_zpid/</t>
         </is>
@@ -3251,7 +3531,7 @@
           <t>803</t>
         </is>
       </c>
-      <c r="F111" t="inlineStr">
+      <c r="F111" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/183-Lincoln-Rd-Medford-MA-02155/56275377_zpid/</t>
         </is>
@@ -3277,7 +3557,7 @@
           <t>888</t>
         </is>
       </c>
-      <c r="F112" t="inlineStr">
+      <c r="F112" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/15-Milne-Rd-Osterville-MA-02655/55853966_zpid/</t>
         </is>
@@ -3303,7 +3583,7 @@
           <t>1,289</t>
         </is>
       </c>
-      <c r="F113" t="inlineStr">
+      <c r="F113" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/4-Pershing-Rd-Needham-MA-02494/57479045_zpid/</t>
         </is>
@@ -3329,7 +3609,7 @@
           <t>1,860</t>
         </is>
       </c>
-      <c r="F114" t="inlineStr">
+      <c r="F114" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/55-Sheffield-Ln-Northampton-MA-01062/57020171_zpid/</t>
         </is>
@@ -3355,7 +3635,7 @@
           <t>1,522</t>
         </is>
       </c>
-      <c r="F115" t="inlineStr">
+      <c r="F115" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/51-53-Oakland-St-Melrose-MA-02176/165805876_zpid/</t>
         </is>
@@ -3381,7 +3661,7 @@
           <t>2,177</t>
         </is>
       </c>
-      <c r="F116" t="inlineStr">
+      <c r="F116" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/42-Wianno-Rd-Bourne-MA-02532/186977019_zpid/</t>
         </is>
@@ -3407,7 +3687,7 @@
           <t>1,162</t>
         </is>
       </c>
-      <c r="F117" t="inlineStr">
+      <c r="F117" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/16-Common-St-Brookfield-MA-01506/57571006_zpid/</t>
         </is>
@@ -3433,7 +3713,7 @@
           <t>2,283</t>
         </is>
       </c>
-      <c r="F118" t="inlineStr">
+      <c r="F118" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/235-Bay-Rd-Harwich-MA-02645/186996433_zpid/</t>
         </is>
@@ -3459,7 +3739,7 @@
           <t>550</t>
         </is>
       </c>
-      <c r="F119" t="inlineStr">
+      <c r="F119" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/183-Buckwood-Dr-Hyannis-MA-02601/55846204_zpid/</t>
         </is>
@@ -3485,7 +3765,7 @@
           <t>1,860</t>
         </is>
       </c>
-      <c r="F120" t="inlineStr">
+      <c r="F120" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/35-Woodbury-St-Beverly-MA-01915/59225949_zpid/</t>
         </is>
@@ -3511,7 +3791,7 @@
           <t>697</t>
         </is>
       </c>
-      <c r="F121" t="inlineStr">
+      <c r="F121" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/36-Hill-St-Haverhill-MA-01832/56054458_zpid/</t>
         </is>
@@ -3537,7 +3817,7 @@
           <t>(Data Not Found)</t>
         </is>
       </c>
-      <c r="F122" t="inlineStr">
+      <c r="F122" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/27-Hawthorne-Ave-Arlington-MA-02476/56403359_zpid/</t>
         </is>
@@ -3563,7 +3843,7 @@
           <t>1,184</t>
         </is>
       </c>
-      <c r="F123" t="inlineStr">
+      <c r="F123" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/98-Prescott-Rd-Concord-MA-01742/166022245_zpid/</t>
         </is>
@@ -3589,7 +3869,7 @@
           <t>1,416</t>
         </is>
       </c>
-      <c r="F124" t="inlineStr">
+      <c r="F124" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/2-Candida-Ln-Acton-MA-01720/57035751_zpid/</t>
         </is>
@@ -3615,7 +3895,7 @@
           <t>1,120</t>
         </is>
       </c>
-      <c r="F125" t="inlineStr">
+      <c r="F125" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/11-Mary-Chilton-Rd-Needham-MA-02492/57480236_zpid/</t>
         </is>
@@ -3641,7 +3921,7 @@
           <t>1,543</t>
         </is>
       </c>
-      <c r="F126" t="inlineStr">
+      <c r="F126" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/42-Birchtree-Dr-Westwood-MA-02090/57516342_zpid/</t>
         </is>
@@ -3667,7 +3947,7 @@
           <t>1,522</t>
         </is>
       </c>
-      <c r="F127" t="inlineStr">
+      <c r="F127" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/279-Davis-St-Northborough-MA-01532/57625738_zpid/</t>
         </is>
@@ -3693,7 +3973,7 @@
           <t>1,247</t>
         </is>
       </c>
-      <c r="F128" t="inlineStr">
+      <c r="F128" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/32-Oak-Knoll-Dr-Hampden-MA-01036/56173214_zpid/</t>
         </is>
@@ -3719,7 +3999,7 @@
           <t>1,733</t>
         </is>
       </c>
-      <c r="F129" t="inlineStr">
+      <c r="F129" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/49-Ford-Xing-Northampton-MA-01060/246300174_zpid/</t>
         </is>
@@ -3745,7 +4025,7 @@
           <t>1,078</t>
         </is>
       </c>
-      <c r="F130" t="inlineStr">
+      <c r="F130" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/15-Grandview-Rd-Haverhill-MA-01832/56054467_zpid/</t>
         </is>
@@ -3771,7 +4051,7 @@
           <t>2,177</t>
         </is>
       </c>
-      <c r="F131" t="inlineStr">
+      <c r="F131" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/143-Holden-Wood-Rd-Concord-MA-01742/166020986_zpid/</t>
         </is>
@@ -3797,7 +4077,7 @@
           <t>1,670</t>
         </is>
       </c>
-      <c r="F132" t="inlineStr">
+      <c r="F132" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/117-Park-Rd-Chelmsford-MA-01824/56452429_zpid/</t>
         </is>
@@ -3823,7 +4103,7 @@
           <t>1,522</t>
         </is>
       </c>
-      <c r="F133" t="inlineStr">
+      <c r="F133" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/177-Monsen-Rd-Concord-MA-01742/166021937_zpid/</t>
         </is>
@@ -3849,7 +4129,7 @@
           <t>4,650</t>
         </is>
       </c>
-      <c r="F134" t="inlineStr">
+      <c r="F134" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/6-Sutton-Pl-Acton-MA-01720/57031615_zpid/</t>
         </is>
@@ -3875,7 +4155,7 @@
           <t>486</t>
         </is>
       </c>
-      <c r="F135" t="inlineStr">
+      <c r="F135" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/286-College-Farm-Rd-Waltham-MA-02451/56358789_zpid/</t>
         </is>
@@ -3901,7 +4181,7 @@
           <t>719</t>
         </is>
       </c>
-      <c r="F136" t="inlineStr">
+      <c r="F136" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/1-Wade-Rd-Plainville-MA-02762/57492677_zpid/</t>
         </is>
@@ -3927,7 +4207,7 @@
           <t>930</t>
         </is>
       </c>
-      <c r="F137" t="inlineStr">
+      <c r="F137" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/34-Shannon-Way-Dartmouth-MA-02747/59880382_zpid/</t>
         </is>
@@ -3953,7 +4233,7 @@
           <t>2,177</t>
         </is>
       </c>
-      <c r="F138" t="inlineStr">
+      <c r="F138" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/13-Secluded-Rdg-Southwick-MA-01077/56996781_zpid/</t>
         </is>
@@ -3979,7 +4259,7 @@
           <t>613</t>
         </is>
       </c>
-      <c r="F139" t="inlineStr">
+      <c r="F139" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/23-Powell-St-Northampton-MA-01062/57020013_zpid/</t>
         </is>
@@ -4005,7 +4285,7 @@
           <t>296</t>
         </is>
       </c>
-      <c r="F140" t="inlineStr">
+      <c r="F140" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/4-Sheeps-Crossing-Ln-Falmouth-MA-02543/55898730_zpid/</t>
         </is>
@@ -4031,7 +4311,7 @@
           <t>2,092</t>
         </is>
       </c>
-      <c r="F141" t="inlineStr">
+      <c r="F141" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/7-Pheasant-Ln-Topsfield-MA-01983/56969630_zpid/</t>
         </is>
@@ -4057,7 +4337,7 @@
           <t>2,431</t>
         </is>
       </c>
-      <c r="F142" t="inlineStr">
+      <c r="F142" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/336-Station-Rd-Amherst-MA-01002/56258370_zpid/</t>
         </is>
@@ -4083,7 +4363,7 @@
           <t>592</t>
         </is>
       </c>
-      <c r="F143" t="inlineStr">
+      <c r="F143" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/14-Mount-Walley-Rd-Waltham-MA-02451/56359215_zpid/</t>
         </is>
@@ -4109,7 +4389,7 @@
           <t>1,437</t>
         </is>
       </c>
-      <c r="F144" t="inlineStr">
+      <c r="F144" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/10-Aloha-Dr-Hadley-MA-01035/57015527_zpid/</t>
         </is>
@@ -4135,7 +4415,7 @@
           <t>571</t>
         </is>
       </c>
-      <c r="F145" t="inlineStr">
+      <c r="F145" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/18-Mount-Ida-Ter-Waltham-MA-02451/56359233_zpid/</t>
         </is>
@@ -4161,7 +4441,7 @@
           <t>909</t>
         </is>
       </c>
-      <c r="F146" t="inlineStr">
+      <c r="F146" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/7-Oak-Ridge-Rd-East-Falmouth-MA-02536/55891673_zpid/</t>
         </is>
@@ -4187,7 +4467,7 @@
           <t>528</t>
         </is>
       </c>
-      <c r="F147" t="inlineStr">
+      <c r="F147" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/175-Shepardson-Rd-Warwick-MA-01378/56987841_zpid/</t>
         </is>
@@ -4213,7 +4493,7 @@
           <t>824</t>
         </is>
       </c>
-      <c r="F148" t="inlineStr">
+      <c r="F148" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/33-Hill-St-Haverhill-MA-01832/56054482_zpid/</t>
         </is>
@@ -4239,7 +4519,7 @@
           <t>845</t>
         </is>
       </c>
-      <c r="F149" t="inlineStr">
+      <c r="F149" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/6-Pine-Ave-Tyngsboro-MA-01879/57122748_zpid/</t>
         </is>
@@ -4265,7 +4545,7 @@
           <t>845</t>
         </is>
       </c>
-      <c r="F150" t="inlineStr">
+      <c r="F150" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/12-Barbara-Cir-Burlington-MA-01803/57056333_zpid/</t>
         </is>
@@ -4291,7 +4571,7 @@
           <t>634</t>
         </is>
       </c>
-      <c r="F151" t="inlineStr">
+      <c r="F151" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/52-Stickney-Rd-Medford-MA-02155/56275415_zpid/</t>
         </is>
@@ -4317,7 +4597,7 @@
           <t>1,226</t>
         </is>
       </c>
-      <c r="F152" t="inlineStr">
+      <c r="F152" s="0" t="inlineStr">
         <is>
           <t>None</t>
         </is>
@@ -4343,7 +4623,7 @@
           <t>465</t>
         </is>
       </c>
-      <c r="F153" t="inlineStr">
+      <c r="F153" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/37-Andrews-St-Medford-MA-02155/56273730_zpid/</t>
         </is>
@@ -4369,7 +4649,7 @@
           <t>528</t>
         </is>
       </c>
-      <c r="F154" t="inlineStr">
+      <c r="F154" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/49-Braemore-Rd-Waltham-MA-02451/56358904_zpid/</t>
         </is>
@@ -4395,7 +4675,7 @@
           <t>1,015</t>
         </is>
       </c>
-      <c r="F155" t="inlineStr">
+      <c r="F155" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/1-Stockdale-Rd-Needham-MA-02492/57478584_zpid/</t>
         </is>
@@ -4421,7 +4701,7 @@
           <t>1,141</t>
         </is>
       </c>
-      <c r="F156" t="inlineStr">
+      <c r="F156" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/67-Greenwood-Ave-Needham-MA-02492/57475276_zpid/</t>
         </is>
@@ -4447,7 +4727,7 @@
           <t>1,754</t>
         </is>
       </c>
-      <c r="F157" t="inlineStr">
+      <c r="F157" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/34-Seltsam-Way-Pembroke-MA-02359/121878579_zpid/</t>
         </is>
@@ -4473,7 +4753,7 @@
           <t>1,966</t>
         </is>
       </c>
-      <c r="F158" t="inlineStr">
+      <c r="F158" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/260-Vaughn-Hill-Rd-Bolton-MA-01740/57568665_zpid/</t>
         </is>
@@ -4499,7 +4779,7 @@
           <t>2,642</t>
         </is>
       </c>
-      <c r="F159" t="inlineStr">
+      <c r="F159" s="0" t="inlineStr">
         <is>
           <t>None</t>
         </is>
@@ -4525,7 +4805,7 @@
           <t>867</t>
         </is>
       </c>
-      <c r="F160" t="inlineStr">
+      <c r="F160" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/76-Woodlot-Rd-Amherst-MA-01002/56258359_zpid/</t>
         </is>
@@ -4551,7 +4831,7 @@
           <t>2,240</t>
         </is>
       </c>
-      <c r="F161" t="inlineStr">
+      <c r="F161" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/26-Foxglove-Ln-Amherst-MA-01002/56258411_zpid/</t>
         </is>
@@ -4577,7 +4857,7 @@
           <t>2,705</t>
         </is>
       </c>
-      <c r="F162" t="inlineStr">
+      <c r="F162" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/12-Bayberry-Ln-Hadley-MA-01035/67714823_zpid/</t>
         </is>
@@ -4603,7 +4883,7 @@
           <t>1,141</t>
         </is>
       </c>
-      <c r="F163" t="inlineStr">
+      <c r="F163" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/124-Moser-St-Northampton-MA-01060/121251942_zpid/</t>
         </is>
@@ -4629,7 +4909,7 @@
           <t>1,754</t>
         </is>
       </c>
-      <c r="F164" t="inlineStr">
+      <c r="F164" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/442-East-St-Easthampton-MA-01027/59881486_zpid/</t>
         </is>
@@ -4655,7 +4935,7 @@
           <t>1,416</t>
         </is>
       </c>
-      <c r="F165" t="inlineStr">
+      <c r="F165" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/5-Bean-Porridge-Hill-Rd-Westminster-MA-01473/57681454_zpid/</t>
         </is>
@@ -4681,7 +4961,7 @@
           <t>803</t>
         </is>
       </c>
-      <c r="F166" t="inlineStr">
+      <c r="F166" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/68-McGee-Dr-Hyannis-MA-02601/55846054_zpid/</t>
         </is>
@@ -4707,7 +4987,7 @@
           <t>1,141</t>
         </is>
       </c>
-      <c r="F167" t="inlineStr">
+      <c r="F167" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/118-Wild-Harbor-Rd-North-Falmouth-MA-02556/55881954_zpid/</t>
         </is>
@@ -4733,7 +5013,7 @@
           <t>1,289</t>
         </is>
       </c>
-      <c r="F168" t="inlineStr">
+      <c r="F168" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/46-Scotland-Heights-Rd-Haverhill-MA-01832/56056737_zpid/</t>
         </is>
@@ -4759,7 +5039,7 @@
           <t>1,416</t>
         </is>
       </c>
-      <c r="F169" t="inlineStr">
+      <c r="F169" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/13-Kenwood-St-Chelmsford-MA-01824/56451880_zpid/</t>
         </is>
@@ -4785,7 +5065,7 @@
           <t>1,437</t>
         </is>
       </c>
-      <c r="F170" t="inlineStr">
+      <c r="F170" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/22-Orchard-Ln-Groton-MA-01450/61315789_zpid/</t>
         </is>
@@ -4811,7 +5091,7 @@
           <t>613</t>
         </is>
       </c>
-      <c r="F171" t="inlineStr">
+      <c r="F171" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/84-Ramshead-Rd-Medford-MA-02155/56275351_zpid/</t>
         </is>
@@ -4837,7 +5117,7 @@
           <t>444</t>
         </is>
       </c>
-      <c r="F172" t="inlineStr">
+      <c r="F172" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/25-Stockdale-Rd-Needham-MA-02492/57478581_zpid/</t>
         </is>
@@ -4863,7 +5143,7 @@
           <t>486</t>
         </is>
       </c>
-      <c r="F173" t="inlineStr">
+      <c r="F173" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/34-Rawson-Rd-Bellingham-MA-02019/57424042_zpid/</t>
         </is>
@@ -4889,7 +5169,7 @@
           <t>2,071</t>
         </is>
       </c>
-      <c r="F174" t="inlineStr">
+      <c r="F174" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/155-Raymond-Dr-Hampden-MA-01036/56173315_zpid/</t>
         </is>
@@ -4915,7 +5195,7 @@
           <t>2,240</t>
         </is>
       </c>
-      <c r="F175" t="inlineStr">
+      <c r="F175" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/37-Harris-St-Amherst-MA-01002/56254550_zpid/</t>
         </is>
@@ -4941,7 +5221,7 @@
           <t>1,818</t>
         </is>
       </c>
-      <c r="F176" t="inlineStr">
+      <c r="F176" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/19-Foxglove-Ln-Amherst-MA-01002/56258404_zpid/</t>
         </is>
@@ -4967,7 +5247,7 @@
           <t>550</t>
         </is>
       </c>
-      <c r="F177" t="inlineStr">
+      <c r="F177" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/10-Frost-Ln-Hadley-MA-01035/57015383_zpid/</t>
         </is>
@@ -4993,7 +5273,7 @@
           <t>1,099</t>
         </is>
       </c>
-      <c r="F178" t="inlineStr">
+      <c r="F178" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/104-Wildflower-Dr-Amherst-MA-01002/56258337_zpid/</t>
         </is>
@@ -5019,7 +5299,7 @@
           <t>2,050</t>
         </is>
       </c>
-      <c r="F179" t="inlineStr">
+      <c r="F179" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/152-Birchtree-Dr-Westwood-MA-02090/57515978_zpid/</t>
         </is>
@@ -5045,7 +5325,7 @@
           <t>317</t>
         </is>
       </c>
-      <c r="F180" t="inlineStr">
+      <c r="F180" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/21-Blaisdell-Rd-Medford-MA-02155/56275330_zpid/</t>
         </is>
@@ -5071,7 +5351,7 @@
           <t>655</t>
         </is>
       </c>
-      <c r="F181" t="inlineStr">
+      <c r="F181" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/28-Longview-Rd-North-Falmouth-MA-02556/55883394_zpid/</t>
         </is>
@@ -5097,7 +5377,7 @@
           <t>1,310</t>
         </is>
       </c>
-      <c r="F182" t="inlineStr">
+      <c r="F182" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/25-Kaileys-Way-Groton-MA-01450/57066228_zpid/</t>
         </is>
@@ -5123,7 +5403,7 @@
           <t>1,099</t>
         </is>
       </c>
-      <c r="F183" t="inlineStr">
+      <c r="F183" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/55-Cedar-Hill-Rd-Bellingham-MA-02019/57423546_zpid/</t>
         </is>
@@ -5149,7 +5429,7 @@
           <t>1,015</t>
         </is>
       </c>
-      <c r="F184" t="inlineStr">
+      <c r="F184" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/10-Hillview-Ln-Plymouth-MA-02360/71374281_zpid/</t>
         </is>
@@ -5175,7 +5455,7 @@
           <t>1,310</t>
         </is>
       </c>
-      <c r="F185" t="inlineStr">
+      <c r="F185" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/15-Hope-St-Hopedale-MA-01747/57603536_zpid/</t>
         </is>
@@ -5201,7 +5481,7 @@
           <t>1,923</t>
         </is>
       </c>
-      <c r="F186" t="inlineStr">
+      <c r="F186" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/7-Kennedy-Dr-Hadley-MA-01035/57015490_zpid/</t>
         </is>
@@ -5227,7 +5507,7 @@
           <t>1,966</t>
         </is>
       </c>
-      <c r="F187" t="inlineStr">
+      <c r="F187" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/2-Bayberry-Ln-Hadley-MA-01035/61806217_zpid/</t>
         </is>
@@ -5253,7 +5533,7 @@
           <t>1,226</t>
         </is>
       </c>
-      <c r="F188" t="inlineStr">
+      <c r="F188" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/130-Hillcrest-Dr-Northampton-MA-01062/57020096_zpid/</t>
         </is>
@@ -5279,7 +5559,7 @@
           <t>2,536</t>
         </is>
       </c>
-      <c r="F189" t="inlineStr">
+      <c r="F189" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/4-Moser-St-Northampton-MA-01060/102990282_zpid/</t>
         </is>
@@ -5305,7 +5585,7 @@
           <t>1,902</t>
         </is>
       </c>
-      <c r="F190" t="inlineStr">
+      <c r="F190" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/5-Elm-Top-Ln-Beverly-MA-01915/59225870_zpid/</t>
         </is>
@@ -5331,7 +5611,7 @@
           <t>888</t>
         </is>
       </c>
-      <c r="F191" t="inlineStr">
+      <c r="F191" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/89-Park-Rd-Chelmsford-MA-01824/56451860_zpid/</t>
         </is>
@@ -5357,7 +5637,7 @@
           <t>1,522</t>
         </is>
       </c>
-      <c r="F192" t="inlineStr">
+      <c r="F192" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/4-Grasshopper-Ln-Oxford-MA-01540/60027617_zpid/</t>
         </is>
@@ -5383,7 +5663,7 @@
           <t>1,184</t>
         </is>
       </c>
-      <c r="F193" t="inlineStr">
+      <c r="F193" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/17-Bakers-Dr-Harwich-MA-02645/55904878_zpid/</t>
         </is>
@@ -5409,7 +5689,7 @@
           <t>254</t>
         </is>
       </c>
-      <c r="F194" t="inlineStr">
+      <c r="F194" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/49-Bakers-Dr-Harwich-MA-02645/186993268_zpid/</t>
         </is>
@@ -5435,7 +5715,7 @@
           <t>909</t>
         </is>
       </c>
-      <c r="F195" t="inlineStr">
+      <c r="F195" s="0" t="inlineStr">
         <is>
           <t>None</t>
         </is>
@@ -5461,7 +5741,7 @@
           <t>1,818</t>
         </is>
       </c>
-      <c r="F196" t="inlineStr">
+      <c r="F196" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/1123-Monument-St-Concord-MA-01742/166021646_zpid/</t>
         </is>
@@ -5487,7 +5767,7 @@
           <t>1,437</t>
         </is>
       </c>
-      <c r="F197" t="inlineStr">
+      <c r="F197" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/58-Farmers-Cliff-Rd-Concord-MA-01742/166021917_zpid/</t>
         </is>
@@ -5513,7 +5793,7 @@
           <t>972</t>
         </is>
       </c>
-      <c r="F198" t="inlineStr">
+      <c r="F198" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/3-Barilone-Cir-Maynard-MA-01754/57089854_zpid/</t>
         </is>
@@ -5539,7 +5819,7 @@
           <t>1,543</t>
         </is>
       </c>
-      <c r="F199" t="inlineStr">
+      <c r="F199" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/16-Ash-Ln-Dudley-MA-01571/59207910_zpid/</t>
         </is>
@@ -5565,7 +5845,7 @@
           <t>2,367</t>
         </is>
       </c>
-      <c r="F200" t="inlineStr">
+      <c r="F200" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/225-Nonotuck-St-B-Northampton-MA-01062/92203160_zpid/</t>
         </is>
@@ -5591,7 +5871,7 @@
           <t>1,247</t>
         </is>
       </c>
-      <c r="F201" t="inlineStr">
+      <c r="F201" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/1-Honey-Hill-Rd-Cummington-MA-01026/57006376_zpid/</t>
         </is>
@@ -5617,7 +5897,7 @@
           <t>1,691</t>
         </is>
       </c>
-      <c r="F202" t="inlineStr">
+      <c r="F202" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/208-Trouble-St-Cummington-MA-01026/57006372_zpid/</t>
         </is>
@@ -5643,7 +5923,7 @@
           <t>845</t>
         </is>
       </c>
-      <c r="F203" t="inlineStr">
+      <c r="F203" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/80-Wigwam-St-Wellfleet-MA-02667/56794929_zpid/</t>
         </is>
@@ -5669,7 +5949,7 @@
           <t>2,536</t>
         </is>
       </c>
-      <c r="F204" t="inlineStr">
+      <c r="F204" s="0" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/100-Waterfield-Rd-Osterville-MA-02655/55854086_zpid/</t>
         </is>

</xml_diff>

<commit_message>
second set of zillow data, small changes to zillow data collection logic
</commit_message>
<xml_diff>
--- a/res-econ_RA_data.xlsx
+++ b/res-econ_RA_data.xlsx
@@ -3530,6 +3530,44 @@
           <t>https://www.zillow.com/homedetails/9-Playstead-Ln-East-Falmouth-MA-02536/55891667_zpid/</t>
         </is>
       </c>
+      <c r="G48" t="n">
+        <v>663000</v>
+      </c>
+      <c r="H48" t="n">
+        <v>513800</v>
+      </c>
+      <c r="I48" t="n">
+        <v>2024</v>
+      </c>
+      <c r="J48" t="inlineStr">
+        <is>
+          <t>1994-03-30</t>
+        </is>
+      </c>
+      <c r="K48" t="n">
+        <v>1154</v>
+      </c>
+      <c r="L48" t="n">
+        <v>1992</v>
+      </c>
+      <c r="M48" t="n">
+        <v>0.3199954086317723</v>
+      </c>
+      <c r="N48" t="inlineStr">
+        <is>
+          <t>Acres</t>
+        </is>
+      </c>
+      <c r="O48" t="inlineStr">
+        <is>
+          <t>Other,Gas</t>
+        </is>
+      </c>
+      <c r="P48" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
     </row>
     <row r="49" ht="15.75" customHeight="1" s="19">
       <c r="A49" s="3" t="inlineStr">
@@ -3556,6 +3594,44 @@
           <t>https://www.zillow.com/homedetails/34-Stedman-St-Chelmsford-MA-01824/56446774_zpid/</t>
         </is>
       </c>
+      <c r="G49" t="n">
+        <v>695000</v>
+      </c>
+      <c r="H49" t="n">
+        <v>560500</v>
+      </c>
+      <c r="I49" t="n">
+        <v>2024</v>
+      </c>
+      <c r="J49" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="K49" t="n">
+        <v>2434</v>
+      </c>
+      <c r="L49" t="n">
+        <v>1895</v>
+      </c>
+      <c r="M49" t="n">
+        <v>0.3899908172635445</v>
+      </c>
+      <c r="N49" t="inlineStr">
+        <is>
+          <t>Acres</t>
+        </is>
+      </c>
+      <c r="O49" t="inlineStr">
+        <is>
+          <t>Other,Oil</t>
+        </is>
+      </c>
+      <c r="P49" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
       <c r="Q49" t="inlineStr">
         <is>
           <t>Zillow URL manually gathered for "Stedman Street" intead of "Steadman Street"</t>
@@ -3587,6 +3663,44 @@
           <t>https://www.zillow.com/homedetails/63-Minuteman-Dr-Concord-MA-01742/166022267_zpid/</t>
         </is>
       </c>
+      <c r="G50" t="n">
+        <v>1520600</v>
+      </c>
+      <c r="H50" t="n">
+        <v>1268600</v>
+      </c>
+      <c r="I50" t="n">
+        <v>2024</v>
+      </c>
+      <c r="J50" t="inlineStr">
+        <is>
+          <t>1989-08-04</t>
+        </is>
+      </c>
+      <c r="K50" t="n">
+        <v>3350</v>
+      </c>
+      <c r="L50" t="n">
+        <v>2004</v>
+      </c>
+      <c r="M50" t="n">
+        <v>0.4699954086317722</v>
+      </c>
+      <c r="N50" t="inlineStr">
+        <is>
+          <t>Acres</t>
+        </is>
+      </c>
+      <c r="O50" t="inlineStr">
+        <is>
+          <t>Gas</t>
+        </is>
+      </c>
+      <c r="P50" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
     </row>
     <row r="51" ht="15.75" customHeight="1" s="19">
       <c r="A51" s="3" t="inlineStr">
@@ -3613,6 +3727,44 @@
           <t>https://www.zillow.com/homedetails/30-Wigwam-St-Wellfleet-MA-02667/56794923_zpid/</t>
         </is>
       </c>
+      <c r="G51" t="n">
+        <v>1450400</v>
+      </c>
+      <c r="H51" t="n">
+        <v>1472700</v>
+      </c>
+      <c r="I51" t="n">
+        <v>2024</v>
+      </c>
+      <c r="J51" t="inlineStr">
+        <is>
+          <t>2009-01-30</t>
+        </is>
+      </c>
+      <c r="K51" t="n">
+        <v>1</v>
+      </c>
+      <c r="L51" t="n">
+        <v>1963</v>
+      </c>
+      <c r="M51" t="n">
+        <v>0.6099862258953168</v>
+      </c>
+      <c r="N51" t="inlineStr">
+        <is>
+          <t>Acres</t>
+        </is>
+      </c>
+      <c r="O51" t="inlineStr">
+        <is>
+          <t>Other,Gas</t>
+        </is>
+      </c>
+      <c r="P51" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
     </row>
     <row r="52" ht="15.75" customHeight="1" s="19">
       <c r="A52" s="3" t="inlineStr">
@@ -3639,6 +3791,44 @@
           <t>https://www.zillow.com/homedetails/21-Tersolo-Rd-Haverhill-MA-01832/56056744_zpid/</t>
         </is>
       </c>
+      <c r="G52" t="n">
+        <v>803400</v>
+      </c>
+      <c r="H52" t="n">
+        <v>682000</v>
+      </c>
+      <c r="I52" t="n">
+        <v>2024</v>
+      </c>
+      <c r="J52" t="inlineStr">
+        <is>
+          <t>2001-01-11</t>
+        </is>
+      </c>
+      <c r="K52" t="n">
+        <v>2707</v>
+      </c>
+      <c r="L52" t="n">
+        <v>2000</v>
+      </c>
+      <c r="M52" t="n">
+        <v>0.9199954086317723</v>
+      </c>
+      <c r="N52" t="inlineStr">
+        <is>
+          <t>Acres</t>
+        </is>
+      </c>
+      <c r="O52" t="inlineStr">
+        <is>
+          <t>Forced air,Gas</t>
+        </is>
+      </c>
+      <c r="P52" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
     </row>
     <row r="53" ht="15.75" customHeight="1" s="19">
       <c r="A53" s="3" t="inlineStr">
@@ -3665,6 +3855,44 @@
           <t>https://www.zillow.com/homedetails/110-Oaklawn-Ave-Orange-MA-01364/56140342_zpid/</t>
         </is>
       </c>
+      <c r="G53" t="n">
+        <v>290100</v>
+      </c>
+      <c r="H53" t="n">
+        <v>228700</v>
+      </c>
+      <c r="I53" t="n">
+        <v>2024</v>
+      </c>
+      <c r="J53" t="inlineStr">
+        <is>
+          <t>2016-02-29</t>
+        </is>
+      </c>
+      <c r="K53" t="n">
+        <v>954</v>
+      </c>
+      <c r="L53" t="n">
+        <v>1988</v>
+      </c>
+      <c r="M53" t="n">
+        <v>0.5199954086317723</v>
+      </c>
+      <c r="N53" t="inlineStr">
+        <is>
+          <t>Acres</t>
+        </is>
+      </c>
+      <c r="O53" t="inlineStr">
+        <is>
+          <t>Forced air,Gas</t>
+        </is>
+      </c>
+      <c r="P53" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
     </row>
     <row r="54" ht="15.75" customHeight="1" s="19">
       <c r="A54" s="3" t="inlineStr">
@@ -3691,6 +3919,44 @@
           <t>https://www.zillow.com/homedetails/226-Paddocks-Path-Dennis-MA-02638/55877916_zpid/</t>
         </is>
       </c>
+      <c r="G54" t="n">
+        <v>732200</v>
+      </c>
+      <c r="H54" t="n">
+        <v>636600</v>
+      </c>
+      <c r="I54" t="n">
+        <v>2024</v>
+      </c>
+      <c r="J54" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="K54" t="n">
+        <v>1430</v>
+      </c>
+      <c r="L54" t="n">
+        <v>1974</v>
+      </c>
+      <c r="M54" t="n">
+        <v>0.4199954086317723</v>
+      </c>
+      <c r="N54" t="inlineStr">
+        <is>
+          <t>Acres</t>
+        </is>
+      </c>
+      <c r="O54" t="inlineStr">
+        <is>
+          <t>Other,Gas</t>
+        </is>
+      </c>
+      <c r="P54" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
     </row>
     <row r="55" ht="15.75" customHeight="1" s="19">
       <c r="A55" s="3" t="inlineStr">
@@ -3715,6 +3981,44 @@
           <t>https://www.zillow.com/homedetails/32-Woodbury-St-Beverly-MA-01915/59226114_zpid/</t>
         </is>
       </c>
+      <c r="G55" t="n">
+        <v>986700</v>
+      </c>
+      <c r="H55" t="n">
+        <v>806100</v>
+      </c>
+      <c r="I55" t="n">
+        <v>2024</v>
+      </c>
+      <c r="J55" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="K55" t="n">
+        <v>2103</v>
+      </c>
+      <c r="L55" t="n">
+        <v>1950</v>
+      </c>
+      <c r="M55" t="n">
+        <v>8712</v>
+      </c>
+      <c r="N55" t="inlineStr">
+        <is>
+          <t>Square Feet</t>
+        </is>
+      </c>
+      <c r="O55" t="inlineStr">
+        <is>
+          <t>Other,Gas</t>
+        </is>
+      </c>
+      <c r="P55" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
     </row>
     <row r="56" ht="15.75" customHeight="1" s="19">
       <c r="A56" s="3" t="inlineStr">
@@ -3741,6 +4045,44 @@
           <t>https://www.zillow.com/homedetails/27-Windy-Hill-Dr-Plymouth-MA-02360/57545685_zpid/</t>
         </is>
       </c>
+      <c r="G56" t="n">
+        <v>491700</v>
+      </c>
+      <c r="H56" t="n">
+        <v>430200</v>
+      </c>
+      <c r="I56" t="n">
+        <v>2024</v>
+      </c>
+      <c r="J56" t="inlineStr">
+        <is>
+          <t>1988-11-02</t>
+        </is>
+      </c>
+      <c r="K56" t="n">
+        <v>1800</v>
+      </c>
+      <c r="L56" t="n">
+        <v>1982</v>
+      </c>
+      <c r="M56" t="n">
+        <v>1.35</v>
+      </c>
+      <c r="N56" t="inlineStr">
+        <is>
+          <t>Acres</t>
+        </is>
+      </c>
+      <c r="O56" t="inlineStr">
+        <is>
+          <t>Oil</t>
+        </is>
+      </c>
+      <c r="P56" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
     </row>
     <row r="57" ht="15.75" customHeight="1" s="19">
       <c r="A57" s="3" t="inlineStr">
@@ -3765,6 +4107,46 @@
           <t>https://www.zillow.com/homedetails/20-Munroe-St-Somerville-MA-02143/271378798_zpid/</t>
         </is>
       </c>
+      <c r="G57" t="n">
+        <v>1591400</v>
+      </c>
+      <c r="H57" t="n">
+        <v>1369400</v>
+      </c>
+      <c r="I57" t="n">
+        <v>2024</v>
+      </c>
+      <c r="J57" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="K57" t="n">
+        <v>2190</v>
+      </c>
+      <c r="L57" t="n">
+        <v>1925</v>
+      </c>
+      <c r="M57" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="N57" t="inlineStr">
+        <is>
+          <t>sqft</t>
+        </is>
+      </c>
+      <c r="O57" t="inlineStr">
+        <is>
+          <t>Gas</t>
+        </is>
+      </c>
+      <c r="P57" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
     </row>
     <row r="58" ht="15.75" customHeight="1" s="19">
       <c r="A58" s="3" t="inlineStr">
@@ -3791,6 +4173,44 @@
           <t>https://www.zillow.com/homedetails/5-Carrot-Hill-Rd-Falmouth-MA-02543/55898363_zpid/</t>
         </is>
       </c>
+      <c r="G58" t="n">
+        <v>1290600</v>
+      </c>
+      <c r="H58" t="n">
+        <v>1012000</v>
+      </c>
+      <c r="I58" t="n">
+        <v>2024</v>
+      </c>
+      <c r="J58" t="inlineStr">
+        <is>
+          <t>1994-07-29</t>
+        </is>
+      </c>
+      <c r="K58" t="n">
+        <v>2136</v>
+      </c>
+      <c r="L58" t="n">
+        <v>1952</v>
+      </c>
+      <c r="M58" t="n">
+        <v>0.3199954086317723</v>
+      </c>
+      <c r="N58" t="inlineStr">
+        <is>
+          <t>Acres</t>
+        </is>
+      </c>
+      <c r="O58" t="inlineStr">
+        <is>
+          <t>Other,Gas</t>
+        </is>
+      </c>
+      <c r="P58" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
     </row>
     <row r="59" ht="15.75" customHeight="1" s="19">
       <c r="A59" s="3" t="inlineStr">
@@ -3817,6 +4237,44 @@
           <t>https://www.zillow.com/homedetails/110-Lookout-Rd-Yarmouth-Port-MA-02675/55938606_zpid/</t>
         </is>
       </c>
+      <c r="G59" t="n">
+        <v>1234500</v>
+      </c>
+      <c r="H59" t="n">
+        <v>1090400</v>
+      </c>
+      <c r="I59" t="n">
+        <v>2024</v>
+      </c>
+      <c r="J59" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="K59" t="n">
+        <v>2460</v>
+      </c>
+      <c r="L59" t="n">
+        <v>1971</v>
+      </c>
+      <c r="M59" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="N59" t="inlineStr">
+        <is>
+          <t>Acres</t>
+        </is>
+      </c>
+      <c r="O59" t="inlineStr">
+        <is>
+          <t>Forced air,Gas</t>
+        </is>
+      </c>
+      <c r="P59" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
     </row>
     <row r="60" ht="15.75" customHeight="1" s="19">
       <c r="A60" s="3" t="inlineStr">
@@ -3843,6 +4301,44 @@
           <t>https://www.zillow.com/homedetails/35-Sands-Rd-Eastham-MA-02642/56781235_zpid/</t>
         </is>
       </c>
+      <c r="G60" t="n">
+        <v>1115000</v>
+      </c>
+      <c r="H60" t="n">
+        <v>1024100</v>
+      </c>
+      <c r="I60" t="n">
+        <v>2024</v>
+      </c>
+      <c r="J60" t="inlineStr">
+        <is>
+          <t>1997-09-26</t>
+        </is>
+      </c>
+      <c r="K60" t="n">
+        <v>2868</v>
+      </c>
+      <c r="L60" t="n">
+        <v>1969</v>
+      </c>
+      <c r="M60" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="N60" t="inlineStr">
+        <is>
+          <t>Acres</t>
+        </is>
+      </c>
+      <c r="O60" t="inlineStr">
+        <is>
+          <t>Other,Gas</t>
+        </is>
+      </c>
+      <c r="P60" t="inlineStr">
+        <is>
+          <t>Central</t>
+        </is>
+      </c>
     </row>
     <row r="61" ht="15.75" customHeight="1" s="19">
       <c r="A61" s="3" t="inlineStr">
@@ -3869,6 +4365,44 @@
           <t>https://www.zillow.com/homedetails/35-Harborlight-Dr-Plymouth-MA-02360/57540785_zpid/</t>
         </is>
       </c>
+      <c r="G61" t="n">
+        <v>806800</v>
+      </c>
+      <c r="H61" t="n">
+        <v>661300</v>
+      </c>
+      <c r="I61" t="n">
+        <v>2024</v>
+      </c>
+      <c r="J61" t="inlineStr">
+        <is>
+          <t>1996-12-23</t>
+        </is>
+      </c>
+      <c r="K61" t="n">
+        <v>2385</v>
+      </c>
+      <c r="L61" t="n">
+        <v>1996</v>
+      </c>
+      <c r="M61" t="n">
+        <v>0.5799816345270891</v>
+      </c>
+      <c r="N61" t="inlineStr">
+        <is>
+          <t>Acres</t>
+        </is>
+      </c>
+      <c r="O61" t="inlineStr">
+        <is>
+          <t>Other,Oil</t>
+        </is>
+      </c>
+      <c r="P61" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
     </row>
     <row r="62" ht="15.75" customHeight="1" s="19">
       <c r="A62" s="3" t="inlineStr">
@@ -3893,6 +4427,44 @@
           <t>https://www.zillow.com/homedetails/101-Milton-St-Northampton-MA-01062/57022922_zpid/</t>
         </is>
       </c>
+      <c r="G62" t="n">
+        <v>482100</v>
+      </c>
+      <c r="H62" t="n">
+        <v>405300</v>
+      </c>
+      <c r="I62" t="n">
+        <v>2024</v>
+      </c>
+      <c r="J62" t="inlineStr">
+        <is>
+          <t>2013-04-29</t>
+        </is>
+      </c>
+      <c r="K62" t="n">
+        <v>1544</v>
+      </c>
+      <c r="L62" t="n">
+        <v>1900</v>
+      </c>
+      <c r="M62" t="n">
+        <v>0.2899908172635445</v>
+      </c>
+      <c r="N62" t="inlineStr">
+        <is>
+          <t>Acres</t>
+        </is>
+      </c>
+      <c r="O62" t="inlineStr">
+        <is>
+          <t>Forced air,Gas</t>
+        </is>
+      </c>
+      <c r="P62" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
     </row>
     <row r="63" ht="15.75" customHeight="1" s="19">
       <c r="A63" s="3" t="inlineStr">
@@ -3919,6 +4491,44 @@
           <t>https://www.zillow.com/homedetails/321-Pochassic-Rd-Westfield-MA-01085/193631018_zpid/</t>
         </is>
       </c>
+      <c r="G63" t="n">
+        <v>362100</v>
+      </c>
+      <c r="H63" t="n">
+        <v>286000</v>
+      </c>
+      <c r="I63" t="n">
+        <v>2024</v>
+      </c>
+      <c r="J63" t="inlineStr">
+        <is>
+          <t>2014-05-09</t>
+        </is>
+      </c>
+      <c r="K63" t="n">
+        <v>1080</v>
+      </c>
+      <c r="L63" t="n">
+        <v>1985</v>
+      </c>
+      <c r="M63" t="n">
+        <v>1</v>
+      </c>
+      <c r="N63" t="inlineStr">
+        <is>
+          <t>Acres</t>
+        </is>
+      </c>
+      <c r="O63" t="inlineStr">
+        <is>
+          <t>Electric</t>
+        </is>
+      </c>
+      <c r="P63" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
     </row>
     <row r="64" ht="15.75" customHeight="1" s="19">
       <c r="A64" s="3" t="inlineStr">
@@ -3943,6 +4553,44 @@
           <t>https://www.zillow.com/homedetails/401-Queen-Anne-Rd-Harwich-MA-02645/186992422_zpid/</t>
         </is>
       </c>
+      <c r="G64" t="n">
+        <v>475200</v>
+      </c>
+      <c r="H64" t="n">
+        <v>380100</v>
+      </c>
+      <c r="I64" t="n">
+        <v>2024</v>
+      </c>
+      <c r="J64" t="inlineStr">
+        <is>
+          <t>2000-08-01</t>
+        </is>
+      </c>
+      <c r="K64" t="n">
+        <v>1204</v>
+      </c>
+      <c r="L64" t="n">
+        <v>1870</v>
+      </c>
+      <c r="M64" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="N64" t="inlineStr">
+        <is>
+          <t>Acres</t>
+        </is>
+      </c>
+      <c r="O64" t="inlineStr">
+        <is>
+          <t>Gas</t>
+        </is>
+      </c>
+      <c r="P64" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
     </row>
     <row r="65" ht="15.75" customHeight="1" s="19">
       <c r="A65" s="3" t="inlineStr">
@@ -3967,6 +4615,44 @@
           <t>https://www.zillow.com/homedetails/301-Islington-Rd-Newton-MA-02466/56309787_zpid/</t>
         </is>
       </c>
+      <c r="G65" t="n">
+        <v>1787100</v>
+      </c>
+      <c r="H65" t="n">
+        <v>1494700</v>
+      </c>
+      <c r="I65" t="n">
+        <v>2024</v>
+      </c>
+      <c r="J65" t="inlineStr">
+        <is>
+          <t>1982-08-01</t>
+        </is>
+      </c>
+      <c r="K65" t="n">
+        <v>2229</v>
+      </c>
+      <c r="L65" t="n">
+        <v>1945</v>
+      </c>
+      <c r="M65" t="n">
+        <v>0.3199954086317723</v>
+      </c>
+      <c r="N65" t="inlineStr">
+        <is>
+          <t>Acres</t>
+        </is>
+      </c>
+      <c r="O65" t="inlineStr">
+        <is>
+          <t>Other,Gas</t>
+        </is>
+      </c>
+      <c r="P65" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
     </row>
     <row r="66" ht="15.75" customHeight="1" s="19">
       <c r="A66" s="3" t="inlineStr">
@@ -3993,6 +4679,44 @@
           <t>https://www.zillow.com/homedetails/100-Jeffrey-Rd-Springfield-MA-01119/56216024_zpid/</t>
         </is>
       </c>
+      <c r="G66" t="n">
+        <v>369200</v>
+      </c>
+      <c r="H66" t="n">
+        <v>363600</v>
+      </c>
+      <c r="I66" t="n">
+        <v>2024</v>
+      </c>
+      <c r="J66" t="inlineStr">
+        <is>
+          <t>2019-04-30</t>
+        </is>
+      </c>
+      <c r="K66" t="n">
+        <v>1588</v>
+      </c>
+      <c r="L66" t="n">
+        <v>1955</v>
+      </c>
+      <c r="M66" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="N66" t="inlineStr">
+        <is>
+          <t>Acres</t>
+        </is>
+      </c>
+      <c r="O66" t="inlineStr">
+        <is>
+          <t>Forced air,Oil</t>
+        </is>
+      </c>
+      <c r="P66" t="inlineStr">
+        <is>
+          <t>Central</t>
+        </is>
+      </c>
     </row>
     <row r="67" ht="15.75" customHeight="1" s="19">
       <c r="A67" s="3" t="inlineStr">
@@ -4019,6 +4743,44 @@
           <t>https://www.zillow.com/homedetails/6-Pheasant-Ln-Topsfield-MA-01983/56969565_zpid/</t>
         </is>
       </c>
+      <c r="G67" t="n">
+        <v>1065600</v>
+      </c>
+      <c r="H67" t="n">
+        <v>891600</v>
+      </c>
+      <c r="I67" t="n">
+        <v>2024</v>
+      </c>
+      <c r="J67" t="inlineStr">
+        <is>
+          <t>1993-01-22</t>
+        </is>
+      </c>
+      <c r="K67" t="n">
+        <v>2768</v>
+      </c>
+      <c r="L67" t="n">
+        <v>1992</v>
+      </c>
+      <c r="M67" t="n">
+        <v>1.119995408631772</v>
+      </c>
+      <c r="N67" t="inlineStr">
+        <is>
+          <t>Acres</t>
+        </is>
+      </c>
+      <c r="O67" t="inlineStr">
+        <is>
+          <t>Other,Oil</t>
+        </is>
+      </c>
+      <c r="P67" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
     </row>
     <row r="68" ht="15.75" customHeight="1" s="19">
       <c r="A68" s="3" t="inlineStr">
@@ -4043,6 +4805,44 @@
           <t>https://www.zillow.com/homedetails/21-Crescent-Rd-Needham-MA-02494/57477934_zpid/</t>
         </is>
       </c>
+      <c r="G68" t="n">
+        <v>1723000</v>
+      </c>
+      <c r="H68" t="n">
+        <v>1776100</v>
+      </c>
+      <c r="I68" t="n">
+        <v>2024</v>
+      </c>
+      <c r="J68" t="inlineStr">
+        <is>
+          <t>2020-12-11</t>
+        </is>
+      </c>
+      <c r="K68" t="n">
+        <v>3064</v>
+      </c>
+      <c r="L68" t="n">
+        <v>2020</v>
+      </c>
+      <c r="M68" t="n">
+        <v>6969</v>
+      </c>
+      <c r="N68" t="inlineStr">
+        <is>
+          <t>Square Feet</t>
+        </is>
+      </c>
+      <c r="O68" t="inlineStr">
+        <is>
+          <t>Forced air,Gas</t>
+        </is>
+      </c>
+      <c r="P68" t="inlineStr">
+        <is>
+          <t>Central</t>
+        </is>
+      </c>
     </row>
     <row r="69" ht="15.75" customHeight="1" s="19">
       <c r="A69" s="3" t="inlineStr">
@@ -4067,6 +4867,44 @@
           <t>https://www.zillow.com/homedetails/250-Summer-St-Lee-MA-01238/56804136_zpid/</t>
         </is>
       </c>
+      <c r="G69" t="n">
+        <v>444000</v>
+      </c>
+      <c r="H69" t="n">
+        <v>378900</v>
+      </c>
+      <c r="I69" t="n">
+        <v>2024</v>
+      </c>
+      <c r="J69" t="inlineStr">
+        <is>
+          <t>2024-08-20</t>
+        </is>
+      </c>
+      <c r="K69" t="n">
+        <v>2212</v>
+      </c>
+      <c r="L69" t="n">
+        <v>1900</v>
+      </c>
+      <c r="M69" t="n">
+        <v>2.32</v>
+      </c>
+      <c r="N69" t="inlineStr">
+        <is>
+          <t>Acres</t>
+        </is>
+      </c>
+      <c r="O69" t="inlineStr">
+        <is>
+          <t>Solar,Oil,Furnace,Hot Water</t>
+        </is>
+      </c>
+      <c r="P69" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
     </row>
     <row r="70" ht="15.75" customHeight="1" s="19">
       <c r="A70" s="3" t="inlineStr">
@@ -4091,6 +4929,44 @@
           <t>https://www.zillow.com/homedetails/1-Sea-Mist-Ln-Rockport-MA-01966/56957270_zpid/</t>
         </is>
       </c>
+      <c r="G70" t="n">
+        <v>712700</v>
+      </c>
+      <c r="H70" t="n">
+        <v>554700</v>
+      </c>
+      <c r="I70" t="n">
+        <v>2024</v>
+      </c>
+      <c r="J70" t="inlineStr">
+        <is>
+          <t>1993-05-18</t>
+        </is>
+      </c>
+      <c r="K70" t="n">
+        <v>1556</v>
+      </c>
+      <c r="L70" t="n">
+        <v>1956</v>
+      </c>
+      <c r="M70" t="n">
+        <v>0.35</v>
+      </c>
+      <c r="N70" t="inlineStr">
+        <is>
+          <t>Acres</t>
+        </is>
+      </c>
+      <c r="O70" t="inlineStr">
+        <is>
+          <t>Forced air,Oil</t>
+        </is>
+      </c>
+      <c r="P70" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
     </row>
     <row r="71" ht="15.75" customHeight="1" s="19">
       <c r="A71" s="3" t="inlineStr">
@@ -4117,6 +4993,44 @@
           <t>https://www.zillow.com/homedetails/184-N-Leverett-Rd-Leverett-MA-01054/80863083_zpid/</t>
         </is>
       </c>
+      <c r="G71" t="n">
+        <v>614200</v>
+      </c>
+      <c r="H71" t="n">
+        <v>477100</v>
+      </c>
+      <c r="I71" t="n">
+        <v>2024</v>
+      </c>
+      <c r="J71" t="inlineStr">
+        <is>
+          <t>2006-03-31</t>
+        </is>
+      </c>
+      <c r="K71" t="n">
+        <v>2387</v>
+      </c>
+      <c r="L71" t="n">
+        <v>1773</v>
+      </c>
+      <c r="M71" t="n">
+        <v>8.970821854912764</v>
+      </c>
+      <c r="N71" t="inlineStr">
+        <is>
+          <t>Acres</t>
+        </is>
+      </c>
+      <c r="O71" t="inlineStr">
+        <is>
+          <t>Forced air,Stove,Gas,Oil,Wood / Pellet</t>
+        </is>
+      </c>
+      <c r="P71" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
     </row>
     <row r="72" ht="15.75" customHeight="1" s="19">
       <c r="A72" s="3" t="inlineStr">
@@ -4143,6 +5057,44 @@
           <t>https://www.zillow.com/homedetails/18-Knollwood-Dr-Dartmouth-MA-02747/55966575_zpid/</t>
         </is>
       </c>
+      <c r="G72" t="n">
+        <v>670200</v>
+      </c>
+      <c r="H72" t="n">
+        <v>537900</v>
+      </c>
+      <c r="I72" t="n">
+        <v>2024</v>
+      </c>
+      <c r="J72" t="inlineStr">
+        <is>
+          <t>2003-08-01</t>
+        </is>
+      </c>
+      <c r="K72" t="n">
+        <v>2021</v>
+      </c>
+      <c r="L72" t="n">
+        <v>1991</v>
+      </c>
+      <c r="M72" t="n">
+        <v>0.9182966023875114</v>
+      </c>
+      <c r="N72" t="inlineStr">
+        <is>
+          <t>Acres</t>
+        </is>
+      </c>
+      <c r="O72" t="inlineStr">
+        <is>
+          <t>Other,Oil</t>
+        </is>
+      </c>
+      <c r="P72" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
     </row>
     <row r="73" ht="15.75" customHeight="1" s="19">
       <c r="A73" s="3" t="inlineStr">
@@ -4169,6 +5121,44 @@
           <t>https://www.zillow.com/homedetails/45-Greenwood-Ave-Needham-MA-02492/57475272_zpid/</t>
         </is>
       </c>
+      <c r="G73" t="n">
+        <v>1689900</v>
+      </c>
+      <c r="H73" t="n">
+        <v>1016500</v>
+      </c>
+      <c r="I73" t="n">
+        <v>2024</v>
+      </c>
+      <c r="J73" t="inlineStr">
+        <is>
+          <t>1993-06-16</t>
+        </is>
+      </c>
+      <c r="K73" t="n">
+        <v>3176</v>
+      </c>
+      <c r="L73" t="n">
+        <v>1914</v>
+      </c>
+      <c r="M73" t="n">
+        <v>8276</v>
+      </c>
+      <c r="N73" t="inlineStr">
+        <is>
+          <t>Square Feet</t>
+        </is>
+      </c>
+      <c r="O73" t="inlineStr">
+        <is>
+          <t>Baseboard,Heat pump,Gas,Solar</t>
+        </is>
+      </c>
+      <c r="P73" t="inlineStr">
+        <is>
+          <t>Central,Solar</t>
+        </is>
+      </c>
     </row>
     <row r="74" ht="15.75" customHeight="1" s="19">
       <c r="A74" s="3" t="inlineStr">
@@ -4195,6 +5185,44 @@
           <t>https://www.zillow.com/homedetails/3-Bowers-Ave-Tyngsboro-MA-01879/57122674_zpid/</t>
         </is>
       </c>
+      <c r="G74" t="n">
+        <v>778200</v>
+      </c>
+      <c r="H74" t="n">
+        <v>616200</v>
+      </c>
+      <c r="I74" t="n">
+        <v>2024</v>
+      </c>
+      <c r="J74" t="inlineStr">
+        <is>
+          <t>2004-05-28</t>
+        </is>
+      </c>
+      <c r="K74" t="n">
+        <v>2510</v>
+      </c>
+      <c r="L74" t="n">
+        <v>1985</v>
+      </c>
+      <c r="M74" t="n">
+        <v>0.3899908172635445</v>
+      </c>
+      <c r="N74" t="inlineStr">
+        <is>
+          <t>Acres</t>
+        </is>
+      </c>
+      <c r="O74" t="inlineStr">
+        <is>
+          <t>Forced air,Oil</t>
+        </is>
+      </c>
+      <c r="P74" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
     </row>
     <row r="75" ht="15.75" customHeight="1" s="19">
       <c r="A75" s="3" t="inlineStr">
@@ -4221,6 +5249,44 @@
           <t>https://www.zillow.com/homedetails/24-Green-Valley-Rd-Medway-MA-02053/57461159_zpid/</t>
         </is>
       </c>
+      <c r="G75" t="n">
+        <v>878300</v>
+      </c>
+      <c r="H75" t="n">
+        <v>715300</v>
+      </c>
+      <c r="I75" t="n">
+        <v>2024</v>
+      </c>
+      <c r="J75" t="inlineStr">
+        <is>
+          <t>2002-03-22</t>
+        </is>
+      </c>
+      <c r="K75" t="n">
+        <v>2715</v>
+      </c>
+      <c r="L75" t="n">
+        <v>1977</v>
+      </c>
+      <c r="M75" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="N75" t="inlineStr">
+        <is>
+          <t>Acres</t>
+        </is>
+      </c>
+      <c r="O75" t="inlineStr">
+        <is>
+          <t>Other,Oil</t>
+        </is>
+      </c>
+      <c r="P75" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
     </row>
     <row r="76" ht="15.75" customHeight="1" s="19">
       <c r="A76" s="3" t="inlineStr">
@@ -4245,6 +5311,44 @@
           <t>https://www.zillow.com/homedetails/105-E-Gate-Rd-Brewster-MA-02631/186846759_zpid/</t>
         </is>
       </c>
+      <c r="G76" t="n">
+        <v>1578200</v>
+      </c>
+      <c r="H76" t="n">
+        <v>1319700</v>
+      </c>
+      <c r="I76" t="n">
+        <v>2024</v>
+      </c>
+      <c r="J76" t="inlineStr">
+        <is>
+          <t>1990-08-08</t>
+        </is>
+      </c>
+      <c r="K76" t="n">
+        <v>3345</v>
+      </c>
+      <c r="L76" t="n">
+        <v>1988</v>
+      </c>
+      <c r="M76" t="n">
+        <v>7.7</v>
+      </c>
+      <c r="N76" t="inlineStr">
+        <is>
+          <t>Acres</t>
+        </is>
+      </c>
+      <c r="O76" t="inlineStr">
+        <is>
+          <t>Oil</t>
+        </is>
+      </c>
+      <c r="P76" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
     </row>
     <row r="77" ht="15.75" customHeight="1" s="19">
       <c r="A77" s="3" t="inlineStr">
@@ -4271,6 +5375,44 @@
           <t>https://www.zillow.com/homedetails/26-Walnut-Rd-South-Hamilton-MA-01982/56924745_zpid/</t>
         </is>
       </c>
+      <c r="G77" t="n">
+        <v>1142400</v>
+      </c>
+      <c r="H77" t="n">
+        <v>679800</v>
+      </c>
+      <c r="I77" t="n">
+        <v>2024</v>
+      </c>
+      <c r="J77" t="inlineStr">
+        <is>
+          <t>2019-10-16</t>
+        </is>
+      </c>
+      <c r="K77" t="n">
+        <v>3138</v>
+      </c>
+      <c r="L77" t="n">
+        <v>1891</v>
+      </c>
+      <c r="M77" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="N77" t="inlineStr">
+        <is>
+          <t>Acres</t>
+        </is>
+      </c>
+      <c r="O77" t="inlineStr">
+        <is>
+          <t>Radiant,Gas,Other</t>
+        </is>
+      </c>
+      <c r="P77" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
     </row>
     <row r="78" ht="15.75" customHeight="1" s="19">
       <c r="A78" s="3" t="inlineStr">
@@ -4295,6 +5437,44 @@
           <t>https://www.zillow.com/homedetails/42-Lake-Ave-Framingham-MA-01702/165996355_zpid/</t>
         </is>
       </c>
+      <c r="G78" t="n">
+        <v>939400</v>
+      </c>
+      <c r="H78" t="n">
+        <v>726500</v>
+      </c>
+      <c r="I78" t="n">
+        <v>2024</v>
+      </c>
+      <c r="J78" t="inlineStr">
+        <is>
+          <t>1990-06-22</t>
+        </is>
+      </c>
+      <c r="K78" t="n">
+        <v>2484</v>
+      </c>
+      <c r="L78" t="n">
+        <v>1919</v>
+      </c>
+      <c r="M78" t="n">
+        <v>3484</v>
+      </c>
+      <c r="N78" t="inlineStr">
+        <is>
+          <t>Square Feet</t>
+        </is>
+      </c>
+      <c r="O78" t="inlineStr">
+        <is>
+          <t>Oil</t>
+        </is>
+      </c>
+      <c r="P78" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
     </row>
     <row r="79" ht="15.75" customHeight="1" s="19">
       <c r="A79" s="3" t="inlineStr">
@@ -4321,6 +5501,44 @@
           <t>https://www.zillow.com/homedetails/17-Fernwood-Dr-Hampden-MA-01036/56173594_zpid/</t>
         </is>
       </c>
+      <c r="G79" t="n">
+        <v>389300</v>
+      </c>
+      <c r="H79" t="n">
+        <v>313600</v>
+      </c>
+      <c r="I79" t="n">
+        <v>2024</v>
+      </c>
+      <c r="J79" t="inlineStr">
+        <is>
+          <t>2016-04-01</t>
+        </is>
+      </c>
+      <c r="K79" t="n">
+        <v>1325</v>
+      </c>
+      <c r="L79" t="n">
+        <v>1963</v>
+      </c>
+      <c r="M79" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="N79" t="inlineStr">
+        <is>
+          <t>Acres</t>
+        </is>
+      </c>
+      <c r="O79" t="inlineStr">
+        <is>
+          <t>Other,Gas</t>
+        </is>
+      </c>
+      <c r="P79" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
     </row>
     <row r="80" ht="15.75" customHeight="1" s="19">
       <c r="A80" s="3" t="inlineStr">
@@ -4347,6 +5565,44 @@
           <t>https://www.zillow.com/homedetails/342-Belknap-Rd-Framingham-MA-01701/165986610_zpid/</t>
         </is>
       </c>
+      <c r="G80" t="n">
+        <v>783700</v>
+      </c>
+      <c r="H80" t="n">
+        <v>636000</v>
+      </c>
+      <c r="I80" t="n">
+        <v>2024</v>
+      </c>
+      <c r="J80" t="inlineStr">
+        <is>
+          <t>2003-09-29</t>
+        </is>
+      </c>
+      <c r="K80" t="n">
+        <v>1534</v>
+      </c>
+      <c r="L80" t="n">
+        <v>1964</v>
+      </c>
+      <c r="M80" t="n">
+        <v>0.4899908172635445</v>
+      </c>
+      <c r="N80" t="inlineStr">
+        <is>
+          <t>Acres</t>
+        </is>
+      </c>
+      <c r="O80" t="inlineStr">
+        <is>
+          <t>Gas</t>
+        </is>
+      </c>
+      <c r="P80" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
     </row>
     <row r="81" ht="15.75" customHeight="1" s="19">
       <c r="A81" s="3" t="inlineStr">
@@ -4373,6 +5629,44 @@
           <t>https://www.zillow.com/homedetails/435-Martins-Pond-Rd-Groton-MA-01450/57066211_zpid/</t>
         </is>
       </c>
+      <c r="G81" t="n">
+        <v>689700</v>
+      </c>
+      <c r="H81" t="n">
+        <v>620450</v>
+      </c>
+      <c r="I81" t="n">
+        <v>2024</v>
+      </c>
+      <c r="J81" t="inlineStr">
+        <is>
+          <t>1995-01-04</t>
+        </is>
+      </c>
+      <c r="K81" t="n">
+        <v>1472</v>
+      </c>
+      <c r="L81" t="n">
+        <v>1978</v>
+      </c>
+      <c r="M81" t="n">
+        <v>15.1</v>
+      </c>
+      <c r="N81" t="inlineStr">
+        <is>
+          <t>Acres</t>
+        </is>
+      </c>
+      <c r="O81" t="inlineStr">
+        <is>
+          <t>Forced air,Oil</t>
+        </is>
+      </c>
+      <c r="P81" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
     </row>
     <row r="82" ht="15.75" customHeight="1" s="19">
       <c r="A82" s="3" t="inlineStr">
@@ -4399,6 +5693,44 @@
           <t>https://www.zillow.com/homedetails/103-Farm-St-Bellingham-MA-02019/123883120_zpid/</t>
         </is>
       </c>
+      <c r="G82" t="n">
+        <v>731700</v>
+      </c>
+      <c r="H82" t="n">
+        <v>544400</v>
+      </c>
+      <c r="I82" t="n">
+        <v>2024</v>
+      </c>
+      <c r="J82" t="inlineStr">
+        <is>
+          <t>2014-05-23</t>
+        </is>
+      </c>
+      <c r="K82" t="n">
+        <v>2381</v>
+      </c>
+      <c r="L82" t="n">
+        <v>2013</v>
+      </c>
+      <c r="M82" t="n">
+        <v>1.051997245179063</v>
+      </c>
+      <c r="N82" t="inlineStr">
+        <is>
+          <t>Acres</t>
+        </is>
+      </c>
+      <c r="O82" t="inlineStr">
+        <is>
+          <t>Forced air,Gas,Solar</t>
+        </is>
+      </c>
+      <c r="P82" t="inlineStr">
+        <is>
+          <t>Central</t>
+        </is>
+      </c>
     </row>
     <row r="83" ht="15.75" customHeight="1" s="19">
       <c r="A83" s="3" t="inlineStr">
@@ -4454,6 +5786,44 @@
           <t>https://www.zillow.com/homedetails/4-Vineyard-Ave-Clinton-MA-01510/57577271_zpid/</t>
         </is>
       </c>
+      <c r="G84" t="n">
+        <v>544200</v>
+      </c>
+      <c r="H84" t="n">
+        <v>425200</v>
+      </c>
+      <c r="I84" t="n">
+        <v>2024</v>
+      </c>
+      <c r="J84" t="inlineStr">
+        <is>
+          <t>2017-05-12</t>
+        </is>
+      </c>
+      <c r="K84" t="n">
+        <v>1765</v>
+      </c>
+      <c r="L84" t="n">
+        <v>1950</v>
+      </c>
+      <c r="M84" t="n">
+        <v>0.4299816345270891</v>
+      </c>
+      <c r="N84" t="inlineStr">
+        <is>
+          <t>Acres</t>
+        </is>
+      </c>
+      <c r="O84" t="inlineStr">
+        <is>
+          <t>Baseboard,Oil</t>
+        </is>
+      </c>
+      <c r="P84" t="inlineStr">
+        <is>
+          <t>Solar</t>
+        </is>
+      </c>
     </row>
     <row r="85" ht="15.75" customHeight="1" s="19">
       <c r="A85" s="3" t="inlineStr">
@@ -4480,6 +5850,44 @@
           <t>https://www.zillow.com/homedetails/335-Grand-Ave-Falmouth-MA-02540/55896521_zpid/</t>
         </is>
       </c>
+      <c r="G85" t="n">
+        <v>1916200</v>
+      </c>
+      <c r="H85" t="n">
+        <v>1127600</v>
+      </c>
+      <c r="I85" t="n">
+        <v>2024</v>
+      </c>
+      <c r="J85" t="inlineStr">
+        <is>
+          <t>2016-05-13</t>
+        </is>
+      </c>
+      <c r="K85" t="n">
+        <v>4162</v>
+      </c>
+      <c r="L85" t="n">
+        <v>1880</v>
+      </c>
+      <c r="M85" t="n">
+        <v>3920</v>
+      </c>
+      <c r="N85" t="inlineStr">
+        <is>
+          <t>Square Feet</t>
+        </is>
+      </c>
+      <c r="O85" t="inlineStr">
+        <is>
+          <t>Baseboard,Other,Gas,Other</t>
+        </is>
+      </c>
+      <c r="P85" t="inlineStr">
+        <is>
+          <t>Solar</t>
+        </is>
+      </c>
     </row>
     <row r="86" ht="15.75" customHeight="1" s="19">
       <c r="A86" s="3" t="inlineStr">
@@ -4506,6 +5914,44 @@
           <t>https://www.zillow.com/homedetails/55-Orchard-Hill-Dr-Plymouth-MA-02360/123191116_zpid/</t>
         </is>
       </c>
+      <c r="G86" t="n">
+        <v>1208300</v>
+      </c>
+      <c r="H86" t="n">
+        <v>960600</v>
+      </c>
+      <c r="I86" t="n">
+        <v>2024</v>
+      </c>
+      <c r="J86" t="inlineStr">
+        <is>
+          <t>2014-12-19</t>
+        </is>
+      </c>
+      <c r="K86" t="n">
+        <v>3814</v>
+      </c>
+      <c r="L86" t="n">
+        <v>2014</v>
+      </c>
+      <c r="M86" t="n">
+        <v>0.9399908172635445</v>
+      </c>
+      <c r="N86" t="inlineStr">
+        <is>
+          <t>Acres</t>
+        </is>
+      </c>
+      <c r="O86" t="inlineStr">
+        <is>
+          <t>Forced air,Gas</t>
+        </is>
+      </c>
+      <c r="P86" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
     </row>
     <row r="87" ht="15.75" customHeight="1" s="19">
       <c r="A87" s="3" t="inlineStr">
@@ -4530,6 +5976,44 @@
           <t>https://www.zillow.com/homedetails/9-Theresa-Ave-Burlington-MA-01803/57055850_zpid/</t>
         </is>
       </c>
+      <c r="G87" t="n">
+        <v>1164200</v>
+      </c>
+      <c r="H87" t="n">
+        <v>889100</v>
+      </c>
+      <c r="I87" t="n">
+        <v>2024</v>
+      </c>
+      <c r="J87" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="K87" t="n">
+        <v>2262</v>
+      </c>
+      <c r="L87" t="n">
+        <v>1995</v>
+      </c>
+      <c r="M87" t="n">
+        <v>0.8099862258953168</v>
+      </c>
+      <c r="N87" t="inlineStr">
+        <is>
+          <t>Acres</t>
+        </is>
+      </c>
+      <c r="O87" t="inlineStr">
+        <is>
+          <t>Forced air,Gas</t>
+        </is>
+      </c>
+      <c r="P87" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
     </row>
     <row r="88" ht="15.75" customHeight="1" s="19">
       <c r="A88" s="3" t="inlineStr">
@@ -4556,6 +6040,44 @@
           <t>https://www.zillow.com/homedetails/32-Pearl-Brook-Rd-Lunenburg-MA-01462/57611448_zpid/</t>
         </is>
       </c>
+      <c r="G88" t="n">
+        <v>487600</v>
+      </c>
+      <c r="H88" t="n">
+        <v>434900</v>
+      </c>
+      <c r="I88" t="n">
+        <v>2024</v>
+      </c>
+      <c r="J88" t="inlineStr">
+        <is>
+          <t>1988-04-22</t>
+        </is>
+      </c>
+      <c r="K88" t="n">
+        <v>1344</v>
+      </c>
+      <c r="L88" t="n">
+        <v>1970</v>
+      </c>
+      <c r="M88" t="n">
+        <v>0.4599862258953168</v>
+      </c>
+      <c r="N88" t="inlineStr">
+        <is>
+          <t>Acres</t>
+        </is>
+      </c>
+      <c r="O88" t="inlineStr">
+        <is>
+          <t>Other,Oil</t>
+        </is>
+      </c>
+      <c r="P88" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
     </row>
     <row r="89" ht="15.75" customHeight="1" s="19">
       <c r="A89" s="3" t="inlineStr">
@@ -4580,6 +6102,44 @@
           <t>https://www.zillow.com/homedetails/23-Whittemore-St-Arlington-MA-02474/56393572_zpid/</t>
         </is>
       </c>
+      <c r="G89" t="n">
+        <v>1566100</v>
+      </c>
+      <c r="H89" t="n">
+        <v>1331100</v>
+      </c>
+      <c r="I89" t="n">
+        <v>2024</v>
+      </c>
+      <c r="J89" t="inlineStr">
+        <is>
+          <t>2011-07-19</t>
+        </is>
+      </c>
+      <c r="K89" t="n">
+        <v>1794</v>
+      </c>
+      <c r="L89" t="n">
+        <v>1900</v>
+      </c>
+      <c r="M89" t="n">
+        <v>3292</v>
+      </c>
+      <c r="N89" t="inlineStr">
+        <is>
+          <t>Square Feet</t>
+        </is>
+      </c>
+      <c r="O89" t="inlineStr">
+        <is>
+          <t>Forced air,Gas</t>
+        </is>
+      </c>
+      <c r="P89" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
     </row>
     <row r="90" ht="15.75" customHeight="1" s="19">
       <c r="A90" s="3" t="inlineStr">
@@ -4606,6 +6166,44 @@
           <t>https://www.zillow.com/homedetails/38-Southwick-Rd-Sutton-MA-01590/57655803_zpid/</t>
         </is>
       </c>
+      <c r="G90" t="n">
+        <v>870400</v>
+      </c>
+      <c r="H90" t="n">
+        <v>691900</v>
+      </c>
+      <c r="I90" t="n">
+        <v>2024</v>
+      </c>
+      <c r="J90" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="K90" t="n">
+        <v>3132</v>
+      </c>
+      <c r="L90" t="n">
+        <v>1980</v>
+      </c>
+      <c r="M90" t="n">
+        <v>12.9</v>
+      </c>
+      <c r="N90" t="inlineStr">
+        <is>
+          <t>Acres</t>
+        </is>
+      </c>
+      <c r="O90" t="inlineStr">
+        <is>
+          <t>Other,Oil</t>
+        </is>
+      </c>
+      <c r="P90" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
     </row>
     <row r="91" ht="15.75" customHeight="1" s="19">
       <c r="A91" s="3" t="inlineStr">
@@ -4656,6 +6254,44 @@
           <t>https://www.zillow.com/homedetails/100-W-Chestnut-Hill-Rd-Montague-MA-01351/56984464_zpid/</t>
         </is>
       </c>
+      <c r="G92" t="n">
+        <v>320300</v>
+      </c>
+      <c r="H92" t="n">
+        <v>247800</v>
+      </c>
+      <c r="I92" t="n">
+        <v>2024</v>
+      </c>
+      <c r="J92" t="inlineStr">
+        <is>
+          <t>2012-10-26</t>
+        </is>
+      </c>
+      <c r="K92" t="n">
+        <v>869</v>
+      </c>
+      <c r="L92" t="n">
+        <v>1972</v>
+      </c>
+      <c r="M92" t="n">
+        <v>4.013888888888889</v>
+      </c>
+      <c r="N92" t="inlineStr">
+        <is>
+          <t>Acres</t>
+        </is>
+      </c>
+      <c r="O92" t="inlineStr">
+        <is>
+          <t>Forced air,Gas</t>
+        </is>
+      </c>
+      <c r="P92" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
     </row>
     <row r="93" ht="15.75" customHeight="1" s="19">
       <c r="A93" s="3" t="inlineStr">
@@ -4680,6 +6316,44 @@
           <t>https://www.zillow.com/homedetails/5-Chestnut-Hill-Rd-Warwick-MA-01378/56987857_zpid/</t>
         </is>
       </c>
+      <c r="G93" t="n">
+        <v>299400</v>
+      </c>
+      <c r="H93" t="n">
+        <v>235800</v>
+      </c>
+      <c r="I93" t="n">
+        <v>2024</v>
+      </c>
+      <c r="J93" t="inlineStr">
+        <is>
+          <t>1987-11-27</t>
+        </is>
+      </c>
+      <c r="K93" t="n">
+        <v>1862</v>
+      </c>
+      <c r="L93" t="n">
+        <v>1790</v>
+      </c>
+      <c r="M93" t="n">
+        <v>2</v>
+      </c>
+      <c r="N93" t="inlineStr">
+        <is>
+          <t>Acres</t>
+        </is>
+      </c>
+      <c r="O93" t="inlineStr">
+        <is>
+          <t>Other,Oil</t>
+        </is>
+      </c>
+      <c r="P93" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
     </row>
     <row r="94" ht="15.75" customHeight="1" s="19">
       <c r="A94" s="3" t="inlineStr">
@@ -4704,6 +6378,44 @@
           <t>https://www.zillow.com/homedetails/100-Montclair-Ave-Waltham-MA-02451/56358859_zpid/</t>
         </is>
       </c>
+      <c r="G94" t="n">
+        <v>639200</v>
+      </c>
+      <c r="H94" t="n">
+        <v>528000</v>
+      </c>
+      <c r="I94" t="n">
+        <v>2024</v>
+      </c>
+      <c r="J94" t="inlineStr">
+        <is>
+          <t>2013-12-23</t>
+        </is>
+      </c>
+      <c r="K94" t="n">
+        <v>1425</v>
+      </c>
+      <c r="L94" t="n">
+        <v>1952</v>
+      </c>
+      <c r="M94" t="n">
+        <v>3136</v>
+      </c>
+      <c r="N94" t="inlineStr">
+        <is>
+          <t>Square Feet</t>
+        </is>
+      </c>
+      <c r="O94" t="inlineStr">
+        <is>
+          <t>Baseboard,Oil</t>
+        </is>
+      </c>
+      <c r="P94" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
     </row>
     <row r="95" ht="15.75" customHeight="1" s="19">
       <c r="A95" s="3" t="inlineStr">
@@ -4761,6 +6473,44 @@
           <t>https://www.zillow.com/homedetails/114-Pine-St-Northampton-MA-01062/57021156_zpid/</t>
         </is>
       </c>
+      <c r="G96" t="n">
+        <v>561900</v>
+      </c>
+      <c r="H96" t="n">
+        <v>521700</v>
+      </c>
+      <c r="I96" t="n">
+        <v>2024</v>
+      </c>
+      <c r="J96" t="inlineStr">
+        <is>
+          <t>2001-02-09</t>
+        </is>
+      </c>
+      <c r="K96" t="n">
+        <v>2329</v>
+      </c>
+      <c r="L96" t="n">
+        <v>1900</v>
+      </c>
+      <c r="M96" t="n">
+        <v>0.9399908172635445</v>
+      </c>
+      <c r="N96" t="inlineStr">
+        <is>
+          <t>Acres</t>
+        </is>
+      </c>
+      <c r="O96" t="inlineStr">
+        <is>
+          <t>Other,Gas</t>
+        </is>
+      </c>
+      <c r="P96" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
     </row>
     <row r="97" ht="15.75" customHeight="1" s="19">
       <c r="A97" s="3" t="inlineStr">
@@ -4785,6 +6535,44 @@
           <t>https://www.zillow.com/homedetails/27-Hammond-Rd-Hopedale-MA-01747/57602678_zpid/</t>
         </is>
       </c>
+      <c r="G97" t="n">
+        <v>744700</v>
+      </c>
+      <c r="H97" t="n">
+        <v>646500</v>
+      </c>
+      <c r="I97" t="n">
+        <v>2024</v>
+      </c>
+      <c r="J97" t="inlineStr">
+        <is>
+          <t>2010-03-30</t>
+        </is>
+      </c>
+      <c r="K97" t="n">
+        <v>1700</v>
+      </c>
+      <c r="L97" t="n">
+        <v>1986</v>
+      </c>
+      <c r="M97" t="n">
+        <v>0.4595730027548209</v>
+      </c>
+      <c r="N97" t="inlineStr">
+        <is>
+          <t>Acres</t>
+        </is>
+      </c>
+      <c r="O97" t="inlineStr">
+        <is>
+          <t>Other,Oil</t>
+        </is>
+      </c>
+      <c r="P97" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
     </row>
     <row r="98" ht="15.75" customHeight="1" s="19">
       <c r="A98" s="3" t="inlineStr">
@@ -4809,6 +6597,44 @@
           <t>https://www.zillow.com/homedetails/38-Blackberry-Ln-Brewster-MA-02631/56769623_zpid/</t>
         </is>
       </c>
+      <c r="G98" t="n">
+        <v>849500</v>
+      </c>
+      <c r="H98" t="n">
+        <v>659200</v>
+      </c>
+      <c r="I98" t="n">
+        <v>2024</v>
+      </c>
+      <c r="J98" t="inlineStr">
+        <is>
+          <t>2013-04-05</t>
+        </is>
+      </c>
+      <c r="K98" t="n">
+        <v>1600</v>
+      </c>
+      <c r="L98" t="n">
+        <v>1985</v>
+      </c>
+      <c r="M98" t="n">
+        <v>0.5899908172635445</v>
+      </c>
+      <c r="N98" t="inlineStr">
+        <is>
+          <t>Acres</t>
+        </is>
+      </c>
+      <c r="O98" t="inlineStr">
+        <is>
+          <t>Other,Gas</t>
+        </is>
+      </c>
+      <c r="P98" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
     </row>
     <row r="99" ht="15.75" customHeight="1" s="19">
       <c r="A99" s="3" t="inlineStr">
@@ -4833,6 +6659,44 @@
       <c r="F99" s="6" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/50-Deerpath-Rd-Dedham-MA-02026/61317928_zpid/</t>
+        </is>
+      </c>
+      <c r="G99" t="n">
+        <v>1748600</v>
+      </c>
+      <c r="H99" t="n">
+        <v>1561900</v>
+      </c>
+      <c r="I99" t="n">
+        <v>2024</v>
+      </c>
+      <c r="J99" t="inlineStr">
+        <is>
+          <t>2005-07-29</t>
+        </is>
+      </c>
+      <c r="K99" t="n">
+        <v>3756</v>
+      </c>
+      <c r="L99" t="n">
+        <v>1998</v>
+      </c>
+      <c r="M99" t="n">
+        <v>0.9199954086317723</v>
+      </c>
+      <c r="N99" t="inlineStr">
+        <is>
+          <t>Acres</t>
+        </is>
+      </c>
+      <c r="O99" t="inlineStr">
+        <is>
+          <t>Forced air,Oil</t>
+        </is>
+      </c>
+      <c r="P99" t="inlineStr">
+        <is>
+          <t>None</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
finished Zillow data collection, written to Excel
</commit_message>
<xml_diff>
--- a/res-econ_RA_data.xlsx
+++ b/res-econ_RA_data.xlsx
@@ -6982,7 +6982,7 @@
         </is>
       </c>
       <c r="G104" t="n">
-        <v>1540400</v>
+        <v>1554700</v>
       </c>
       <c r="H104" t="n">
         <v>1167700</v>
@@ -7045,6 +7045,44 @@
           <t>https://www.zillow.com/homedetails/458-East-St-Easthampton-MA-01027/57009565_zpid/</t>
         </is>
       </c>
+      <c r="G105" t="n">
+        <v>396300</v>
+      </c>
+      <c r="H105" t="n">
+        <v>343700</v>
+      </c>
+      <c r="I105" t="n">
+        <v>2024</v>
+      </c>
+      <c r="J105" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="K105" t="n">
+        <v>1456</v>
+      </c>
+      <c r="L105" t="n">
+        <v>1974</v>
+      </c>
+      <c r="M105" t="n">
+        <v>2.129981634527089</v>
+      </c>
+      <c r="N105" t="inlineStr">
+        <is>
+          <t>Acres</t>
+        </is>
+      </c>
+      <c r="O105" t="inlineStr">
+        <is>
+          <t>Baseboard,Electric</t>
+        </is>
+      </c>
+      <c r="P105" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
     </row>
     <row r="106" ht="15.75" customHeight="1" s="19">
       <c r="A106" s="3" t="inlineStr">
@@ -7071,6 +7109,46 @@
           <t>https://www.zillow.com/homedetails/23-Orchard-St-Northampton-MA-01060/87798678_zpid/</t>
         </is>
       </c>
+      <c r="G106" t="n">
+        <v>462300</v>
+      </c>
+      <c r="H106" t="n">
+        <v>356900</v>
+      </c>
+      <c r="I106" t="n">
+        <v>2024</v>
+      </c>
+      <c r="J106" t="inlineStr">
+        <is>
+          <t>2018-08-13</t>
+        </is>
+      </c>
+      <c r="K106" t="n">
+        <v>1314</v>
+      </c>
+      <c r="L106" t="n">
+        <v>1900</v>
+      </c>
+      <c r="M106" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="N106" t="inlineStr">
+        <is>
+          <t>sqft</t>
+        </is>
+      </c>
+      <c r="O106" t="inlineStr">
+        <is>
+          <t>Forced air,Oil</t>
+        </is>
+      </c>
+      <c r="P106" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
     </row>
     <row r="107" ht="15.75" customHeight="1" s="19">
       <c r="A107" s="3" t="inlineStr">
@@ -7095,6 +7173,44 @@
           <t>https://www.zillow.com/homedetails/770-Waltham-St-Lexington-MA-02421/56488902_zpid/</t>
         </is>
       </c>
+      <c r="G107" t="n">
+        <v>1927500</v>
+      </c>
+      <c r="H107" t="n">
+        <v>1634000</v>
+      </c>
+      <c r="I107" t="n">
+        <v>2024</v>
+      </c>
+      <c r="J107" t="inlineStr">
+        <is>
+          <t>1992-11-13</t>
+        </is>
+      </c>
+      <c r="K107" t="n">
+        <v>2516</v>
+      </c>
+      <c r="L107" t="n">
+        <v>2019</v>
+      </c>
+      <c r="M107" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="N107" t="inlineStr">
+        <is>
+          <t>Acres</t>
+        </is>
+      </c>
+      <c r="O107" t="inlineStr">
+        <is>
+          <t>Other,Gas</t>
+        </is>
+      </c>
+      <c r="P107" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
     </row>
     <row r="108" ht="15.75" customHeight="1" s="19">
       <c r="A108" s="3" t="inlineStr">
@@ -7121,6 +7237,44 @@
           <t>https://www.zillow.com/homedetails/100-Moser-St-Northampton-MA-01060/121252390_zpid/</t>
         </is>
       </c>
+      <c r="G108" t="n">
+        <v>868600</v>
+      </c>
+      <c r="H108" t="n">
+        <v>717000</v>
+      </c>
+      <c r="I108" t="n">
+        <v>2024</v>
+      </c>
+      <c r="J108" t="inlineStr">
+        <is>
+          <t>2013-12-20</t>
+        </is>
+      </c>
+      <c r="K108" t="n">
+        <v>2020</v>
+      </c>
+      <c r="L108" t="n">
+        <v>2014</v>
+      </c>
+      <c r="M108" t="n">
+        <v>6534</v>
+      </c>
+      <c r="N108" t="inlineStr">
+        <is>
+          <t>Square Feet</t>
+        </is>
+      </c>
+      <c r="O108" t="inlineStr">
+        <is>
+          <t>Gas</t>
+        </is>
+      </c>
+      <c r="P108" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
     </row>
     <row r="109" ht="15.75" customHeight="1" s="19">
       <c r="A109" s="3" t="inlineStr">
@@ -7147,6 +7301,52 @@
           <t>https://www.zillow.com/homedetails/82-Rocky-Neck-Ave-A-Gloucester-MA-01930/2111229081_zpid/</t>
         </is>
       </c>
+      <c r="G109" t="n">
+        <v>626000</v>
+      </c>
+      <c r="H109" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="I109" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="J109" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="K109" t="n">
+        <v>1400</v>
+      </c>
+      <c r="L109" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="M109" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="N109" t="inlineStr">
+        <is>
+          <t>sqft</t>
+        </is>
+      </c>
+      <c r="O109" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="P109" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
     </row>
     <row r="110" ht="15.75" customHeight="1" s="19">
       <c r="A110" s="3" t="inlineStr">
@@ -7173,6 +7373,44 @@
           <t>https://www.zillow.com/homedetails/48-Gannett-Pasture-Ln-Scituate-MA-02066/57222367_zpid/</t>
         </is>
       </c>
+      <c r="G110" t="n">
+        <v>1129800</v>
+      </c>
+      <c r="H110" t="n">
+        <v>893500</v>
+      </c>
+      <c r="I110" t="n">
+        <v>2024</v>
+      </c>
+      <c r="J110" t="inlineStr">
+        <is>
+          <t>1993-12-17</t>
+        </is>
+      </c>
+      <c r="K110" t="n">
+        <v>2268</v>
+      </c>
+      <c r="L110" t="n">
+        <v>1994</v>
+      </c>
+      <c r="M110" t="n">
+        <v>4.529981634527089</v>
+      </c>
+      <c r="N110" t="inlineStr">
+        <is>
+          <t>Acres</t>
+        </is>
+      </c>
+      <c r="O110" t="inlineStr">
+        <is>
+          <t>Baseboard,Oil</t>
+        </is>
+      </c>
+      <c r="P110" t="inlineStr">
+        <is>
+          <t>Solar</t>
+        </is>
+      </c>
     </row>
     <row r="111" ht="15.75" customHeight="1" s="19">
       <c r="A111" s="3" t="inlineStr">
@@ -7197,6 +7435,44 @@
           <t>https://www.zillow.com/homedetails/183-Lincoln-Rd-Medford-MA-02155/56275377_zpid/</t>
         </is>
       </c>
+      <c r="G111" t="n">
+        <v>1012200</v>
+      </c>
+      <c r="H111" t="n">
+        <v>883900</v>
+      </c>
+      <c r="I111" t="n">
+        <v>2024</v>
+      </c>
+      <c r="J111" t="inlineStr">
+        <is>
+          <t>1999-09-02</t>
+        </is>
+      </c>
+      <c r="K111" t="n">
+        <v>2101</v>
+      </c>
+      <c r="L111" t="n">
+        <v>1920</v>
+      </c>
+      <c r="M111" t="n">
+        <v>8712</v>
+      </c>
+      <c r="N111" t="inlineStr">
+        <is>
+          <t>Square Feet</t>
+        </is>
+      </c>
+      <c r="O111" t="inlineStr">
+        <is>
+          <t>Other,Gas</t>
+        </is>
+      </c>
+      <c r="P111" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
     </row>
     <row r="112" ht="15.75" customHeight="1" s="19">
       <c r="A112" s="3" t="inlineStr">
@@ -7221,6 +7497,44 @@
           <t>https://www.zillow.com/homedetails/15-Milne-Rd-Osterville-MA-02655/55853966_zpid/</t>
         </is>
       </c>
+      <c r="G112" t="n">
+        <v>916400</v>
+      </c>
+      <c r="H112" t="n">
+        <v>627000</v>
+      </c>
+      <c r="I112" t="n">
+        <v>2024</v>
+      </c>
+      <c r="J112" t="inlineStr">
+        <is>
+          <t>2012-04-19</t>
+        </is>
+      </c>
+      <c r="K112" t="n">
+        <v>1316</v>
+      </c>
+      <c r="L112" t="n">
+        <v>1952</v>
+      </c>
+      <c r="M112" t="n">
+        <v>0.3899908172635445</v>
+      </c>
+      <c r="N112" t="inlineStr">
+        <is>
+          <t>Acres</t>
+        </is>
+      </c>
+      <c r="O112" t="inlineStr">
+        <is>
+          <t>Other,Gas</t>
+        </is>
+      </c>
+      <c r="P112" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
     </row>
     <row r="113" ht="15.75" customHeight="1" s="19">
       <c r="A113" s="3" t="inlineStr">
@@ -7247,6 +7561,44 @@
           <t>https://www.zillow.com/homedetails/4-Pershing-Rd-Needham-MA-02494/57479045_zpid/</t>
         </is>
       </c>
+      <c r="G113" t="n">
+        <v>1369100</v>
+      </c>
+      <c r="H113" t="n">
+        <v>1036900</v>
+      </c>
+      <c r="I113" t="n">
+        <v>2024</v>
+      </c>
+      <c r="J113" t="inlineStr">
+        <is>
+          <t>1989-11-22</t>
+        </is>
+      </c>
+      <c r="K113" t="n">
+        <v>2283</v>
+      </c>
+      <c r="L113" t="n">
+        <v>1951</v>
+      </c>
+      <c r="M113" t="n">
+        <v>8712</v>
+      </c>
+      <c r="N113" t="inlineStr">
+        <is>
+          <t>Square Feet</t>
+        </is>
+      </c>
+      <c r="O113" t="inlineStr">
+        <is>
+          <t>Solar</t>
+        </is>
+      </c>
+      <c r="P113" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
     </row>
     <row r="114" ht="15.75" customHeight="1" s="19">
       <c r="A114" s="3" t="inlineStr">
@@ -7273,6 +7625,44 @@
           <t>https://www.zillow.com/homedetails/55-Sheffield-Ln-Northampton-MA-01062/57020171_zpid/</t>
         </is>
       </c>
+      <c r="G114" t="n">
+        <v>633700</v>
+      </c>
+      <c r="H114" t="n">
+        <v>571700</v>
+      </c>
+      <c r="I114" t="n">
+        <v>2024</v>
+      </c>
+      <c r="J114" t="inlineStr">
+        <is>
+          <t>1989-12-04</t>
+        </is>
+      </c>
+      <c r="K114" t="n">
+        <v>1920</v>
+      </c>
+      <c r="L114" t="n">
+        <v>1960</v>
+      </c>
+      <c r="M114" t="n">
+        <v>0.2899908172635445</v>
+      </c>
+      <c r="N114" t="inlineStr">
+        <is>
+          <t>Acres</t>
+        </is>
+      </c>
+      <c r="O114" t="inlineStr">
+        <is>
+          <t>Forced air,Gas</t>
+        </is>
+      </c>
+      <c r="P114" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
     </row>
     <row r="115" ht="15.75" customHeight="1" s="19">
       <c r="A115" s="3" t="inlineStr">
@@ -7299,6 +7689,44 @@
           <t>https://www.zillow.com/homedetails/51-53-Oakland-St-Melrose-MA-02176/165805876_zpid/</t>
         </is>
       </c>
+      <c r="G115" t="n">
+        <v>1188700</v>
+      </c>
+      <c r="H115" t="n">
+        <v>832400</v>
+      </c>
+      <c r="I115" t="n">
+        <v>2024</v>
+      </c>
+      <c r="J115" t="inlineStr">
+        <is>
+          <t>1996-10-25</t>
+        </is>
+      </c>
+      <c r="K115" t="n">
+        <v>5230</v>
+      </c>
+      <c r="L115" t="n">
+        <v>1874</v>
+      </c>
+      <c r="M115" t="n">
+        <v>0.4099862258953168</v>
+      </c>
+      <c r="N115" t="inlineStr">
+        <is>
+          <t>Acres</t>
+        </is>
+      </c>
+      <c r="O115" t="inlineStr">
+        <is>
+          <t>Oil</t>
+        </is>
+      </c>
+      <c r="P115" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
     </row>
     <row r="116" ht="15.75" customHeight="1" s="19">
       <c r="A116" s="3" t="inlineStr">
@@ -7325,6 +7753,44 @@
           <t>https://www.zillow.com/homedetails/42-Wianno-Rd-Bourne-MA-02532/186977019_zpid/</t>
         </is>
       </c>
+      <c r="G116" t="n">
+        <v>1774900</v>
+      </c>
+      <c r="H116" t="n">
+        <v>1450200</v>
+      </c>
+      <c r="I116" t="n">
+        <v>2024</v>
+      </c>
+      <c r="J116" t="inlineStr">
+        <is>
+          <t>2001-04-02</t>
+        </is>
+      </c>
+      <c r="K116" t="n">
+        <v>1924</v>
+      </c>
+      <c r="L116" t="n">
+        <v>1973</v>
+      </c>
+      <c r="M116" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="N116" t="inlineStr">
+        <is>
+          <t>Acres</t>
+        </is>
+      </c>
+      <c r="O116" t="inlineStr">
+        <is>
+          <t>Gas</t>
+        </is>
+      </c>
+      <c r="P116" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
     </row>
     <row r="117" ht="15.75" customHeight="1" s="19">
       <c r="A117" s="3" t="inlineStr">
@@ -7351,6 +7817,44 @@
           <t>https://www.zillow.com/homedetails/16-Common-St-Brookfield-MA-01506/57571006_zpid/</t>
         </is>
       </c>
+      <c r="G117" t="n">
+        <v>352500</v>
+      </c>
+      <c r="H117" t="n">
+        <v>329500</v>
+      </c>
+      <c r="I117" t="n">
+        <v>2024</v>
+      </c>
+      <c r="J117" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="K117" t="n">
+        <v>2896</v>
+      </c>
+      <c r="L117" t="n">
+        <v>1910</v>
+      </c>
+      <c r="M117" t="n">
+        <v>0.35</v>
+      </c>
+      <c r="N117" t="inlineStr">
+        <is>
+          <t>Acres</t>
+        </is>
+      </c>
+      <c r="O117" t="inlineStr">
+        <is>
+          <t>Other,Oil</t>
+        </is>
+      </c>
+      <c r="P117" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
     </row>
     <row r="118" ht="15.75" customHeight="1" s="19">
       <c r="A118" s="3" t="inlineStr">
@@ -7377,6 +7881,44 @@
           <t>https://www.zillow.com/homedetails/235-Bay-Rd-Harwich-MA-02645/186996433_zpid/</t>
         </is>
       </c>
+      <c r="G118" t="n">
+        <v>1780500</v>
+      </c>
+      <c r="H118" t="n">
+        <v>1528200</v>
+      </c>
+      <c r="I118" t="n">
+        <v>2024</v>
+      </c>
+      <c r="J118" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="K118" t="n">
+        <v>2986</v>
+      </c>
+      <c r="L118" t="n">
+        <v>2008</v>
+      </c>
+      <c r="M118" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="N118" t="inlineStr">
+        <is>
+          <t>Acres</t>
+        </is>
+      </c>
+      <c r="O118" t="inlineStr">
+        <is>
+          <t>Gas</t>
+        </is>
+      </c>
+      <c r="P118" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
     </row>
     <row r="119" ht="15.75" customHeight="1" s="19">
       <c r="A119" s="3" t="inlineStr">
@@ -7401,6 +7943,44 @@
           <t>https://www.zillow.com/homedetails/183-Buckwood-Dr-Hyannis-MA-02601/55846204_zpid/</t>
         </is>
       </c>
+      <c r="G119" t="n">
+        <v>519700</v>
+      </c>
+      <c r="H119" t="n">
+        <v>401200</v>
+      </c>
+      <c r="I119" t="n">
+        <v>2024</v>
+      </c>
+      <c r="J119" t="inlineStr">
+        <is>
+          <t>2016-05-16</t>
+        </is>
+      </c>
+      <c r="K119" t="n">
+        <v>1032</v>
+      </c>
+      <c r="L119" t="n">
+        <v>1970</v>
+      </c>
+      <c r="M119" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="N119" t="inlineStr">
+        <is>
+          <t>Acres</t>
+        </is>
+      </c>
+      <c r="O119" t="inlineStr">
+        <is>
+          <t>Forced air,Gas</t>
+        </is>
+      </c>
+      <c r="P119" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
     </row>
     <row r="120" ht="15.75" customHeight="1" s="19">
       <c r="A120" s="3" t="inlineStr">
@@ -7427,6 +8007,44 @@
           <t>https://www.zillow.com/homedetails/35-Woodbury-St-Beverly-MA-01915/59225949_zpid/</t>
         </is>
       </c>
+      <c r="G120" t="n">
+        <v>1115800</v>
+      </c>
+      <c r="H120" t="n">
+        <v>891800</v>
+      </c>
+      <c r="I120" t="n">
+        <v>2024</v>
+      </c>
+      <c r="J120" t="inlineStr">
+        <is>
+          <t>1996-05-31</t>
+        </is>
+      </c>
+      <c r="K120" t="n">
+        <v>2127</v>
+      </c>
+      <c r="L120" t="n">
+        <v>1969</v>
+      </c>
+      <c r="M120" t="n">
+        <v>0.2599862258953168</v>
+      </c>
+      <c r="N120" t="inlineStr">
+        <is>
+          <t>Acres</t>
+        </is>
+      </c>
+      <c r="O120" t="inlineStr">
+        <is>
+          <t>Other,Gas</t>
+        </is>
+      </c>
+      <c r="P120" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
     </row>
     <row r="121" ht="15.75" customHeight="1" s="19">
       <c r="A121" s="3" t="inlineStr">
@@ -7451,6 +8069,44 @@
           <t>https://www.zillow.com/homedetails/36-Hill-St-Haverhill-MA-01832/56054458_zpid/</t>
         </is>
       </c>
+      <c r="G121" t="n">
+        <v>657700</v>
+      </c>
+      <c r="H121" t="n">
+        <v>514700</v>
+      </c>
+      <c r="I121" t="n">
+        <v>2024</v>
+      </c>
+      <c r="J121" t="inlineStr">
+        <is>
+          <t>1999-01-08</t>
+        </is>
+      </c>
+      <c r="K121" t="n">
+        <v>1800</v>
+      </c>
+      <c r="L121" t="n">
+        <v>1999</v>
+      </c>
+      <c r="M121" t="n">
+        <v>0.3443985307621671</v>
+      </c>
+      <c r="N121" t="inlineStr">
+        <is>
+          <t>Acres</t>
+        </is>
+      </c>
+      <c r="O121" t="inlineStr">
+        <is>
+          <t>Forced air,Gas</t>
+        </is>
+      </c>
+      <c r="P121" t="inlineStr">
+        <is>
+          <t>Central</t>
+        </is>
+      </c>
     </row>
     <row r="122" ht="15.75" customHeight="1" s="19">
       <c r="A122" s="3" t="inlineStr">
@@ -7477,6 +8133,46 @@
           <t>https://www.zillow.com/homedetails/27-Hawthorne-Ave-Arlington-MA-02476/56403359_zpid/</t>
         </is>
       </c>
+      <c r="G122" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="H122" t="n">
+        <v>833100</v>
+      </c>
+      <c r="I122" t="n">
+        <v>2024</v>
+      </c>
+      <c r="J122" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="K122" t="n">
+        <v>1284</v>
+      </c>
+      <c r="L122" t="n">
+        <v>1930</v>
+      </c>
+      <c r="M122" t="n">
+        <v>5662</v>
+      </c>
+      <c r="N122" t="inlineStr">
+        <is>
+          <t>Square Feet</t>
+        </is>
+      </c>
+      <c r="O122" t="inlineStr">
+        <is>
+          <t>Other,Gas</t>
+        </is>
+      </c>
+      <c r="P122" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
     </row>
     <row r="123" ht="15.75" customHeight="1" s="19">
       <c r="A123" s="3" t="inlineStr">
@@ -7503,6 +8199,44 @@
           <t>https://www.zillow.com/homedetails/98-Prescott-Rd-Concord-MA-01742/166022245_zpid/</t>
         </is>
       </c>
+      <c r="G123" t="n">
+        <v>942000</v>
+      </c>
+      <c r="H123" t="n">
+        <v>791400</v>
+      </c>
+      <c r="I123" t="n">
+        <v>2024</v>
+      </c>
+      <c r="J123" t="inlineStr">
+        <is>
+          <t>2004-09-03</t>
+        </is>
+      </c>
+      <c r="K123" t="n">
+        <v>1144</v>
+      </c>
+      <c r="L123" t="n">
+        <v>1953</v>
+      </c>
+      <c r="M123" t="n">
+        <v>0.6399908172635446</v>
+      </c>
+      <c r="N123" t="inlineStr">
+        <is>
+          <t>Acres</t>
+        </is>
+      </c>
+      <c r="O123" t="inlineStr">
+        <is>
+          <t>Oil</t>
+        </is>
+      </c>
+      <c r="P123" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
     </row>
     <row r="124" ht="15.75" customHeight="1" s="19">
       <c r="A124" s="3" t="inlineStr">
@@ -7529,6 +8263,44 @@
           <t>https://www.zillow.com/homedetails/2-Candida-Ln-Acton-MA-01720/57035751_zpid/</t>
         </is>
       </c>
+      <c r="G124" t="n">
+        <v>1251700</v>
+      </c>
+      <c r="H124" t="n">
+        <v>1014100</v>
+      </c>
+      <c r="I124" t="n">
+        <v>2024</v>
+      </c>
+      <c r="J124" t="inlineStr">
+        <is>
+          <t>1999-06-16</t>
+        </is>
+      </c>
+      <c r="K124" t="n">
+        <v>2692</v>
+      </c>
+      <c r="L124" t="n">
+        <v>1988</v>
+      </c>
+      <c r="M124" t="n">
+        <v>1.769995408631772</v>
+      </c>
+      <c r="N124" t="inlineStr">
+        <is>
+          <t>Acres</t>
+        </is>
+      </c>
+      <c r="O124" t="inlineStr">
+        <is>
+          <t>Forced air,Oil,Other</t>
+        </is>
+      </c>
+      <c r="P124" t="inlineStr">
+        <is>
+          <t>Central</t>
+        </is>
+      </c>
     </row>
     <row r="125" ht="15.75" customHeight="1" s="19">
       <c r="A125" s="3" t="inlineStr">
@@ -7555,6 +8327,44 @@
           <t>https://www.zillow.com/homedetails/11-Mary-Chilton-Rd-Needham-MA-02492/57480236_zpid/</t>
         </is>
       </c>
+      <c r="G125" t="n">
+        <v>1218600</v>
+      </c>
+      <c r="H125" t="n">
+        <v>869800</v>
+      </c>
+      <c r="I125" t="n">
+        <v>2024</v>
+      </c>
+      <c r="J125" t="inlineStr">
+        <is>
+          <t>2000-07-19</t>
+        </is>
+      </c>
+      <c r="K125" t="n">
+        <v>1640</v>
+      </c>
+      <c r="L125" t="n">
+        <v>1982</v>
+      </c>
+      <c r="M125" t="n">
+        <v>10018</v>
+      </c>
+      <c r="N125" t="inlineStr">
+        <is>
+          <t>Square Feet</t>
+        </is>
+      </c>
+      <c r="O125" t="inlineStr">
+        <is>
+          <t>Other,Gas</t>
+        </is>
+      </c>
+      <c r="P125" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
     </row>
     <row r="126" ht="15.75" customHeight="1" s="19">
       <c r="A126" s="3" t="inlineStr">
@@ -7581,6 +8391,44 @@
           <t>https://www.zillow.com/homedetails/42-Birchtree-Dr-Westwood-MA-02090/57516342_zpid/</t>
         </is>
       </c>
+      <c r="G126" t="n">
+        <v>1364400</v>
+      </c>
+      <c r="H126" t="n">
+        <v>1064400</v>
+      </c>
+      <c r="I126" t="n">
+        <v>2024</v>
+      </c>
+      <c r="J126" t="inlineStr">
+        <is>
+          <t>2005-04-06</t>
+        </is>
+      </c>
+      <c r="K126" t="n">
+        <v>2336</v>
+      </c>
+      <c r="L126" t="n">
+        <v>1950</v>
+      </c>
+      <c r="M126" t="n">
+        <v>0.85</v>
+      </c>
+      <c r="N126" t="inlineStr">
+        <is>
+          <t>Acres</t>
+        </is>
+      </c>
+      <c r="O126" t="inlineStr">
+        <is>
+          <t>Other,Oil</t>
+        </is>
+      </c>
+      <c r="P126" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
     </row>
     <row r="127" ht="15.75" customHeight="1" s="19">
       <c r="A127" s="3" t="inlineStr">
@@ -7607,6 +8455,44 @@
           <t>https://www.zillow.com/homedetails/279-Davis-St-Northborough-MA-01532/57625738_zpid/</t>
         </is>
       </c>
+      <c r="G127" t="n">
+        <v>892100</v>
+      </c>
+      <c r="H127" t="n">
+        <v>666300</v>
+      </c>
+      <c r="I127" t="n">
+        <v>2024</v>
+      </c>
+      <c r="J127" t="inlineStr">
+        <is>
+          <t>2011-06-29</t>
+        </is>
+      </c>
+      <c r="K127" t="n">
+        <v>2200</v>
+      </c>
+      <c r="L127" t="n">
+        <v>1984</v>
+      </c>
+      <c r="M127" t="n">
+        <v>0.9799816345270891</v>
+      </c>
+      <c r="N127" t="inlineStr">
+        <is>
+          <t>Acres</t>
+        </is>
+      </c>
+      <c r="O127" t="inlineStr">
+        <is>
+          <t>Other,Gas</t>
+        </is>
+      </c>
+      <c r="P127" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
     </row>
     <row r="128" ht="15.75" customHeight="1" s="19">
       <c r="A128" s="3" t="inlineStr">
@@ -7633,6 +8519,44 @@
           <t>https://www.zillow.com/homedetails/32-Oak-Knoll-Dr-Hampden-MA-01036/56173214_zpid/</t>
         </is>
       </c>
+      <c r="G128" t="n">
+        <v>391500</v>
+      </c>
+      <c r="H128" t="n">
+        <v>311800</v>
+      </c>
+      <c r="I128" t="n">
+        <v>2024</v>
+      </c>
+      <c r="J128" t="inlineStr">
+        <is>
+          <t>2014-10-31</t>
+        </is>
+      </c>
+      <c r="K128" t="n">
+        <v>1348</v>
+      </c>
+      <c r="L128" t="n">
+        <v>1964</v>
+      </c>
+      <c r="M128" t="n">
+        <v>1.75</v>
+      </c>
+      <c r="N128" t="inlineStr">
+        <is>
+          <t>Acres</t>
+        </is>
+      </c>
+      <c r="O128" t="inlineStr">
+        <is>
+          <t>Baseboard,Stove,Gas</t>
+        </is>
+      </c>
+      <c r="P128" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
     </row>
     <row r="129" ht="15.75" customHeight="1" s="19">
       <c r="A129" s="3" t="inlineStr">
@@ -7659,6 +8583,44 @@
           <t>https://www.zillow.com/homedetails/49-Ford-Xing-Northampton-MA-01060/246300174_zpid/</t>
         </is>
       </c>
+      <c r="G129" t="n">
+        <v>797800</v>
+      </c>
+      <c r="H129" t="n">
+        <v>706900</v>
+      </c>
+      <c r="I129" t="n">
+        <v>2024</v>
+      </c>
+      <c r="J129" t="inlineStr">
+        <is>
+          <t>2019-04-25</t>
+        </is>
+      </c>
+      <c r="K129" t="n">
+        <v>2238</v>
+      </c>
+      <c r="L129" t="n">
+        <v>2017</v>
+      </c>
+      <c r="M129" t="n">
+        <v>4356</v>
+      </c>
+      <c r="N129" t="inlineStr">
+        <is>
+          <t>Square Feet</t>
+        </is>
+      </c>
+      <c r="O129" t="inlineStr">
+        <is>
+          <t>Gas</t>
+        </is>
+      </c>
+      <c r="P129" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
     </row>
     <row r="130" ht="15.75" customHeight="1" s="19">
       <c r="A130" s="3" t="inlineStr">
@@ -7685,6 +8647,44 @@
           <t>https://www.zillow.com/homedetails/15-Grandview-Rd-Haverhill-MA-01832/56054467_zpid/</t>
         </is>
       </c>
+      <c r="G130" t="n">
+        <v>518700</v>
+      </c>
+      <c r="H130" t="n">
+        <v>402900</v>
+      </c>
+      <c r="I130" t="n">
+        <v>2024</v>
+      </c>
+      <c r="J130" t="inlineStr">
+        <is>
+          <t>2004-06-22</t>
+        </is>
+      </c>
+      <c r="K130" t="n">
+        <v>1292</v>
+      </c>
+      <c r="L130" t="n">
+        <v>1969</v>
+      </c>
+      <c r="M130" t="n">
+        <v>9600</v>
+      </c>
+      <c r="N130" t="inlineStr">
+        <is>
+          <t>Square Feet</t>
+        </is>
+      </c>
+      <c r="O130" t="inlineStr">
+        <is>
+          <t>Other,Oil</t>
+        </is>
+      </c>
+      <c r="P130" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
     </row>
     <row r="131" ht="15.75" customHeight="1" s="19">
       <c r="A131" s="3" t="inlineStr">
@@ -7711,6 +8711,44 @@
           <t>https://www.zillow.com/homedetails/143-Holden-Wood-Rd-Concord-MA-01742/166020986_zpid/</t>
         </is>
       </c>
+      <c r="G131" t="n">
+        <v>1516700</v>
+      </c>
+      <c r="H131" t="n">
+        <v>1231700</v>
+      </c>
+      <c r="I131" t="n">
+        <v>2024</v>
+      </c>
+      <c r="J131" t="inlineStr">
+        <is>
+          <t>1993-02-26</t>
+        </is>
+      </c>
+      <c r="K131" t="n">
+        <v>2785</v>
+      </c>
+      <c r="L131" t="n">
+        <v>1952</v>
+      </c>
+      <c r="M131" t="n">
+        <v>1.009986225895317</v>
+      </c>
+      <c r="N131" t="inlineStr">
+        <is>
+          <t>Acres</t>
+        </is>
+      </c>
+      <c r="O131" t="inlineStr">
+        <is>
+          <t>Oil</t>
+        </is>
+      </c>
+      <c r="P131" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
     </row>
     <row r="132" ht="15.75" customHeight="1" s="19">
       <c r="A132" s="3" t="inlineStr">
@@ -7737,6 +8775,44 @@
           <t>https://www.zillow.com/homedetails/117-Park-Rd-Chelmsford-MA-01824/56452429_zpid/</t>
         </is>
       </c>
+      <c r="G132" t="n">
+        <v>1179900</v>
+      </c>
+      <c r="H132" t="n">
+        <v>969900</v>
+      </c>
+      <c r="I132" t="n">
+        <v>2024</v>
+      </c>
+      <c r="J132" t="inlineStr">
+        <is>
+          <t>2005-07-22</t>
+        </is>
+      </c>
+      <c r="K132" t="n">
+        <v>2664</v>
+      </c>
+      <c r="L132" t="n">
+        <v>1993</v>
+      </c>
+      <c r="M132" t="n">
+        <v>0.932277318640955</v>
+      </c>
+      <c r="N132" t="inlineStr">
+        <is>
+          <t>Acres</t>
+        </is>
+      </c>
+      <c r="O132" t="inlineStr">
+        <is>
+          <t>Forced air,Gas</t>
+        </is>
+      </c>
+      <c r="P132" t="inlineStr">
+        <is>
+          <t>Central</t>
+        </is>
+      </c>
     </row>
     <row r="133" ht="15.75" customHeight="1" s="19">
       <c r="A133" s="3" t="inlineStr">
@@ -7763,6 +8839,44 @@
           <t>https://www.zillow.com/homedetails/177-Monsen-Rd-Concord-MA-01742/166021937_zpid/</t>
         </is>
       </c>
+      <c r="G133" t="n">
+        <v>1487400</v>
+      </c>
+      <c r="H133" t="n">
+        <v>1103200</v>
+      </c>
+      <c r="I133" t="n">
+        <v>2024</v>
+      </c>
+      <c r="J133" t="inlineStr">
+        <is>
+          <t>2011-12-09</t>
+        </is>
+      </c>
+      <c r="K133" t="n">
+        <v>2856</v>
+      </c>
+      <c r="L133" t="n">
+        <v>1955</v>
+      </c>
+      <c r="M133" t="n">
+        <v>0.6791322314049587</v>
+      </c>
+      <c r="N133" t="inlineStr">
+        <is>
+          <t>Acres</t>
+        </is>
+      </c>
+      <c r="O133" t="inlineStr">
+        <is>
+          <t>Forced air,Propane / Butane</t>
+        </is>
+      </c>
+      <c r="P133" t="inlineStr">
+        <is>
+          <t>Central</t>
+        </is>
+      </c>
     </row>
     <row r="134" ht="15.75" customHeight="1" s="19">
       <c r="A134" s="3" t="inlineStr">
@@ -7789,6 +8903,44 @@
           <t>https://www.zillow.com/homedetails/6-Sutton-Pl-Acton-MA-01720/57031615_zpid/</t>
         </is>
       </c>
+      <c r="G134" t="n">
+        <v>2647500</v>
+      </c>
+      <c r="H134" t="n">
+        <v>1528300</v>
+      </c>
+      <c r="I134" t="n">
+        <v>2024</v>
+      </c>
+      <c r="J134" t="inlineStr">
+        <is>
+          <t>2021-05-13</t>
+        </is>
+      </c>
+      <c r="K134" t="n">
+        <v>8229</v>
+      </c>
+      <c r="L134" t="n">
+        <v>1983</v>
+      </c>
+      <c r="M134" t="n">
+        <v>4.179981634527089</v>
+      </c>
+      <c r="N134" t="inlineStr">
+        <is>
+          <t>Acres</t>
+        </is>
+      </c>
+      <c r="O134" t="inlineStr">
+        <is>
+          <t>Forced air,Radiant,Propane / Butane</t>
+        </is>
+      </c>
+      <c r="P134" t="inlineStr">
+        <is>
+          <t>Central</t>
+        </is>
+      </c>
     </row>
     <row r="135" ht="15.75" customHeight="1" s="19">
       <c r="A135" s="3" t="inlineStr">
@@ -7813,6 +8965,44 @@
           <t>https://www.zillow.com/homedetails/286-College-Farm-Rd-Waltham-MA-02451/56358789_zpid/</t>
         </is>
       </c>
+      <c r="G135" t="n">
+        <v>773600</v>
+      </c>
+      <c r="H135" t="n">
+        <v>573600</v>
+      </c>
+      <c r="I135" t="n">
+        <v>2024</v>
+      </c>
+      <c r="J135" t="inlineStr">
+        <is>
+          <t>2020-10-16</t>
+        </is>
+      </c>
+      <c r="K135" t="n">
+        <v>1430</v>
+      </c>
+      <c r="L135" t="n">
+        <v>1940</v>
+      </c>
+      <c r="M135" t="n">
+        <v>10454</v>
+      </c>
+      <c r="N135" t="inlineStr">
+        <is>
+          <t>Square Feet</t>
+        </is>
+      </c>
+      <c r="O135" t="inlineStr">
+        <is>
+          <t>Forced air,Gas</t>
+        </is>
+      </c>
+      <c r="P135" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
     </row>
     <row r="136" ht="15.75" customHeight="1" s="19">
       <c r="A136" s="3" t="inlineStr">
@@ -7837,6 +9027,44 @@
           <t>https://www.zillow.com/homedetails/1-Wade-Rd-Plainville-MA-02762/57492677_zpid/</t>
         </is>
       </c>
+      <c r="G136" t="n">
+        <v>676800</v>
+      </c>
+      <c r="H136" t="n">
+        <v>454800</v>
+      </c>
+      <c r="I136" t="n">
+        <v>2024</v>
+      </c>
+      <c r="J136" t="inlineStr">
+        <is>
+          <t>2022-07-22</t>
+        </is>
+      </c>
+      <c r="K136" t="n">
+        <v>2205</v>
+      </c>
+      <c r="L136" t="n">
+        <v>1955</v>
+      </c>
+      <c r="M136" t="n">
+        <v>0.36</v>
+      </c>
+      <c r="N136" t="inlineStr">
+        <is>
+          <t>Acres</t>
+        </is>
+      </c>
+      <c r="O136" t="inlineStr">
+        <is>
+          <t>Forced Air,Oil</t>
+        </is>
+      </c>
+      <c r="P136" t="inlineStr">
+        <is>
+          <t>Central Air</t>
+        </is>
+      </c>
     </row>
     <row r="137" ht="15.75" customHeight="1" s="19">
       <c r="A137" s="3" t="inlineStr">
@@ -7861,6 +9089,44 @@
           <t>https://www.zillow.com/homedetails/34-Shannon-Way-Dartmouth-MA-02747/59880382_zpid/</t>
         </is>
       </c>
+      <c r="G137" t="n">
+        <v>587500</v>
+      </c>
+      <c r="H137" t="n">
+        <v>470100</v>
+      </c>
+      <c r="I137" t="n">
+        <v>2024</v>
+      </c>
+      <c r="J137" t="inlineStr">
+        <is>
+          <t>2001-10-02</t>
+        </is>
+      </c>
+      <c r="K137" t="n">
+        <v>1768</v>
+      </c>
+      <c r="L137" t="n">
+        <v>2001</v>
+      </c>
+      <c r="M137" t="n">
+        <v>0.9399908172635445</v>
+      </c>
+      <c r="N137" t="inlineStr">
+        <is>
+          <t>Acres</t>
+        </is>
+      </c>
+      <c r="O137" t="inlineStr">
+        <is>
+          <t>Other,Oil</t>
+        </is>
+      </c>
+      <c r="P137" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
     </row>
     <row r="138" ht="15.75" customHeight="1" s="19">
       <c r="A138" s="3" t="inlineStr">
@@ -7887,6 +9153,44 @@
           <t>https://www.zillow.com/homedetails/13-Secluded-Rdg-Southwick-MA-01077/56996781_zpid/</t>
         </is>
       </c>
+      <c r="G138" t="n">
+        <v>634700</v>
+      </c>
+      <c r="H138" t="n">
+        <v>549800</v>
+      </c>
+      <c r="I138" t="n">
+        <v>2024</v>
+      </c>
+      <c r="J138" t="inlineStr">
+        <is>
+          <t>2010-11-19</t>
+        </is>
+      </c>
+      <c r="K138" t="n">
+        <v>3023</v>
+      </c>
+      <c r="L138" t="n">
+        <v>1997</v>
+      </c>
+      <c r="M138" t="n">
+        <v>1.260238751147842</v>
+      </c>
+      <c r="N138" t="inlineStr">
+        <is>
+          <t>Acres</t>
+        </is>
+      </c>
+      <c r="O138" t="inlineStr">
+        <is>
+          <t>Forced air,Oil</t>
+        </is>
+      </c>
+      <c r="P138" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
     </row>
     <row r="139" ht="15.75" customHeight="1" s="19">
       <c r="A139" s="3" t="inlineStr">
@@ -7911,6 +9215,44 @@
           <t>https://www.zillow.com/homedetails/23-Powell-St-Northampton-MA-01062/57020013_zpid/</t>
         </is>
       </c>
+      <c r="G139" t="n">
+        <v>521400</v>
+      </c>
+      <c r="H139" t="n">
+        <v>389300</v>
+      </c>
+      <c r="I139" t="n">
+        <v>2024</v>
+      </c>
+      <c r="J139" t="inlineStr">
+        <is>
+          <t>2014-07-31</t>
+        </is>
+      </c>
+      <c r="K139" t="n">
+        <v>1506</v>
+      </c>
+      <c r="L139" t="n">
+        <v>1900</v>
+      </c>
+      <c r="M139" t="n">
+        <v>0.4199954086317723</v>
+      </c>
+      <c r="N139" t="inlineStr">
+        <is>
+          <t>Acres</t>
+        </is>
+      </c>
+      <c r="O139" t="inlineStr">
+        <is>
+          <t>Forced air,Gas</t>
+        </is>
+      </c>
+      <c r="P139" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
     </row>
     <row r="140" ht="15.75" customHeight="1" s="19">
       <c r="A140" s="3" t="inlineStr">
@@ -7935,6 +9277,44 @@
           <t>https://www.zillow.com/homedetails/4-Sheeps-Crossing-Ln-Falmouth-MA-02543/55898730_zpid/</t>
         </is>
       </c>
+      <c r="G140" t="n">
+        <v>1137800</v>
+      </c>
+      <c r="H140" t="n">
+        <v>943100</v>
+      </c>
+      <c r="I140" t="n">
+        <v>2024</v>
+      </c>
+      <c r="J140" t="inlineStr">
+        <is>
+          <t>1995-03-09</t>
+        </is>
+      </c>
+      <c r="K140" t="n">
+        <v>2221</v>
+      </c>
+      <c r="L140" t="n">
+        <v>1846</v>
+      </c>
+      <c r="M140" t="n">
+        <v>0.9399908172635445</v>
+      </c>
+      <c r="N140" t="inlineStr">
+        <is>
+          <t>Acres</t>
+        </is>
+      </c>
+      <c r="O140" t="inlineStr">
+        <is>
+          <t>Other,Gas</t>
+        </is>
+      </c>
+      <c r="P140" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
     </row>
     <row r="141" ht="15.75" customHeight="1" s="19">
       <c r="A141" s="3" t="inlineStr">
@@ -7961,6 +9341,44 @@
           <t>https://www.zillow.com/homedetails/7-Pheasant-Ln-Topsfield-MA-01983/56969630_zpid/</t>
         </is>
       </c>
+      <c r="G141" t="n">
+        <v>1232600</v>
+      </c>
+      <c r="H141" t="n">
+        <v>1018500</v>
+      </c>
+      <c r="I141" t="n">
+        <v>2024</v>
+      </c>
+      <c r="J141" t="inlineStr">
+        <is>
+          <t>2012-06-08</t>
+        </is>
+      </c>
+      <c r="K141" t="n">
+        <v>3768</v>
+      </c>
+      <c r="L141" t="n">
+        <v>1987</v>
+      </c>
+      <c r="M141" t="n">
+        <v>1</v>
+      </c>
+      <c r="N141" t="inlineStr">
+        <is>
+          <t>Acres</t>
+        </is>
+      </c>
+      <c r="O141" t="inlineStr">
+        <is>
+          <t>Forced air,Oil</t>
+        </is>
+      </c>
+      <c r="P141" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
     </row>
     <row r="142" ht="15.75" customHeight="1" s="19">
       <c r="A142" s="3" t="inlineStr">
@@ -7987,6 +9405,44 @@
           <t>https://www.zillow.com/homedetails/336-Station-Rd-Amherst-MA-01002/56258370_zpid/</t>
         </is>
       </c>
+      <c r="G142" t="n">
+        <v>780000</v>
+      </c>
+      <c r="H142" t="n">
+        <v>693600</v>
+      </c>
+      <c r="I142" t="n">
+        <v>2024</v>
+      </c>
+      <c r="J142" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="K142" t="n">
+        <v>3078</v>
+      </c>
+      <c r="L142" t="n">
+        <v>1994</v>
+      </c>
+      <c r="M142" t="n">
+        <v>2.65</v>
+      </c>
+      <c r="N142" t="inlineStr">
+        <is>
+          <t>Acres</t>
+        </is>
+      </c>
+      <c r="O142" t="inlineStr">
+        <is>
+          <t>Forced air,Oil</t>
+        </is>
+      </c>
+      <c r="P142" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
     </row>
     <row r="143" ht="15.75" customHeight="1" s="19">
       <c r="A143" s="3" t="inlineStr">
@@ -8011,6 +9467,44 @@
           <t>https://www.zillow.com/homedetails/14-Mount-Walley-Rd-Waltham-MA-02451/56359215_zpid/</t>
         </is>
       </c>
+      <c r="G143" t="n">
+        <v>653200</v>
+      </c>
+      <c r="H143" t="n">
+        <v>509600</v>
+      </c>
+      <c r="I143" t="n">
+        <v>2024</v>
+      </c>
+      <c r="J143" t="inlineStr">
+        <is>
+          <t>2021-11-22</t>
+        </is>
+      </c>
+      <c r="K143" t="n">
+        <v>1000</v>
+      </c>
+      <c r="L143" t="n">
+        <v>1955</v>
+      </c>
+      <c r="M143" t="n">
+        <v>3484</v>
+      </c>
+      <c r="N143" t="inlineStr">
+        <is>
+          <t>Square Feet</t>
+        </is>
+      </c>
+      <c r="O143" t="inlineStr">
+        <is>
+          <t>Other,Oil</t>
+        </is>
+      </c>
+      <c r="P143" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
     </row>
     <row r="144" ht="15.75" customHeight="1" s="19">
       <c r="A144" s="3" t="inlineStr">
@@ -8037,6 +9531,44 @@
           <t>https://www.zillow.com/homedetails/10-Aloha-Dr-Hadley-MA-01035/57015527_zpid/</t>
         </is>
       </c>
+      <c r="G144" t="n">
+        <v>549100</v>
+      </c>
+      <c r="H144" t="n">
+        <v>437800</v>
+      </c>
+      <c r="I144" t="n">
+        <v>2024</v>
+      </c>
+      <c r="J144" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="K144" t="n">
+        <v>2000</v>
+      </c>
+      <c r="L144" t="n">
+        <v>1986</v>
+      </c>
+      <c r="M144" t="n">
+        <v>0.5099862258953168</v>
+      </c>
+      <c r="N144" t="inlineStr">
+        <is>
+          <t>Acres</t>
+        </is>
+      </c>
+      <c r="O144" t="inlineStr">
+        <is>
+          <t>Other,Oil</t>
+        </is>
+      </c>
+      <c r="P144" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
     </row>
     <row r="145" ht="15.75" customHeight="1" s="19">
       <c r="A145" s="3" t="inlineStr">
@@ -8061,6 +9593,44 @@
           <t>https://www.zillow.com/homedetails/18-Mount-Ida-Ter-Waltham-MA-02451/56359233_zpid/</t>
         </is>
       </c>
+      <c r="G145" t="n">
+        <v>646300</v>
+      </c>
+      <c r="H145" t="n">
+        <v>496600</v>
+      </c>
+      <c r="I145" t="n">
+        <v>2024</v>
+      </c>
+      <c r="J145" t="inlineStr">
+        <is>
+          <t>2017-05-23</t>
+        </is>
+      </c>
+      <c r="K145" t="n">
+        <v>912</v>
+      </c>
+      <c r="L145" t="n">
+        <v>1952</v>
+      </c>
+      <c r="M145" t="n">
+        <v>3920</v>
+      </c>
+      <c r="N145" t="inlineStr">
+        <is>
+          <t>Square Feet</t>
+        </is>
+      </c>
+      <c r="O145" t="inlineStr">
+        <is>
+          <t>Other,Oil</t>
+        </is>
+      </c>
+      <c r="P145" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
     </row>
     <row r="146" ht="15.75" customHeight="1" s="19">
       <c r="A146" s="3" t="inlineStr">
@@ -8085,6 +9655,44 @@
           <t>https://www.zillow.com/homedetails/7-Oak-Ridge-Rd-East-Falmouth-MA-02536/55891673_zpid/</t>
         </is>
       </c>
+      <c r="G146" t="n">
+        <v>741600</v>
+      </c>
+      <c r="H146" t="n">
+        <v>567000</v>
+      </c>
+      <c r="I146" t="n">
+        <v>2024</v>
+      </c>
+      <c r="J146" t="inlineStr">
+        <is>
+          <t>2012-06-08</t>
+        </is>
+      </c>
+      <c r="K146" t="n">
+        <v>1684</v>
+      </c>
+      <c r="L146" t="n">
+        <v>1973</v>
+      </c>
+      <c r="M146" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="N146" t="inlineStr">
+        <is>
+          <t>Acres</t>
+        </is>
+      </c>
+      <c r="O146" t="inlineStr">
+        <is>
+          <t>Other,Gas</t>
+        </is>
+      </c>
+      <c r="P146" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
     </row>
     <row r="147" ht="15.75" customHeight="1" s="19">
       <c r="A147" s="3" t="inlineStr">
@@ -8109,6 +9717,44 @@
           <t>https://www.zillow.com/homedetails/175-Shepardson-Rd-Warwick-MA-01378/56987841_zpid/</t>
         </is>
       </c>
+      <c r="G147" t="n">
+        <v>412000</v>
+      </c>
+      <c r="H147" t="n">
+        <v>333000</v>
+      </c>
+      <c r="I147" t="n">
+        <v>2024</v>
+      </c>
+      <c r="J147" t="inlineStr">
+        <is>
+          <t>2022-09-15</t>
+        </is>
+      </c>
+      <c r="K147" t="n">
+        <v>1680</v>
+      </c>
+      <c r="L147" t="n">
+        <v>1988</v>
+      </c>
+      <c r="M147" t="n">
+        <v>3.1</v>
+      </c>
+      <c r="N147" t="inlineStr">
+        <is>
+          <t>Acres</t>
+        </is>
+      </c>
+      <c r="O147" t="inlineStr">
+        <is>
+          <t>Baseboard,Oil,Wood,Wood Stove</t>
+        </is>
+      </c>
+      <c r="P147" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
     </row>
     <row r="148" ht="15.75" customHeight="1" s="19">
       <c r="A148" s="3" t="inlineStr">
@@ -8133,6 +9779,44 @@
           <t>https://www.zillow.com/homedetails/33-Hill-St-Haverhill-MA-01832/56054482_zpid/</t>
         </is>
       </c>
+      <c r="G148" t="n">
+        <v>632700</v>
+      </c>
+      <c r="H148" t="n">
+        <v>483500</v>
+      </c>
+      <c r="I148" t="n">
+        <v>2024</v>
+      </c>
+      <c r="J148" t="inlineStr">
+        <is>
+          <t>2003-07-11</t>
+        </is>
+      </c>
+      <c r="K148" t="n">
+        <v>1632</v>
+      </c>
+      <c r="L148" t="n">
+        <v>1998</v>
+      </c>
+      <c r="M148" t="n">
+        <v>0.328305785123967</v>
+      </c>
+      <c r="N148" t="inlineStr">
+        <is>
+          <t>Acres</t>
+        </is>
+      </c>
+      <c r="O148" t="inlineStr">
+        <is>
+          <t>Baseboard,Gas</t>
+        </is>
+      </c>
+      <c r="P148" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
     </row>
     <row r="149" ht="15.75" customHeight="1" s="19">
       <c r="A149" s="3" t="inlineStr">
@@ -8157,6 +9841,44 @@
           <t>https://www.zillow.com/homedetails/6-Pine-Ave-Tyngsboro-MA-01879/57122748_zpid/</t>
         </is>
       </c>
+      <c r="G149" t="n">
+        <v>640800</v>
+      </c>
+      <c r="H149" t="n">
+        <v>517100</v>
+      </c>
+      <c r="I149" t="n">
+        <v>2024</v>
+      </c>
+      <c r="J149" t="inlineStr">
+        <is>
+          <t>2010-09-15</t>
+        </is>
+      </c>
+      <c r="K149" t="n">
+        <v>2376</v>
+      </c>
+      <c r="L149" t="n">
+        <v>1983</v>
+      </c>
+      <c r="M149" t="n">
+        <v>1</v>
+      </c>
+      <c r="N149" t="inlineStr">
+        <is>
+          <t>Acres</t>
+        </is>
+      </c>
+      <c r="O149" t="inlineStr">
+        <is>
+          <t>Forced air,Gas</t>
+        </is>
+      </c>
+      <c r="P149" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
     </row>
     <row r="150" ht="15.75" customHeight="1" s="19">
       <c r="A150" s="3" t="inlineStr">
@@ -8181,6 +9903,44 @@
           <t>https://www.zillow.com/homedetails/12-Barbara-Cir-Burlington-MA-01803/57056333_zpid/</t>
         </is>
       </c>
+      <c r="G150" t="n">
+        <v>815500</v>
+      </c>
+      <c r="H150" t="n">
+        <v>585000</v>
+      </c>
+      <c r="I150" t="n">
+        <v>2024</v>
+      </c>
+      <c r="J150" t="inlineStr">
+        <is>
+          <t>2019-10-18</t>
+        </is>
+      </c>
+      <c r="K150" t="n">
+        <v>1800</v>
+      </c>
+      <c r="L150" t="n">
+        <v>1970</v>
+      </c>
+      <c r="M150" t="n">
+        <v>0.4899908172635445</v>
+      </c>
+      <c r="N150" t="inlineStr">
+        <is>
+          <t>Acres</t>
+        </is>
+      </c>
+      <c r="O150" t="inlineStr">
+        <is>
+          <t>Forced air,Gas</t>
+        </is>
+      </c>
+      <c r="P150" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
     </row>
     <row r="151" ht="15.75" customHeight="1" s="19">
       <c r="A151" s="3" t="inlineStr">
@@ -8205,6 +9965,44 @@
           <t>https://www.zillow.com/homedetails/52-Stickney-Rd-Medford-MA-02155/56275415_zpid/</t>
         </is>
       </c>
+      <c r="G151" t="n">
+        <v>954000</v>
+      </c>
+      <c r="H151" t="n">
+        <v>777300</v>
+      </c>
+      <c r="I151" t="n">
+        <v>2024</v>
+      </c>
+      <c r="J151" t="inlineStr">
+        <is>
+          <t>2020-10-28</t>
+        </is>
+      </c>
+      <c r="K151" t="n">
+        <v>1316</v>
+      </c>
+      <c r="L151" t="n">
+        <v>1945</v>
+      </c>
+      <c r="M151" t="n">
+        <v>6969</v>
+      </c>
+      <c r="N151" t="inlineStr">
+        <is>
+          <t>Square Feet</t>
+        </is>
+      </c>
+      <c r="O151" t="inlineStr">
+        <is>
+          <t>Other,Gas</t>
+        </is>
+      </c>
+      <c r="P151" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
     </row>
     <row r="152" ht="15.75" customHeight="1" s="19">
       <c r="A152" s="3" t="inlineStr">
@@ -8231,6 +10029,44 @@
           <t>https://www.zillow.com/homedetails/16-Stedman-St-Chelmsford-MA-01824/56446782_zpid/</t>
         </is>
       </c>
+      <c r="G152" t="n">
+        <v>884300</v>
+      </c>
+      <c r="H152" t="n">
+        <v>713100</v>
+      </c>
+      <c r="I152" t="n">
+        <v>2024</v>
+      </c>
+      <c r="J152" t="inlineStr">
+        <is>
+          <t>2010-03-31</t>
+        </is>
+      </c>
+      <c r="K152" t="n">
+        <v>3287</v>
+      </c>
+      <c r="L152" t="n">
+        <v>1915</v>
+      </c>
+      <c r="M152" t="n">
+        <v>0.5050505050505051</v>
+      </c>
+      <c r="N152" t="inlineStr">
+        <is>
+          <t>Acres</t>
+        </is>
+      </c>
+      <c r="O152" t="inlineStr">
+        <is>
+          <t>Forced air,Gas</t>
+        </is>
+      </c>
+      <c r="P152" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
       <c r="Q152" t="inlineStr">
         <is>
           <t>Zillow URL manually gathered for "Stedman Street" intead of "Steadman Street"</t>
@@ -8260,6 +10096,44 @@
           <t>https://www.zillow.com/homedetails/37-Andrews-St-Medford-MA-02155/56273730_zpid/</t>
         </is>
       </c>
+      <c r="G153" t="n">
+        <v>821800</v>
+      </c>
+      <c r="H153" t="n">
+        <v>665400</v>
+      </c>
+      <c r="I153" t="n">
+        <v>2024</v>
+      </c>
+      <c r="J153" t="inlineStr">
+        <is>
+          <t>2019-07-16</t>
+        </is>
+      </c>
+      <c r="K153" t="n">
+        <v>1517</v>
+      </c>
+      <c r="L153" t="n">
+        <v>1959</v>
+      </c>
+      <c r="M153" t="n">
+        <v>4748</v>
+      </c>
+      <c r="N153" t="inlineStr">
+        <is>
+          <t>Square Feet</t>
+        </is>
+      </c>
+      <c r="O153" t="inlineStr">
+        <is>
+          <t>Forced air,Gas</t>
+        </is>
+      </c>
+      <c r="P153" t="inlineStr">
+        <is>
+          <t>Central</t>
+        </is>
+      </c>
     </row>
     <row r="154" ht="15.75" customHeight="1" s="19">
       <c r="A154" s="3" t="inlineStr">
@@ -8284,6 +10158,44 @@
           <t>https://www.zillow.com/homedetails/49-Braemore-Rd-Waltham-MA-02451/56358904_zpid/</t>
         </is>
       </c>
+      <c r="G154" t="n">
+        <v>766000</v>
+      </c>
+      <c r="H154" t="n">
+        <v>608400</v>
+      </c>
+      <c r="I154" t="n">
+        <v>2024</v>
+      </c>
+      <c r="J154" t="inlineStr">
+        <is>
+          <t>2020-07-27</t>
+        </is>
+      </c>
+      <c r="K154" t="n">
+        <v>1296</v>
+      </c>
+      <c r="L154" t="n">
+        <v>1988</v>
+      </c>
+      <c r="M154" t="n">
+        <v>3049</v>
+      </c>
+      <c r="N154" t="inlineStr">
+        <is>
+          <t>Square Feet</t>
+        </is>
+      </c>
+      <c r="O154" t="inlineStr">
+        <is>
+          <t>Baseboard,Oil</t>
+        </is>
+      </c>
+      <c r="P154" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
     </row>
     <row r="155" ht="15.75" customHeight="1" s="19">
       <c r="A155" s="3" t="inlineStr">
@@ -8310,6 +10222,44 @@
           <t>https://www.zillow.com/homedetails/1-Stockdale-Rd-Needham-MA-02492/57478584_zpid/</t>
         </is>
       </c>
+      <c r="G155" t="n">
+        <v>1361500</v>
+      </c>
+      <c r="H155" t="n">
+        <v>889600</v>
+      </c>
+      <c r="I155" t="n">
+        <v>2024</v>
+      </c>
+      <c r="J155" t="inlineStr">
+        <is>
+          <t>2014-05-06</t>
+        </is>
+      </c>
+      <c r="K155" t="n">
+        <v>1748</v>
+      </c>
+      <c r="L155" t="n">
+        <v>1974</v>
+      </c>
+      <c r="M155" t="n">
+        <v>0.2699954086317723</v>
+      </c>
+      <c r="N155" t="inlineStr">
+        <is>
+          <t>Acres</t>
+        </is>
+      </c>
+      <c r="O155" t="inlineStr">
+        <is>
+          <t>Other,Electric</t>
+        </is>
+      </c>
+      <c r="P155" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
     </row>
     <row r="156" ht="15.75" customHeight="1" s="19">
       <c r="A156" s="3" t="inlineStr">
@@ -8336,6 +10286,44 @@
           <t>https://www.zillow.com/homedetails/67-Greenwood-Ave-Needham-MA-02492/57475276_zpid/</t>
         </is>
       </c>
+      <c r="G156" t="n">
+        <v>1438800</v>
+      </c>
+      <c r="H156" t="n">
+        <v>908000</v>
+      </c>
+      <c r="I156" t="n">
+        <v>2024</v>
+      </c>
+      <c r="J156" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="K156" t="n">
+        <v>2240</v>
+      </c>
+      <c r="L156" t="n">
+        <v>1997</v>
+      </c>
+      <c r="M156" t="n">
+        <v>8712</v>
+      </c>
+      <c r="N156" t="inlineStr">
+        <is>
+          <t>Square Feet</t>
+        </is>
+      </c>
+      <c r="O156" t="inlineStr">
+        <is>
+          <t>Other,Oil</t>
+        </is>
+      </c>
+      <c r="P156" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
     </row>
     <row r="157" ht="15.75" customHeight="1" s="19">
       <c r="A157" s="3" t="inlineStr">
@@ -8362,6 +10350,44 @@
           <t>https://www.zillow.com/homedetails/34-Seltsam-Way-Pembroke-MA-02359/121878579_zpid/</t>
         </is>
       </c>
+      <c r="G157" t="n">
+        <v>1189800</v>
+      </c>
+      <c r="H157" t="n">
+        <v>983000</v>
+      </c>
+      <c r="I157" t="n">
+        <v>2024</v>
+      </c>
+      <c r="J157" t="inlineStr">
+        <is>
+          <t>2016-11-15</t>
+        </is>
+      </c>
+      <c r="K157" t="n">
+        <v>2955</v>
+      </c>
+      <c r="L157" t="n">
+        <v>2013</v>
+      </c>
+      <c r="M157" t="n">
+        <v>0.9199954086317723</v>
+      </c>
+      <c r="N157" t="inlineStr">
+        <is>
+          <t>Acres</t>
+        </is>
+      </c>
+      <c r="O157" t="inlineStr">
+        <is>
+          <t>Forced air,Gas</t>
+        </is>
+      </c>
+      <c r="P157" t="inlineStr">
+        <is>
+          <t>Central</t>
+        </is>
+      </c>
     </row>
     <row r="158" ht="15.75" customHeight="1" s="19">
       <c r="A158" s="3" t="inlineStr">
@@ -8388,6 +10414,44 @@
           <t>https://www.zillow.com/homedetails/260-Vaughn-Hill-Rd-Bolton-MA-01740/57568665_zpid/</t>
         </is>
       </c>
+      <c r="G158" t="n">
+        <v>963800</v>
+      </c>
+      <c r="H158" t="n">
+        <v>792300</v>
+      </c>
+      <c r="I158" t="n">
+        <v>2024</v>
+      </c>
+      <c r="J158" t="inlineStr">
+        <is>
+          <t>2004-04-29</t>
+        </is>
+      </c>
+      <c r="K158" t="n">
+        <v>2828</v>
+      </c>
+      <c r="L158" t="n">
+        <v>1987</v>
+      </c>
+      <c r="M158" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="N158" t="inlineStr">
+        <is>
+          <t>Acres</t>
+        </is>
+      </c>
+      <c r="O158" t="inlineStr">
+        <is>
+          <t>Other,Oil</t>
+        </is>
+      </c>
+      <c r="P158" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
     </row>
     <row r="159" ht="15.75" customHeight="1" s="19">
       <c r="A159" s="3" t="inlineStr">
@@ -8443,6 +10507,44 @@
           <t>https://www.zillow.com/homedetails/76-Woodlot-Rd-Amherst-MA-01002/56258359_zpid/</t>
         </is>
       </c>
+      <c r="G160" t="n">
+        <v>710300</v>
+      </c>
+      <c r="H160" t="n">
+        <v>636500</v>
+      </c>
+      <c r="I160" t="n">
+        <v>2024</v>
+      </c>
+      <c r="J160" t="inlineStr">
+        <is>
+          <t>2022-08-16</t>
+        </is>
+      </c>
+      <c r="K160" t="n">
+        <v>3176</v>
+      </c>
+      <c r="L160" t="n">
+        <v>1988</v>
+      </c>
+      <c r="M160" t="n">
+        <v>0.5900000000000001</v>
+      </c>
+      <c r="N160" t="inlineStr">
+        <is>
+          <t>Acres</t>
+        </is>
+      </c>
+      <c r="O160" t="inlineStr">
+        <is>
+          <t>Baseboard,Oil,ENERGY STAR Qualified Equipment</t>
+        </is>
+      </c>
+      <c r="P160" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
     </row>
     <row r="161" ht="15.75" customHeight="1" s="19">
       <c r="A161" s="3" t="inlineStr">
@@ -8469,6 +10571,44 @@
           <t>https://www.zillow.com/homedetails/26-Foxglove-Ln-Amherst-MA-01002/56258411_zpid/</t>
         </is>
       </c>
+      <c r="G161" t="n">
+        <v>694300</v>
+      </c>
+      <c r="H161" t="n">
+        <v>573000</v>
+      </c>
+      <c r="I161" t="n">
+        <v>2024</v>
+      </c>
+      <c r="J161" t="inlineStr">
+        <is>
+          <t>2018-09-06</t>
+        </is>
+      </c>
+      <c r="K161" t="n">
+        <v>2174</v>
+      </c>
+      <c r="L161" t="n">
+        <v>1985</v>
+      </c>
+      <c r="M161" t="n">
+        <v>0.7299816345270891</v>
+      </c>
+      <c r="N161" t="inlineStr">
+        <is>
+          <t>Acres</t>
+        </is>
+      </c>
+      <c r="O161" t="inlineStr">
+        <is>
+          <t>Other,Oil</t>
+        </is>
+      </c>
+      <c r="P161" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
     </row>
     <row r="162" ht="15.75" customHeight="1" s="19">
       <c r="A162" s="3" t="inlineStr">
@@ -8495,6 +10635,44 @@
           <t>https://www.zillow.com/homedetails/12-Bayberry-Ln-Hadley-MA-01035/67714823_zpid/</t>
         </is>
       </c>
+      <c r="G162" t="n">
+        <v>1292800</v>
+      </c>
+      <c r="H162" t="n">
+        <v>1142800</v>
+      </c>
+      <c r="I162" t="n">
+        <v>2024</v>
+      </c>
+      <c r="J162" t="inlineStr">
+        <is>
+          <t>2013-07-19</t>
+        </is>
+      </c>
+      <c r="K162" t="n">
+        <v>7000</v>
+      </c>
+      <c r="L162" t="n">
+        <v>2005</v>
+      </c>
+      <c r="M162" t="n">
+        <v>1</v>
+      </c>
+      <c r="N162" t="inlineStr">
+        <is>
+          <t>Acres</t>
+        </is>
+      </c>
+      <c r="O162" t="inlineStr">
+        <is>
+          <t>Forced air,Oil</t>
+        </is>
+      </c>
+      <c r="P162" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
     </row>
     <row r="163" ht="15.75" customHeight="1" s="19">
       <c r="A163" s="3" t="inlineStr">
@@ -8521,6 +10699,44 @@
           <t>https://www.zillow.com/homedetails/124-Moser-St-Northampton-MA-01060/121251942_zpid/</t>
         </is>
       </c>
+      <c r="G163" t="n">
+        <v>803400</v>
+      </c>
+      <c r="H163" t="n">
+        <v>706600</v>
+      </c>
+      <c r="I163" t="n">
+        <v>2024</v>
+      </c>
+      <c r="J163" t="inlineStr">
+        <is>
+          <t>2021-09-30</t>
+        </is>
+      </c>
+      <c r="K163" t="n">
+        <v>1952</v>
+      </c>
+      <c r="L163" t="n">
+        <v>2013</v>
+      </c>
+      <c r="M163" t="n">
+        <v>5227</v>
+      </c>
+      <c r="N163" t="inlineStr">
+        <is>
+          <t>Square Feet</t>
+        </is>
+      </c>
+      <c r="O163" t="inlineStr">
+        <is>
+          <t>Forced air,Gas</t>
+        </is>
+      </c>
+      <c r="P163" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
     </row>
     <row r="164" ht="15.75" customHeight="1" s="19">
       <c r="A164" s="3" t="inlineStr">
@@ -8547,6 +10763,44 @@
           <t>https://www.zillow.com/homedetails/442-East-St-Easthampton-MA-01027/59881486_zpid/</t>
         </is>
       </c>
+      <c r="G164" t="n">
+        <v>438800</v>
+      </c>
+      <c r="H164" t="n">
+        <v>373100</v>
+      </c>
+      <c r="I164" t="n">
+        <v>2024</v>
+      </c>
+      <c r="J164" t="inlineStr">
+        <is>
+          <t>2018-05-31</t>
+        </is>
+      </c>
+      <c r="K164" t="n">
+        <v>1440</v>
+      </c>
+      <c r="L164" t="n">
+        <v>1997</v>
+      </c>
+      <c r="M164" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="N164" t="inlineStr">
+        <is>
+          <t>Acres</t>
+        </is>
+      </c>
+      <c r="O164" t="inlineStr">
+        <is>
+          <t>Forced air,Oil</t>
+        </is>
+      </c>
+      <c r="P164" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
     </row>
     <row r="165" ht="15.75" customHeight="1" s="19">
       <c r="A165" s="3" t="inlineStr">
@@ -8573,6 +10827,44 @@
           <t>https://www.zillow.com/homedetails/5-Bean-Porridge-Hill-Rd-Westminster-MA-01473/57681454_zpid/</t>
         </is>
       </c>
+      <c r="G165" t="n">
+        <v>651200</v>
+      </c>
+      <c r="H165" t="n">
+        <v>510500</v>
+      </c>
+      <c r="I165" t="n">
+        <v>2024</v>
+      </c>
+      <c r="J165" t="inlineStr">
+        <is>
+          <t>2017-08-07</t>
+        </is>
+      </c>
+      <c r="K165" t="n">
+        <v>3195</v>
+      </c>
+      <c r="L165" t="n">
+        <v>1991</v>
+      </c>
+      <c r="M165" t="n">
+        <v>2.289990817263544</v>
+      </c>
+      <c r="N165" t="inlineStr">
+        <is>
+          <t>Acres</t>
+        </is>
+      </c>
+      <c r="O165" t="inlineStr">
+        <is>
+          <t>Other,Oil</t>
+        </is>
+      </c>
+      <c r="P165" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
     </row>
     <row r="166" ht="15.75" customHeight="1" s="19">
       <c r="A166" s="3" t="inlineStr">
@@ -8597,6 +10889,44 @@
           <t>https://www.zillow.com/homedetails/68-McGee-Dr-Hyannis-MA-02601/55846054_zpid/</t>
         </is>
       </c>
+      <c r="G166" t="n">
+        <v>585000</v>
+      </c>
+      <c r="H166" t="n">
+        <v>512400</v>
+      </c>
+      <c r="I166" t="n">
+        <v>2024</v>
+      </c>
+      <c r="J166" t="inlineStr">
+        <is>
+          <t>2009-11-24</t>
+        </is>
+      </c>
+      <c r="K166" t="n">
+        <v>1152</v>
+      </c>
+      <c r="L166" t="n">
+        <v>1989</v>
+      </c>
+      <c r="M166" t="n">
+        <v>0.3399908172635445</v>
+      </c>
+      <c r="N166" t="inlineStr">
+        <is>
+          <t>Acres</t>
+        </is>
+      </c>
+      <c r="O166" t="inlineStr">
+        <is>
+          <t>Forced air,Gas</t>
+        </is>
+      </c>
+      <c r="P166" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
     </row>
     <row r="167" ht="15.75" customHeight="1" s="19">
       <c r="A167" s="3" t="inlineStr">
@@ -8623,6 +10953,44 @@
           <t>https://www.zillow.com/homedetails/118-Wild-Harbor-Rd-North-Falmouth-MA-02556/55881954_zpid/</t>
         </is>
       </c>
+      <c r="G167" t="n">
+        <v>1516600</v>
+      </c>
+      <c r="H167" t="n">
+        <v>1089700</v>
+      </c>
+      <c r="I167" t="n">
+        <v>2024</v>
+      </c>
+      <c r="J167" t="inlineStr">
+        <is>
+          <t>2017-01-19</t>
+        </is>
+      </c>
+      <c r="K167" t="n">
+        <v>3002</v>
+      </c>
+      <c r="L167" t="n">
+        <v>1900</v>
+      </c>
+      <c r="M167" t="n">
+        <v>0.9399908172635445</v>
+      </c>
+      <c r="N167" t="inlineStr">
+        <is>
+          <t>Acres</t>
+        </is>
+      </c>
+      <c r="O167" t="inlineStr">
+        <is>
+          <t>Other,Oil</t>
+        </is>
+      </c>
+      <c r="P167" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
     </row>
     <row r="168" ht="15.75" customHeight="1" s="19">
       <c r="A168" s="3" t="inlineStr">
@@ -8649,6 +11017,44 @@
           <t>https://www.zillow.com/homedetails/46-Scotland-Heights-Rd-Haverhill-MA-01832/56056737_zpid/</t>
         </is>
       </c>
+      <c r="G168" t="n">
+        <v>832300</v>
+      </c>
+      <c r="H168" t="n">
+        <v>706200</v>
+      </c>
+      <c r="I168" t="n">
+        <v>2024</v>
+      </c>
+      <c r="J168" t="inlineStr">
+        <is>
+          <t>2000-05-01</t>
+        </is>
+      </c>
+      <c r="K168" t="n">
+        <v>2632</v>
+      </c>
+      <c r="L168" t="n">
+        <v>1999</v>
+      </c>
+      <c r="M168" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="N168" t="inlineStr">
+        <is>
+          <t>Acres</t>
+        </is>
+      </c>
+      <c r="O168" t="inlineStr">
+        <is>
+          <t>Forced air,Gas</t>
+        </is>
+      </c>
+      <c r="P168" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
     </row>
     <row r="169" ht="15.75" customHeight="1" s="19">
       <c r="A169" s="3" t="inlineStr">
@@ -8675,6 +11081,44 @@
           <t>https://www.zillow.com/homedetails/13-Kenwood-St-Chelmsford-MA-01824/56451880_zpid/</t>
         </is>
       </c>
+      <c r="G169" t="n">
+        <v>920900</v>
+      </c>
+      <c r="H169" t="n">
+        <v>779600</v>
+      </c>
+      <c r="I169" t="n">
+        <v>2024</v>
+      </c>
+      <c r="J169" t="inlineStr">
+        <is>
+          <t>2021-09-13</t>
+        </is>
+      </c>
+      <c r="K169" t="n">
+        <v>2352</v>
+      </c>
+      <c r="L169" t="n">
+        <v>2013</v>
+      </c>
+      <c r="M169" t="n">
+        <v>0.3699954086317723</v>
+      </c>
+      <c r="N169" t="inlineStr">
+        <is>
+          <t>Acres</t>
+        </is>
+      </c>
+      <c r="O169" t="inlineStr">
+        <is>
+          <t>Baseboard,Gas</t>
+        </is>
+      </c>
+      <c r="P169" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
     </row>
     <row r="170" ht="15.75" customHeight="1" s="19">
       <c r="A170" s="3" t="inlineStr">
@@ -8701,6 +11145,44 @@
           <t>https://www.zillow.com/homedetails/22-Orchard-Ln-Groton-MA-01450/61315789_zpid/</t>
         </is>
       </c>
+      <c r="G170" t="n">
+        <v>713700</v>
+      </c>
+      <c r="H170" t="n">
+        <v>616100</v>
+      </c>
+      <c r="I170" t="n">
+        <v>2024</v>
+      </c>
+      <c r="J170" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="K170" t="n">
+        <v>3050</v>
+      </c>
+      <c r="L170" t="n">
+        <v>1969</v>
+      </c>
+      <c r="M170" t="n">
+        <v>3.1</v>
+      </c>
+      <c r="N170" t="inlineStr">
+        <is>
+          <t>Acres</t>
+        </is>
+      </c>
+      <c r="O170" t="inlineStr">
+        <is>
+          <t>Other,Oil,Other</t>
+        </is>
+      </c>
+      <c r="P170" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
     </row>
     <row r="171" ht="15.75" customHeight="1" s="19">
       <c r="A171" s="3" t="inlineStr">
@@ -8725,6 +11207,44 @@
           <t>https://www.zillow.com/homedetails/84-Ramshead-Rd-Medford-MA-02155/56275351_zpid/</t>
         </is>
       </c>
+      <c r="G171" t="n">
+        <v>1117100</v>
+      </c>
+      <c r="H171" t="n">
+        <v>783600</v>
+      </c>
+      <c r="I171" t="n">
+        <v>2024</v>
+      </c>
+      <c r="J171" t="inlineStr">
+        <is>
+          <t>2021-10-07</t>
+        </is>
+      </c>
+      <c r="K171" t="n">
+        <v>1806</v>
+      </c>
+      <c r="L171" t="n">
+        <v>1935</v>
+      </c>
+      <c r="M171" t="n">
+        <v>6098</v>
+      </c>
+      <c r="N171" t="inlineStr">
+        <is>
+          <t>Square Feet</t>
+        </is>
+      </c>
+      <c r="O171" t="inlineStr">
+        <is>
+          <t>Other,Gas</t>
+        </is>
+      </c>
+      <c r="P171" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
     </row>
     <row r="172" ht="15.75" customHeight="1" s="19">
       <c r="A172" s="3" t="inlineStr">
@@ -8749,6 +11269,44 @@
           <t>https://www.zillow.com/homedetails/25-Stockdale-Rd-Needham-MA-02492/57478581_zpid/</t>
         </is>
       </c>
+      <c r="G172" t="n">
+        <v>1172000</v>
+      </c>
+      <c r="H172" t="n">
+        <v>797400</v>
+      </c>
+      <c r="I172" t="n">
+        <v>2024</v>
+      </c>
+      <c r="J172" t="inlineStr">
+        <is>
+          <t>2005-06-03</t>
+        </is>
+      </c>
+      <c r="K172" t="n">
+        <v>1461</v>
+      </c>
+      <c r="L172" t="n">
+        <v>1934</v>
+      </c>
+      <c r="M172" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="N172" t="inlineStr">
+        <is>
+          <t>Acres</t>
+        </is>
+      </c>
+      <c r="O172" t="inlineStr">
+        <is>
+          <t>Forced air,Oil</t>
+        </is>
+      </c>
+      <c r="P172" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
     </row>
     <row r="173" ht="15.75" customHeight="1" s="19">
       <c r="A173" s="3" t="inlineStr">
@@ -8773,6 +11331,44 @@
           <t>https://www.zillow.com/homedetails/34-Rawson-Rd-Bellingham-MA-02019/57424042_zpid/</t>
         </is>
       </c>
+      <c r="G173" t="n">
+        <v>580600</v>
+      </c>
+      <c r="H173" t="n">
+        <v>420500</v>
+      </c>
+      <c r="I173" t="n">
+        <v>2024</v>
+      </c>
+      <c r="J173" t="inlineStr">
+        <is>
+          <t>1993-01-15</t>
+        </is>
+      </c>
+      <c r="K173" t="n">
+        <v>1512</v>
+      </c>
+      <c r="L173" t="n">
+        <v>1992</v>
+      </c>
+      <c r="M173" t="n">
+        <v>0.5399908172635446</v>
+      </c>
+      <c r="N173" t="inlineStr">
+        <is>
+          <t>Acres</t>
+        </is>
+      </c>
+      <c r="O173" t="inlineStr">
+        <is>
+          <t>Other,Gas</t>
+        </is>
+      </c>
+      <c r="P173" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
     </row>
     <row r="174" ht="15.75" customHeight="1" s="19">
       <c r="A174" s="3" t="inlineStr">
@@ -8799,6 +11395,44 @@
           <t>https://www.zillow.com/homedetails/155-Raymond-Dr-Hampden-MA-01036/56173315_zpid/</t>
         </is>
       </c>
+      <c r="G174" t="n">
+        <v>422800</v>
+      </c>
+      <c r="H174" t="n">
+        <v>364900</v>
+      </c>
+      <c r="I174" t="n">
+        <v>2024</v>
+      </c>
+      <c r="J174" t="inlineStr">
+        <is>
+          <t>2021-05-25</t>
+        </is>
+      </c>
+      <c r="K174" t="n">
+        <v>1593</v>
+      </c>
+      <c r="L174" t="n">
+        <v>1967</v>
+      </c>
+      <c r="M174" t="n">
+        <v>0.6887052341597796</v>
+      </c>
+      <c r="N174" t="inlineStr">
+        <is>
+          <t>Acres</t>
+        </is>
+      </c>
+      <c r="O174" t="inlineStr">
+        <is>
+          <t>Baseboard,Electric</t>
+        </is>
+      </c>
+      <c r="P174" t="inlineStr">
+        <is>
+          <t>Central</t>
+        </is>
+      </c>
     </row>
     <row r="175" ht="15.75" customHeight="1" s="19">
       <c r="A175" s="3" t="inlineStr">
@@ -8825,6 +11459,44 @@
           <t>https://www.zillow.com/homedetails/37-Harris-St-Amherst-MA-01002/56254550_zpid/</t>
         </is>
       </c>
+      <c r="G175" t="n">
+        <v>672500</v>
+      </c>
+      <c r="H175" t="n">
+        <v>567100</v>
+      </c>
+      <c r="I175" t="n">
+        <v>2024</v>
+      </c>
+      <c r="J175" t="inlineStr">
+        <is>
+          <t>2013-10-31</t>
+        </is>
+      </c>
+      <c r="K175" t="n">
+        <v>2430</v>
+      </c>
+      <c r="L175" t="n">
+        <v>1987</v>
+      </c>
+      <c r="M175" t="n">
+        <v>0.6399908172635446</v>
+      </c>
+      <c r="N175" t="inlineStr">
+        <is>
+          <t>Acres</t>
+        </is>
+      </c>
+      <c r="O175" t="inlineStr">
+        <is>
+          <t>Forced air,Electric</t>
+        </is>
+      </c>
+      <c r="P175" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
     </row>
     <row r="176" ht="15.75" customHeight="1" s="19">
       <c r="A176" s="3" t="inlineStr">
@@ -8851,6 +11523,44 @@
           <t>https://www.zillow.com/homedetails/19-Foxglove-Ln-Amherst-MA-01002/56258404_zpid/</t>
         </is>
       </c>
+      <c r="G176" t="n">
+        <v>795900</v>
+      </c>
+      <c r="H176" t="n">
+        <v>686600</v>
+      </c>
+      <c r="I176" t="n">
+        <v>2024</v>
+      </c>
+      <c r="J176" t="inlineStr">
+        <is>
+          <t>2017-11-21</t>
+        </is>
+      </c>
+      <c r="K176" t="n">
+        <v>2640</v>
+      </c>
+      <c r="L176" t="n">
+        <v>1984</v>
+      </c>
+      <c r="M176" t="n">
+        <v>0.8399908172635445</v>
+      </c>
+      <c r="N176" t="inlineStr">
+        <is>
+          <t>Acres</t>
+        </is>
+      </c>
+      <c r="O176" t="inlineStr">
+        <is>
+          <t>Forced air,Oil</t>
+        </is>
+      </c>
+      <c r="P176" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
     </row>
     <row r="177" ht="15.75" customHeight="1" s="19">
       <c r="A177" s="3" t="inlineStr">
@@ -8875,6 +11585,44 @@
           <t>https://www.zillow.com/homedetails/10-Frost-Ln-Hadley-MA-01035/57015383_zpid/</t>
         </is>
       </c>
+      <c r="G177" t="n">
+        <v>549800</v>
+      </c>
+      <c r="H177" t="n">
+        <v>418900</v>
+      </c>
+      <c r="I177" t="n">
+        <v>2024</v>
+      </c>
+      <c r="J177" t="inlineStr">
+        <is>
+          <t>2016-08-04</t>
+        </is>
+      </c>
+      <c r="K177" t="n">
+        <v>1832</v>
+      </c>
+      <c r="L177" t="n">
+        <v>1968</v>
+      </c>
+      <c r="M177" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="N177" t="inlineStr">
+        <is>
+          <t>Acres</t>
+        </is>
+      </c>
+      <c r="O177" t="inlineStr">
+        <is>
+          <t>Baseboard,Oil</t>
+        </is>
+      </c>
+      <c r="P177" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
     </row>
     <row r="178" ht="15.75" customHeight="1" s="19">
       <c r="A178" s="3" t="inlineStr">
@@ -8901,6 +11649,44 @@
           <t>https://www.zillow.com/homedetails/104-Wildflower-Dr-Amherst-MA-01002/56258337_zpid/</t>
         </is>
       </c>
+      <c r="G178" t="n">
+        <v>784700</v>
+      </c>
+      <c r="H178" t="n">
+        <v>711100</v>
+      </c>
+      <c r="I178" t="n">
+        <v>2024</v>
+      </c>
+      <c r="J178" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="K178" t="n">
+        <v>2685</v>
+      </c>
+      <c r="L178" t="n">
+        <v>1986</v>
+      </c>
+      <c r="M178" t="n">
+        <v>0.6899908172635445</v>
+      </c>
+      <c r="N178" t="inlineStr">
+        <is>
+          <t>Acres</t>
+        </is>
+      </c>
+      <c r="O178" t="inlineStr">
+        <is>
+          <t>Forced air,Oil</t>
+        </is>
+      </c>
+      <c r="P178" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
     </row>
     <row r="179" ht="15.75" customHeight="1" s="19">
       <c r="A179" s="3" t="inlineStr">
@@ -8927,6 +11713,44 @@
           <t>https://www.zillow.com/homedetails/152-Birchtree-Dr-Westwood-MA-02090/57515978_zpid/</t>
         </is>
       </c>
+      <c r="G179" t="n">
+        <v>1513000</v>
+      </c>
+      <c r="H179" t="n">
+        <v>1166200</v>
+      </c>
+      <c r="I179" t="n">
+        <v>2024</v>
+      </c>
+      <c r="J179" t="inlineStr">
+        <is>
+          <t>2015-04-22</t>
+        </is>
+      </c>
+      <c r="K179" t="n">
+        <v>2140</v>
+      </c>
+      <c r="L179" t="n">
+        <v>1951</v>
+      </c>
+      <c r="M179" t="n">
+        <v>0.35</v>
+      </c>
+      <c r="N179" t="inlineStr">
+        <is>
+          <t>Acres</t>
+        </is>
+      </c>
+      <c r="O179" t="inlineStr">
+        <is>
+          <t>Forced air,Other,Oil</t>
+        </is>
+      </c>
+      <c r="P179" t="inlineStr">
+        <is>
+          <t>Central</t>
+        </is>
+      </c>
     </row>
     <row r="180" ht="15.75" customHeight="1" s="19">
       <c r="A180" s="3" t="inlineStr">
@@ -8951,6 +11775,44 @@
           <t>https://www.zillow.com/homedetails/21-Blaisdell-Rd-Medford-MA-02155/56275330_zpid/</t>
         </is>
       </c>
+      <c r="G180" t="n">
+        <v>823100</v>
+      </c>
+      <c r="H180" t="n">
+        <v>713900</v>
+      </c>
+      <c r="I180" t="n">
+        <v>2024</v>
+      </c>
+      <c r="J180" t="inlineStr">
+        <is>
+          <t>1998-10-13</t>
+        </is>
+      </c>
+      <c r="K180" t="n">
+        <v>1344</v>
+      </c>
+      <c r="L180" t="n">
+        <v>1940</v>
+      </c>
+      <c r="M180" t="n">
+        <v>6098</v>
+      </c>
+      <c r="N180" t="inlineStr">
+        <is>
+          <t>Square Feet</t>
+        </is>
+      </c>
+      <c r="O180" t="inlineStr">
+        <is>
+          <t>Other,Gas</t>
+        </is>
+      </c>
+      <c r="P180" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
     </row>
     <row r="181" ht="15.75" customHeight="1" s="19">
       <c r="A181" s="3" t="inlineStr">
@@ -8975,6 +11837,44 @@
           <t>https://www.zillow.com/homedetails/28-Longview-Rd-North-Falmouth-MA-02556/55883394_zpid/</t>
         </is>
       </c>
+      <c r="G181" t="n">
+        <v>795600</v>
+      </c>
+      <c r="H181" t="n">
+        <v>567600</v>
+      </c>
+      <c r="I181" t="n">
+        <v>2024</v>
+      </c>
+      <c r="J181" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="K181" t="n">
+        <v>1568</v>
+      </c>
+      <c r="L181" t="n">
+        <v>1983</v>
+      </c>
+      <c r="M181" t="n">
+        <v>1.25</v>
+      </c>
+      <c r="N181" t="inlineStr">
+        <is>
+          <t>Acres</t>
+        </is>
+      </c>
+      <c r="O181" t="inlineStr">
+        <is>
+          <t>Baseboard,Electric</t>
+        </is>
+      </c>
+      <c r="P181" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
     </row>
     <row r="182" ht="15.75" customHeight="1" s="19">
       <c r="A182" s="3" t="inlineStr">
@@ -9001,6 +11901,44 @@
           <t>https://www.zillow.com/homedetails/25-Kaileys-Way-Groton-MA-01450/57066228_zpid/</t>
         </is>
       </c>
+      <c r="G182" t="n">
+        <v>828400</v>
+      </c>
+      <c r="H182" t="n">
+        <v>676900</v>
+      </c>
+      <c r="I182" t="n">
+        <v>2024</v>
+      </c>
+      <c r="J182" t="inlineStr">
+        <is>
+          <t>2020-07-10</t>
+        </is>
+      </c>
+      <c r="K182" t="n">
+        <v>2810</v>
+      </c>
+      <c r="L182" t="n">
+        <v>1997</v>
+      </c>
+      <c r="M182" t="n">
+        <v>2.959986225895317</v>
+      </c>
+      <c r="N182" t="inlineStr">
+        <is>
+          <t>Acres</t>
+        </is>
+      </c>
+      <c r="O182" t="inlineStr">
+        <is>
+          <t>Forced air,Propane / Butane</t>
+        </is>
+      </c>
+      <c r="P182" t="inlineStr">
+        <is>
+          <t>Central</t>
+        </is>
+      </c>
     </row>
     <row r="183" ht="15.75" customHeight="1" s="19">
       <c r="A183" s="3" t="inlineStr">
@@ -9027,6 +11965,44 @@
           <t>https://www.zillow.com/homedetails/55-Cedar-Hill-Rd-Bellingham-MA-02019/57423546_zpid/</t>
         </is>
       </c>
+      <c r="G183" t="n">
+        <v>580600</v>
+      </c>
+      <c r="H183" t="n">
+        <v>439400</v>
+      </c>
+      <c r="I183" t="n">
+        <v>2024</v>
+      </c>
+      <c r="J183" t="inlineStr">
+        <is>
+          <t>2021-11-29</t>
+        </is>
+      </c>
+      <c r="K183" t="n">
+        <v>1483</v>
+      </c>
+      <c r="L183" t="n">
+        <v>1958</v>
+      </c>
+      <c r="M183" t="n">
+        <v>0.3299816345270891</v>
+      </c>
+      <c r="N183" t="inlineStr">
+        <is>
+          <t>Acres</t>
+        </is>
+      </c>
+      <c r="O183" t="inlineStr">
+        <is>
+          <t>Forced air,Oil</t>
+        </is>
+      </c>
+      <c r="P183" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
     </row>
     <row r="184" ht="15.75" customHeight="1" s="19">
       <c r="A184" s="3" t="inlineStr">
@@ -9053,6 +12029,44 @@
           <t>https://www.zillow.com/homedetails/10-Hillview-Ln-Plymouth-MA-02360/71374281_zpid/</t>
         </is>
       </c>
+      <c r="G184" t="n">
+        <v>862000</v>
+      </c>
+      <c r="H184" t="n">
+        <v>739800</v>
+      </c>
+      <c r="I184" t="n">
+        <v>2024</v>
+      </c>
+      <c r="J184" t="inlineStr">
+        <is>
+          <t>2017-10-27</t>
+        </is>
+      </c>
+      <c r="K184" t="n">
+        <v>2160</v>
+      </c>
+      <c r="L184" t="n">
+        <v>2005</v>
+      </c>
+      <c r="M184" t="n">
+        <v>0.5790863177226814</v>
+      </c>
+      <c r="N184" t="inlineStr">
+        <is>
+          <t>Acres</t>
+        </is>
+      </c>
+      <c r="O184" t="inlineStr">
+        <is>
+          <t>Baseboard,Gas</t>
+        </is>
+      </c>
+      <c r="P184" t="inlineStr">
+        <is>
+          <t>Central</t>
+        </is>
+      </c>
     </row>
     <row r="185" ht="15.75" customHeight="1" s="19">
       <c r="A185" s="3" t="inlineStr">
@@ -9079,6 +12093,46 @@
           <t>https://www.zillow.com/homedetails/15-Hope-St-Hopedale-MA-01747/57603536_zpid/</t>
         </is>
       </c>
+      <c r="G185" t="n">
+        <v>356800</v>
+      </c>
+      <c r="H185" t="n">
+        <v>263800</v>
+      </c>
+      <c r="I185" t="n">
+        <v>2024</v>
+      </c>
+      <c r="J185" t="inlineStr">
+        <is>
+          <t>2002-10-29</t>
+        </is>
+      </c>
+      <c r="K185" t="n">
+        <v>1282</v>
+      </c>
+      <c r="L185" t="n">
+        <v>1880</v>
+      </c>
+      <c r="M185" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="N185" t="inlineStr">
+        <is>
+          <t>sqft</t>
+        </is>
+      </c>
+      <c r="O185" t="inlineStr">
+        <is>
+          <t>Forced air,Oil</t>
+        </is>
+      </c>
+      <c r="P185" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
     </row>
     <row r="186" ht="15.75" customHeight="1" s="19">
       <c r="A186" s="3" t="inlineStr">
@@ -9105,6 +12159,44 @@
           <t>https://www.zillow.com/homedetails/7-Kennedy-Dr-Hadley-MA-01035/57015490_zpid/</t>
         </is>
       </c>
+      <c r="G186" t="n">
+        <v>655400</v>
+      </c>
+      <c r="H186" t="n">
+        <v>478200</v>
+      </c>
+      <c r="I186" t="n">
+        <v>2024</v>
+      </c>
+      <c r="J186" t="inlineStr">
+        <is>
+          <t>1996-09-13</t>
+        </is>
+      </c>
+      <c r="K186" t="n">
+        <v>3274</v>
+      </c>
+      <c r="L186" t="n">
+        <v>1972</v>
+      </c>
+      <c r="M186" t="n">
+        <v>0.6599862258953169</v>
+      </c>
+      <c r="N186" t="inlineStr">
+        <is>
+          <t>Acres</t>
+        </is>
+      </c>
+      <c r="O186" t="inlineStr">
+        <is>
+          <t>Other,Oil</t>
+        </is>
+      </c>
+      <c r="P186" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
     </row>
     <row r="187" ht="15.75" customHeight="1" s="19">
       <c r="A187" s="3" t="inlineStr">
@@ -9131,6 +12223,44 @@
           <t>https://www.zillow.com/homedetails/2-Bayberry-Ln-Hadley-MA-01035/61806217_zpid/</t>
         </is>
       </c>
+      <c r="G187" t="n">
+        <v>741900</v>
+      </c>
+      <c r="H187" t="n">
+        <v>637400</v>
+      </c>
+      <c r="I187" t="n">
+        <v>2024</v>
+      </c>
+      <c r="J187" t="inlineStr">
+        <is>
+          <t>2004-04-16</t>
+        </is>
+      </c>
+      <c r="K187" t="n">
+        <v>2424</v>
+      </c>
+      <c r="L187" t="n">
+        <v>2004</v>
+      </c>
+      <c r="M187" t="n">
+        <v>0.7099862258953168</v>
+      </c>
+      <c r="N187" t="inlineStr">
+        <is>
+          <t>Acres</t>
+        </is>
+      </c>
+      <c r="O187" t="inlineStr">
+        <is>
+          <t>Forced air,Oil</t>
+        </is>
+      </c>
+      <c r="P187" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
     </row>
     <row r="188" ht="15.75" customHeight="1" s="19">
       <c r="A188" s="3" t="inlineStr">
@@ -9157,6 +12287,44 @@
           <t>https://www.zillow.com/homedetails/130-Hillcrest-Dr-Northampton-MA-01062/57020096_zpid/</t>
         </is>
       </c>
+      <c r="G188" t="n">
+        <v>926300</v>
+      </c>
+      <c r="H188" t="n">
+        <v>783700</v>
+      </c>
+      <c r="I188" t="n">
+        <v>2024</v>
+      </c>
+      <c r="J188" t="inlineStr">
+        <is>
+          <t>2019-08-30</t>
+        </is>
+      </c>
+      <c r="K188" t="n">
+        <v>2655</v>
+      </c>
+      <c r="L188" t="n">
+        <v>1992</v>
+      </c>
+      <c r="M188" t="n">
+        <v>0.4699954086317722</v>
+      </c>
+      <c r="N188" t="inlineStr">
+        <is>
+          <t>Acres</t>
+        </is>
+      </c>
+      <c r="O188" t="inlineStr">
+        <is>
+          <t>Other,Oil</t>
+        </is>
+      </c>
+      <c r="P188" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
     </row>
     <row r="189" ht="15.75" customHeight="1" s="19">
       <c r="A189" s="3" t="inlineStr">
@@ -9183,6 +12351,46 @@
           <t>https://www.zillow.com/homedetails/4-Moser-St-Northampton-MA-01060/102990282_zpid/</t>
         </is>
       </c>
+      <c r="G189" t="n">
+        <v>422800</v>
+      </c>
+      <c r="H189" t="n">
+        <v>330300</v>
+      </c>
+      <c r="I189" t="n">
+        <v>2024</v>
+      </c>
+      <c r="J189" t="inlineStr">
+        <is>
+          <t>2011-02-11</t>
+        </is>
+      </c>
+      <c r="K189" t="n">
+        <v>1152</v>
+      </c>
+      <c r="L189" t="n">
+        <v>2010</v>
+      </c>
+      <c r="M189" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="N189" t="inlineStr">
+        <is>
+          <t>sqft</t>
+        </is>
+      </c>
+      <c r="O189" t="inlineStr">
+        <is>
+          <t>Forced air,Gas</t>
+        </is>
+      </c>
+      <c r="P189" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
     </row>
     <row r="190" ht="15.75" customHeight="1" s="19">
       <c r="A190" s="3" t="inlineStr">
@@ -9209,6 +12417,44 @@
           <t>https://www.zillow.com/homedetails/5-Elm-Top-Ln-Beverly-MA-01915/59225870_zpid/</t>
         </is>
       </c>
+      <c r="G190" t="n">
+        <v>3896000</v>
+      </c>
+      <c r="H190" t="n">
+        <v>2926200</v>
+      </c>
+      <c r="I190" t="n">
+        <v>2024</v>
+      </c>
+      <c r="J190" t="inlineStr">
+        <is>
+          <t>2006-09-26</t>
+        </is>
+      </c>
+      <c r="K190" t="n">
+        <v>5216</v>
+      </c>
+      <c r="L190" t="n">
+        <v>2006</v>
+      </c>
+      <c r="M190" t="n">
+        <v>0.7599862258953168</v>
+      </c>
+      <c r="N190" t="inlineStr">
+        <is>
+          <t>Acres</t>
+        </is>
+      </c>
+      <c r="O190" t="inlineStr">
+        <is>
+          <t>Forced air,Gas</t>
+        </is>
+      </c>
+      <c r="P190" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
     </row>
     <row r="191" ht="15.75" customHeight="1" s="19">
       <c r="A191" s="3" t="inlineStr">
@@ -9233,6 +12479,44 @@
           <t>https://www.zillow.com/homedetails/89-Park-Rd-Chelmsford-MA-01824/56451860_zpid/</t>
         </is>
       </c>
+      <c r="G191" t="n">
+        <v>879800</v>
+      </c>
+      <c r="H191" t="n">
+        <v>736700</v>
+      </c>
+      <c r="I191" t="n">
+        <v>2024</v>
+      </c>
+      <c r="J191" t="inlineStr">
+        <is>
+          <t>1996-05-31</t>
+        </is>
+      </c>
+      <c r="K191" t="n">
+        <v>2440</v>
+      </c>
+      <c r="L191" t="n">
+        <v>1950</v>
+      </c>
+      <c r="M191" t="n">
+        <v>1.039990817263545</v>
+      </c>
+      <c r="N191" t="inlineStr">
+        <is>
+          <t>Acres</t>
+        </is>
+      </c>
+      <c r="O191" t="inlineStr">
+        <is>
+          <t>Forced air,Oil</t>
+        </is>
+      </c>
+      <c r="P191" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
     </row>
     <row r="192" ht="15.75" customHeight="1" s="19">
       <c r="A192" s="3" t="inlineStr">
@@ -9259,6 +12543,44 @@
           <t>https://www.zillow.com/homedetails/4-Grasshopper-Ln-Oxford-MA-01540/60027617_zpid/</t>
         </is>
       </c>
+      <c r="G192" t="n">
+        <v>609100</v>
+      </c>
+      <c r="H192" t="n">
+        <v>502700</v>
+      </c>
+      <c r="I192" t="n">
+        <v>2024</v>
+      </c>
+      <c r="J192" t="inlineStr">
+        <is>
+          <t>2015-07-27</t>
+        </is>
+      </c>
+      <c r="K192" t="n">
+        <v>1902</v>
+      </c>
+      <c r="L192" t="n">
+        <v>2000</v>
+      </c>
+      <c r="M192" t="n">
+        <v>0.9300045913682278</v>
+      </c>
+      <c r="N192" t="inlineStr">
+        <is>
+          <t>Acres</t>
+        </is>
+      </c>
+      <c r="O192" t="inlineStr">
+        <is>
+          <t>Other,Oil</t>
+        </is>
+      </c>
+      <c r="P192" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
     </row>
     <row r="193" ht="15.75" customHeight="1" s="19">
       <c r="A193" s="3" t="inlineStr">
@@ -9285,6 +12607,44 @@
           <t>https://www.zillow.com/homedetails/17-Bakers-Dr-Harwich-MA-02645/55904878_zpid/</t>
         </is>
       </c>
+      <c r="G193" t="n">
+        <v>639300</v>
+      </c>
+      <c r="H193" t="n">
+        <v>534800</v>
+      </c>
+      <c r="I193" t="n">
+        <v>2024</v>
+      </c>
+      <c r="J193" t="inlineStr">
+        <is>
+          <t>1995-08-31</t>
+        </is>
+      </c>
+      <c r="K193" t="n">
+        <v>1800</v>
+      </c>
+      <c r="L193" t="n">
+        <v>1972</v>
+      </c>
+      <c r="M193" t="n">
+        <v>0.2899908172635445</v>
+      </c>
+      <c r="N193" t="inlineStr">
+        <is>
+          <t>Acres</t>
+        </is>
+      </c>
+      <c r="O193" t="inlineStr">
+        <is>
+          <t>Forced air,Gas</t>
+        </is>
+      </c>
+      <c r="P193" t="inlineStr">
+        <is>
+          <t>Central</t>
+        </is>
+      </c>
     </row>
     <row r="194" ht="15.75" customHeight="1" s="19">
       <c r="A194" s="3" t="inlineStr">
@@ -9309,6 +12669,44 @@
           <t>https://www.zillow.com/homedetails/49-Bakers-Dr-Harwich-MA-02645/186993268_zpid/</t>
         </is>
       </c>
+      <c r="G194" t="n">
+        <v>543900</v>
+      </c>
+      <c r="H194" t="n">
+        <v>441500</v>
+      </c>
+      <c r="I194" t="n">
+        <v>2024</v>
+      </c>
+      <c r="J194" t="inlineStr">
+        <is>
+          <t>2008-10-23</t>
+        </is>
+      </c>
+      <c r="K194" t="n">
+        <v>1040</v>
+      </c>
+      <c r="L194" t="n">
+        <v>1982</v>
+      </c>
+      <c r="M194" t="n">
+        <v>0.2899908172635445</v>
+      </c>
+      <c r="N194" t="inlineStr">
+        <is>
+          <t>Acres</t>
+        </is>
+      </c>
+      <c r="O194" t="inlineStr">
+        <is>
+          <t>Electric</t>
+        </is>
+      </c>
+      <c r="P194" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
     </row>
     <row r="195" ht="15.75" customHeight="1" s="19">
       <c r="A195" s="3" t="inlineStr">
@@ -9333,6 +12731,44 @@
           <t>https://www.zillow.com/homedetails/32-Stedman-St-Chelmsford-MA-01824/56446775_zpid/</t>
         </is>
       </c>
+      <c r="G195" t="n">
+        <v>613200</v>
+      </c>
+      <c r="H195" t="n">
+        <v>480500</v>
+      </c>
+      <c r="I195" t="n">
+        <v>2024</v>
+      </c>
+      <c r="J195" t="inlineStr">
+        <is>
+          <t>1987-11-24</t>
+        </is>
+      </c>
+      <c r="K195" t="n">
+        <v>1919</v>
+      </c>
+      <c r="L195" t="n">
+        <v>1940</v>
+      </c>
+      <c r="M195" t="n">
+        <v>9147</v>
+      </c>
+      <c r="N195" t="inlineStr">
+        <is>
+          <t>Square Feet</t>
+        </is>
+      </c>
+      <c r="O195" t="inlineStr">
+        <is>
+          <t>Other,Gas</t>
+        </is>
+      </c>
+      <c r="P195" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
       <c r="Q195" t="inlineStr">
         <is>
           <t>Zillow URL manually gathered for "Stedman Street" intead of "Steadman Street"</t>
@@ -9364,6 +12800,50 @@
           <t>https://www.zillow.com/homedetails/1123-Monument-St-Concord-MA-01742/166021646_zpid/</t>
         </is>
       </c>
+      <c r="G196" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="H196" t="n">
+        <v>5627400</v>
+      </c>
+      <c r="I196" t="n">
+        <v>2024</v>
+      </c>
+      <c r="J196" t="inlineStr">
+        <is>
+          <t>2013-12-05</t>
+        </is>
+      </c>
+      <c r="K196" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="L196" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="M196" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="N196" t="inlineStr">
+        <is>
+          <t>Acres</t>
+        </is>
+      </c>
+      <c r="O196" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="P196" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
     </row>
     <row r="197" ht="15.75" customHeight="1" s="19">
       <c r="A197" s="3" t="inlineStr">
@@ -9390,6 +12870,44 @@
           <t>https://www.zillow.com/homedetails/58-Farmers-Cliff-Rd-Concord-MA-01742/166021917_zpid/</t>
         </is>
       </c>
+      <c r="G197" t="n">
+        <v>1587500</v>
+      </c>
+      <c r="H197" t="n">
+        <v>1302400</v>
+      </c>
+      <c r="I197" t="n">
+        <v>2024</v>
+      </c>
+      <c r="J197" t="inlineStr">
+        <is>
+          <t>2003-09-03</t>
+        </is>
+      </c>
+      <c r="K197" t="n">
+        <v>3000</v>
+      </c>
+      <c r="L197" t="n">
+        <v>1967</v>
+      </c>
+      <c r="M197" t="n">
+        <v>1.989990817263545</v>
+      </c>
+      <c r="N197" t="inlineStr">
+        <is>
+          <t>Acres</t>
+        </is>
+      </c>
+      <c r="O197" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="P197" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
     </row>
     <row r="198" ht="15.75" customHeight="1" s="19">
       <c r="A198" s="3" t="inlineStr">
@@ -9414,6 +12932,44 @@
           <t>https://www.zillow.com/homedetails/3-Barilone-Cir-Maynard-MA-01754/57089854_zpid/</t>
         </is>
       </c>
+      <c r="G198" t="n">
+        <v>753800</v>
+      </c>
+      <c r="H198" t="n">
+        <v>585400</v>
+      </c>
+      <c r="I198" t="n">
+        <v>2024</v>
+      </c>
+      <c r="J198" t="inlineStr">
+        <is>
+          <t>2016-05-16</t>
+        </is>
+      </c>
+      <c r="K198" t="n">
+        <v>1824</v>
+      </c>
+      <c r="L198" t="n">
+        <v>1992</v>
+      </c>
+      <c r="M198" t="n">
+        <v>0.2699954086317723</v>
+      </c>
+      <c r="N198" t="inlineStr">
+        <is>
+          <t>Acres</t>
+        </is>
+      </c>
+      <c r="O198" t="inlineStr">
+        <is>
+          <t>Forced air,Gas</t>
+        </is>
+      </c>
+      <c r="P198" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
     </row>
     <row r="199" ht="15.75" customHeight="1" s="19">
       <c r="A199" s="3" t="inlineStr">
@@ -9440,6 +12996,44 @@
           <t>https://www.zillow.com/homedetails/16-Ash-Ln-Dudley-MA-01571/59207910_zpid/</t>
         </is>
       </c>
+      <c r="G199" t="n">
+        <v>603900</v>
+      </c>
+      <c r="H199" t="n">
+        <v>532300</v>
+      </c>
+      <c r="I199" t="n">
+        <v>2024</v>
+      </c>
+      <c r="J199" t="inlineStr">
+        <is>
+          <t>2014-07-02</t>
+        </is>
+      </c>
+      <c r="K199" t="n">
+        <v>3348</v>
+      </c>
+      <c r="L199" t="n">
+        <v>2000</v>
+      </c>
+      <c r="M199" t="n">
+        <v>0.4699954086317722</v>
+      </c>
+      <c r="N199" t="inlineStr">
+        <is>
+          <t>Acres</t>
+        </is>
+      </c>
+      <c r="O199" t="inlineStr">
+        <is>
+          <t>Other,Oil</t>
+        </is>
+      </c>
+      <c r="P199" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
     </row>
     <row r="200" ht="15.75" customHeight="1" s="19">
       <c r="A200" s="3" t="inlineStr">
@@ -9466,6 +13060,46 @@
           <t>https://www.zillow.com/homedetails/225-Nonotuck-St-B-Northampton-MA-01062/92203160_zpid/</t>
         </is>
       </c>
+      <c r="G200" t="n">
+        <v>270400</v>
+      </c>
+      <c r="H200" t="n">
+        <v>204100</v>
+      </c>
+      <c r="I200" t="n">
+        <v>2024</v>
+      </c>
+      <c r="J200" t="inlineStr">
+        <is>
+          <t>2020-11-24</t>
+        </is>
+      </c>
+      <c r="K200" t="n">
+        <v>1300</v>
+      </c>
+      <c r="L200" t="n">
+        <v>2012</v>
+      </c>
+      <c r="M200" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="N200" t="inlineStr">
+        <is>
+          <t>sqft</t>
+        </is>
+      </c>
+      <c r="O200" t="inlineStr">
+        <is>
+          <t>Baseboard,Gas</t>
+        </is>
+      </c>
+      <c r="P200" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
     </row>
     <row r="201" ht="15.75" customHeight="1" s="19">
       <c r="A201" s="3" t="inlineStr">
@@ -9492,6 +13126,44 @@
           <t>https://www.zillow.com/homedetails/1-Honey-Hill-Rd-Cummington-MA-01026/57006376_zpid/</t>
         </is>
       </c>
+      <c r="G201" t="n">
+        <v>269100</v>
+      </c>
+      <c r="H201" t="n">
+        <v>193700</v>
+      </c>
+      <c r="I201" t="n">
+        <v>2024</v>
+      </c>
+      <c r="J201" t="inlineStr">
+        <is>
+          <t>2020-04-30</t>
+        </is>
+      </c>
+      <c r="K201" t="n">
+        <v>1137</v>
+      </c>
+      <c r="L201" t="n">
+        <v>1949</v>
+      </c>
+      <c r="M201" t="n">
+        <v>4</v>
+      </c>
+      <c r="N201" t="inlineStr">
+        <is>
+          <t>Acres</t>
+        </is>
+      </c>
+      <c r="O201" t="inlineStr">
+        <is>
+          <t>Forced air,Gas</t>
+        </is>
+      </c>
+      <c r="P201" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
     </row>
     <row r="202" ht="15.75" customHeight="1" s="19">
       <c r="A202" s="3" t="inlineStr">
@@ -9518,6 +13190,44 @@
           <t>https://www.zillow.com/homedetails/208-Trouble-St-Cummington-MA-01026/57006372_zpid/</t>
         </is>
       </c>
+      <c r="G202" t="n">
+        <v>428100</v>
+      </c>
+      <c r="H202" t="n">
+        <v>311923</v>
+      </c>
+      <c r="I202" t="n">
+        <v>2024</v>
+      </c>
+      <c r="J202" t="inlineStr">
+        <is>
+          <t>2017-06-30</t>
+        </is>
+      </c>
+      <c r="K202" t="n">
+        <v>1387</v>
+      </c>
+      <c r="L202" t="n">
+        <v>1990</v>
+      </c>
+      <c r="M202" t="n">
+        <v>19</v>
+      </c>
+      <c r="N202" t="inlineStr">
+        <is>
+          <t>Acres</t>
+        </is>
+      </c>
+      <c r="O202" t="inlineStr">
+        <is>
+          <t>Baseboard,Forced air,Stove,Oil,Wood / Pellet</t>
+        </is>
+      </c>
+      <c r="P202" t="inlineStr">
+        <is>
+          <t>Central,Other</t>
+        </is>
+      </c>
     </row>
     <row r="203" ht="15.75" customHeight="1" s="19">
       <c r="A203" s="3" t="inlineStr">
@@ -9542,6 +13252,44 @@
           <t>https://www.zillow.com/homedetails/80-Wigwam-St-Wellfleet-MA-02667/56794929_zpid/</t>
         </is>
       </c>
+      <c r="G203" t="n">
+        <v>1429900</v>
+      </c>
+      <c r="H203" t="n">
+        <v>1072100</v>
+      </c>
+      <c r="I203" t="n">
+        <v>2024</v>
+      </c>
+      <c r="J203" t="inlineStr">
+        <is>
+          <t>2022-12-02</t>
+        </is>
+      </c>
+      <c r="K203" t="n">
+        <v>1638</v>
+      </c>
+      <c r="L203" t="n">
+        <v>2003</v>
+      </c>
+      <c r="M203" t="n">
+        <v>0.41</v>
+      </c>
+      <c r="N203" t="inlineStr">
+        <is>
+          <t>Acres</t>
+        </is>
+      </c>
+      <c r="O203" t="inlineStr">
+        <is>
+          <t>Hot Water</t>
+        </is>
+      </c>
+      <c r="P203" t="inlineStr">
+        <is>
+          <t>Central Air</t>
+        </is>
+      </c>
     </row>
     <row r="204" ht="15.75" customHeight="1" s="19">
       <c r="A204" s="3" t="inlineStr">
@@ -9568,6 +13316,44 @@
           <t>https://www.zillow.com/homedetails/100-Waterfield-Rd-Osterville-MA-02655/55854086_zpid/</t>
         </is>
       </c>
+      <c r="G204" t="n">
+        <v>1574000</v>
+      </c>
+      <c r="H204" t="n">
+        <v>868300</v>
+      </c>
+      <c r="I204" t="n">
+        <v>2024</v>
+      </c>
+      <c r="J204" t="inlineStr">
+        <is>
+          <t>2023-05-19</t>
+        </is>
+      </c>
+      <c r="K204" t="n">
+        <v>2693</v>
+      </c>
+      <c r="L204" t="n">
+        <v>1972</v>
+      </c>
+      <c r="M204" t="n">
+        <v>0.8300000000000001</v>
+      </c>
+      <c r="N204" t="inlineStr">
+        <is>
+          <t>Acres</t>
+        </is>
+      </c>
+      <c r="O204" t="inlineStr">
+        <is>
+          <t>Hot Water,Other</t>
+        </is>
+      </c>
+      <c r="P204" t="inlineStr">
+        <is>
+          <t>Central Air</t>
+        </is>
+      </c>
     </row>
     <row r="205" ht="15.75" customHeight="1" s="19">
       <c r="A205" s="3" t="inlineStr">
@@ -9592,6 +13378,44 @@
           <t>https://www.zillow.com/homedetails/27-Columbus-Ave-Somerville-MA-02143/56333517_zpid/</t>
         </is>
       </c>
+      <c r="G205" t="n">
+        <v>1835800</v>
+      </c>
+      <c r="H205" t="n">
+        <v>1500200</v>
+      </c>
+      <c r="I205" t="n">
+        <v>2024</v>
+      </c>
+      <c r="J205" t="inlineStr">
+        <is>
+          <t>2019-09-20</t>
+        </is>
+      </c>
+      <c r="K205" t="n">
+        <v>2533</v>
+      </c>
+      <c r="L205" t="n">
+        <v>1878</v>
+      </c>
+      <c r="M205" t="n">
+        <v>4356</v>
+      </c>
+      <c r="N205" t="inlineStr">
+        <is>
+          <t>Square Feet</t>
+        </is>
+      </c>
+      <c r="O205" t="inlineStr">
+        <is>
+          <t>Forced air,Gas</t>
+        </is>
+      </c>
+      <c r="P205" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
     </row>
     <row r="206" ht="15.75" customHeight="1" s="19">
       <c r="A206" s="3" t="inlineStr">
@@ -9618,6 +13442,44 @@
           <t>https://www.zillow.com/homedetails/9-Snake-Brook-Rd-Wayland-MA-01778/57127136_zpid/</t>
         </is>
       </c>
+      <c r="G206" t="n">
+        <v>1402700</v>
+      </c>
+      <c r="H206" t="n">
+        <v>1204300</v>
+      </c>
+      <c r="I206" t="n">
+        <v>2024</v>
+      </c>
+      <c r="J206" t="inlineStr">
+        <is>
+          <t>2020-01-09</t>
+        </is>
+      </c>
+      <c r="K206" t="n">
+        <v>2629</v>
+      </c>
+      <c r="L206" t="n">
+        <v>1954</v>
+      </c>
+      <c r="M206" t="n">
+        <v>1.089990817263545</v>
+      </c>
+      <c r="N206" t="inlineStr">
+        <is>
+          <t>Acres</t>
+        </is>
+      </c>
+      <c r="O206" t="inlineStr">
+        <is>
+          <t>Forced air,Gas</t>
+        </is>
+      </c>
+      <c r="P206" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
     </row>
     <row r="207" ht="15.75" customHeight="1" s="19">
       <c r="A207" s="3" t="inlineStr">
@@ -9642,6 +13504,44 @@
           <t>https://www.zillow.com/homedetails/23-Oak-St-Wayland-MA-01778/57127303_zpid/</t>
         </is>
       </c>
+      <c r="G207" t="n">
+        <v>876800</v>
+      </c>
+      <c r="H207" t="n">
+        <v>717700</v>
+      </c>
+      <c r="I207" t="n">
+        <v>2024</v>
+      </c>
+      <c r="J207" t="inlineStr">
+        <is>
+          <t>2000-06-01</t>
+        </is>
+      </c>
+      <c r="K207" t="n">
+        <v>1872</v>
+      </c>
+      <c r="L207" t="n">
+        <v>1947</v>
+      </c>
+      <c r="M207" t="n">
+        <v>0.3699954086317723</v>
+      </c>
+      <c r="N207" t="inlineStr">
+        <is>
+          <t>Acres</t>
+        </is>
+      </c>
+      <c r="O207" t="inlineStr">
+        <is>
+          <t>Forced air,Oil</t>
+        </is>
+      </c>
+      <c r="P207" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
     </row>
     <row r="208" ht="15.75" customHeight="1" s="19">
       <c r="A208" s="3" t="inlineStr">
@@ -9666,6 +13566,44 @@
           <t>https://www.zillow.com/homedetails/231-Melrose-St-Newton-MA-02466/56309625_zpid/</t>
         </is>
       </c>
+      <c r="G208" t="n">
+        <v>1500600</v>
+      </c>
+      <c r="H208" t="n">
+        <v>1171500</v>
+      </c>
+      <c r="I208" t="n">
+        <v>2024</v>
+      </c>
+      <c r="J208" t="inlineStr">
+        <is>
+          <t>2018-09-28</t>
+        </is>
+      </c>
+      <c r="K208" t="n">
+        <v>1715</v>
+      </c>
+      <c r="L208" t="n">
+        <v>1892</v>
+      </c>
+      <c r="M208" t="n">
+        <v>4356</v>
+      </c>
+      <c r="N208" t="inlineStr">
+        <is>
+          <t>Square Feet</t>
+        </is>
+      </c>
+      <c r="O208" t="inlineStr">
+        <is>
+          <t>Forced air,Heat pump,Electric,Gas</t>
+        </is>
+      </c>
+      <c r="P208" t="inlineStr">
+        <is>
+          <t>Central</t>
+        </is>
+      </c>
     </row>
     <row r="209" ht="15.75" customHeight="1" s="19">
       <c r="A209" s="3" t="inlineStr">
@@ -9690,6 +13628,44 @@
           <t>https://www.zillow.com/homedetails/53-Kingswood-Rd-Newton-MA-02466/56309759_zpid/</t>
         </is>
       </c>
+      <c r="G209" t="n">
+        <v>2374300</v>
+      </c>
+      <c r="H209" t="n">
+        <v>1899900</v>
+      </c>
+      <c r="I209" t="n">
+        <v>2024</v>
+      </c>
+      <c r="J209" t="inlineStr">
+        <is>
+          <t>2009-08-24</t>
+        </is>
+      </c>
+      <c r="K209" t="n">
+        <v>2304</v>
+      </c>
+      <c r="L209" t="n">
+        <v>1947</v>
+      </c>
+      <c r="M209" t="n">
+        <v>0.2618916437098255</v>
+      </c>
+      <c r="N209" t="inlineStr">
+        <is>
+          <t>Acres</t>
+        </is>
+      </c>
+      <c r="O209" t="inlineStr">
+        <is>
+          <t>Forced air,Gas</t>
+        </is>
+      </c>
+      <c r="P209" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
     </row>
     <row r="210" ht="15.75" customHeight="1" s="19">
       <c r="A210" s="3" t="inlineStr">
@@ -9712,6 +13688,44 @@
       <c r="F210" s="6" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/45-July-St-Lowell-MA-01850/56511098_zpid/</t>
+        </is>
+      </c>
+      <c r="G210" t="n">
+        <v>531600</v>
+      </c>
+      <c r="H210" t="n">
+        <v>400700</v>
+      </c>
+      <c r="I210" t="n">
+        <v>2024</v>
+      </c>
+      <c r="J210" t="inlineStr">
+        <is>
+          <t>2022-06-17</t>
+        </is>
+      </c>
+      <c r="K210" t="n">
+        <v>1716</v>
+      </c>
+      <c r="L210" t="n">
+        <v>1930</v>
+      </c>
+      <c r="M210" t="n">
+        <v>6969.6</v>
+      </c>
+      <c r="N210" t="inlineStr">
+        <is>
+          <t>Square Feet</t>
+        </is>
+      </c>
+      <c r="O210" t="inlineStr">
+        <is>
+          <t>Electric Baseboard,Steam,Natural Gas</t>
+        </is>
+      </c>
+      <c r="P210" t="inlineStr">
+        <is>
+          <t>None</t>
         </is>
       </c>
     </row>

</xml_diff>